<commit_message>
Make simple process & Context Crawling process
</commit_message>
<xml_diff>
--- a/Output/NewsCrawlList.xlsx
+++ b/Output/NewsCrawlList.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -345,14 +358,980 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>“10년 내 ‘좀비 사슴’ 먹고 전염된 인간 나올 것” 전문가 경고</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>[서울신문 나우뉴스] 캐나다와 미국 일대를 휩쓴 만성소모성질병(CWD, Chronic wasting disease), 일병 ‘광록병’이 인간에게까지 전염될 수 있다는 전문가들의 우려가 나왔다. 광록병은 사슴이나 엘크 등 사슴류에 감염돼 중추신경계에 손상을 입히며, 뇌가 파괴되면서 스펀지처럼 구멍이 생기는 증상을 동반한다. 평범한 사슴에 비해 인간을 덜 무서워하게 되고 얼굴표정이 사라지며, 마치 광우병에 걸린 소처럼 침을 흘리거나 주저앉는 증상을 보인다. 이 병에 걸린 사슴을 두고 ‘좀비 사슴’이라고 부르는 이유다. UPI 뉴스 등 미국 현지 언론에 따르면 광록병은 광우병과 마찬가지로 변형 단백질인 프리온(Prions)에 의해 유발되며, 이는 박테리아나 바이러스와 달리 몇 년간 자연에서 파괴되지 않고 타액이나 배설물 등을 통해 전염될 수 있다. 광우병 전문가로 꼽히는 마이클 오스터홀름 미네소타대 교수는 지난 7월 미국 미생물학회(American Society for Microbiology)에 발표한 논문을 통해 “광록병에 감염된 사슴고기를 섭취할 경우 변형된 프리온에 의한 증상이 나타나기까지 몇 년의 잠복기가 있을 것”이라면서 “10년 내에 광록병에 전염된 인간의 사례가 속속 나타날 것”이라고 경고했다. 이에 전문가들은 좀비 사슴이 발견되는 캐나다와 미국 일대에서 대대적인 캠페인을 통해 감염된 사슴을 사냥하지 않거나, 사냥한 뒤 특정 테스트를 거친 뒤 고기를 섭취하도록 강력하게 권유해야 한다고 목소리를 높이고 있다. 문제는 해당 질병이 지속적인 확산 추세에 있는 캐나다와 미국 일대에서 여전히 사슴고기 섭취율이 줄지 않고 있다는 사실이다. 지난해 미국에서 발표된 공공야생동물연합 보고서에 따르면 매년 사냥꾼 1만 5000명이 광록병에 감염된 고기를 먹는 것으로 추정되며, 이 병이 확산됨에 따라 그 수는 매년 20% 증가하는 상황이다. 미국 콜로라도주립대학의 마크 자벨 박사는 UPI와 한 인터뷰에서 “사슴고기를 소시지와 스테이크로 가공하는 처리 시설을 통해서도 질병이 확산될 수 있다. 프리온이 고기를 절단하거나 가공하는 장비를 오염시킬 수 있기 때문”이라면서 “이러한 가공 공장은 먹이사슬에 따라 끔찍한 결과를 가져올 수 있다”고 경고했다. 송현서 기자 huimin0217@seoul.co.kr ★ ▶ ⓒ 서울신문(www.seoul.co.kr), 무단전재 및 재배포금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>갤노트10 플러스, 사라진 ‘홍채 인식’ 아쉬움보다 ‘꽉 찬 화면’ 만족감 더 커</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>대담한 변신… 삼성 갤럭시 노트10 플러스 사용해보니 갤럭시 노트10은 흥미로운 스마트폰이다. 보통 신제품은 전작에 사양이나 기능을 추가하기 마련인데 노트10은 노트9에서 몇 가지가 빠졌다. 꼭 필요한 게 아니면 빼고 중요한 것에 집중하겠다는 의지가 읽힌다. 대신 필요한 건 제대로 업그레이드해 사용성을 높였다. 변화에 적응하는 데 따른 불편함도 일부 있지만 그걸 상쇄하고 남을 만큼 장점이 더 많다. 게다가 외부기기와 연결성도 좋아져 ‘갤럭시 생태계’의 가능성도 보여줬다. 일주일간 노트10 플러스를 사용하면서 든 느낌은 노트 시리즈 고유의 중후함이 사라졌다는 것이다. 뒤집어 말하면 젊고 세련된 느낌으로 정체성 변화를 시도했다고 볼 수 있다. 디자인이 날렵해졌고, 불필요한 것들을 뺀 덕분이다. 거기에 딱히 어떤 색이라고 정의할 수 없는 ‘아우라 글로우’라는 색을 주력으로 내세우면서 젊은 감각을 내세운 것도 한몫했다. 노트10에서 사라진 건 이어폰 잭, 홍채인식 기능이다. 노트7에 처음 도입했던 홍채인식을 뺀 건 사용이 적은 탓도 있지만, ‘인피니티-O’ 디스플레이를 적용하기 위해서로 보인다. 노트10은 제품에서 화면이 차지하는 비중이 94.2%까지 높아졌다. 상하좌우 테두리에 빈 공간이 거의 없이 화면이 덮고 있다. 상단 가운데 카메라홀만 있다. 각종 센서는 디스플레이 아래로 들어갔는데 홍채인식 기능은 적외선을 쏘아야 하기 때문에 디스플레이 아래에 넣기 어려웠던 것으로 보인다. 꽉 찬 화면이 주는 만족감이 홍채 인식이 사라진 아쉬움보다 몇 배는 더 컸다. 노트10 플러스는 6.8형 화면임에도 제품 크기는 노트9과 거의 비슷하다. 노트9과 화면 크기가 같은 노트10 일반 모델은 갤럭시S10과 비슷한 크기다. 화면 비중이 너무 높다 보니 터치할 때 오작동이 가끔 나타났다. 왜 엣지 스크린을 포기하지 않을까 하는 아쉬움이 들긴 했지만, 플랫 스크린으로는 디자인을 예쁘게 하는 데는 한계가 있겠다는 생각이 들었다. 노트10에서 가장 불편하다고 느껴진 건 역시 이어폰 잭이 없어진 것이다. 무선 이어폰을 사용하고 있지만, 비행기를 타거나, 무선이어폰 배터리가 떨어지는 때 등 유선 이어폰이 여전히 필요할 때가 있다. 오디오 마니아라면 아끼는 이어폰 하나쯤은 있을 텐데 그걸 못 쓰게 된 것이라 일정 부분 불편함은 어쩔 수 없다. 대신 이어폰 잭이 없어진 건 늘어난 배터리 용량으로 치환된다. 노트10 플러스의 배터리는 4500mAh다. 노트9보다 500mAh 늘어나 노트 시리즈 중 가장 많다. 덕분에 여유 있는 사용이 가능해졌다. 고사양 게임을 하지 않는다면 온종일 사용하는 데 큰 무리가 없는 수준이다. 여기에 노트10은 25W 초고속 충전을 지원한다. 노트9까지는 15W 규격이었는데 더 빨라졌다. 완전 방전상태에서 충전하면 30분 만에 60% 수준으로, 완전히 충전하는 데는 한 시간이 조금 넘게 걸린다. 노트10 플러스는 한 걸음 더 나가 45W 충전까지 지원한다. 단 삼성전자 전용 충전기로만 가능하다. 30분만 충전하면 하루 종일 사용할 수 있는 수준으로 충전할 수 있다고 삼성전자는 설명했다. 카메라 화질은 노트9이나 S10에 비해 큰 폭의 개선은 없었다. 대신 활용할 수 있는 기능이 풍성해졌다. 라이브 포커스는 뒷배경을 흐리게 하는 옵션이 많아져 다양한 사진을 연출할 수 있었다. 사람과 배경을 구별해내는 실력도 더 좋아졌다. 이전에는 인물과 배경의 경계 부분이 많이 뭉개지는 경향이 있었는데, 노트10은 잔머리까지 살려둘 정도로 정확도가 높아졌다. 특히 라이브 포커스 기능이 동영상에도 적용돼 용도에 맞는 동영상을 풍성하게 담을 수 있다는 것도 매력적인 포인트였다. 노트 시리즈의 정체성인 S펜은 스펙을 키우기보다 사용성 개선에 초점을 맞췄다. 특히 손글씨를 타자로 입력한 텍스트로 변환해주는 기능은 직장인에게 아주 유용하다. 지인들에게 이 기능을 시험 삼아 체험해보게 했을 때 다들 깜짝 놀랐다. 대충 써도 정확하게 인식했기 때문이다. 물론 100%라고 하긴 어렵지만, 업무에 도움이 될 수준임은 분명하다. 하지만 대대적으로 광고하고 있는 ‘에어 액션’ 기능은 개선이 필요해 보인다. 생각하는 것만큼 잘 인식이 되지 않아 그냥 화면을 터치하는 쪽이 더 편했다. 노트10은 스마트폰 인터페이스를 PC처럼 바꿔주는 ‘덱스’ 사용이 간편해져 사용성에 날개를 달았다. 이전까지는 덱스를 쓰려면 ‘덱스 패드’ 같은 별도의 기기를 거쳐야 했고 키보드, 마우스도 별도로 연결해야 했다. 하지만 노트10은 UBS 케이블만 PC에 연결하면 된다. 키보드, 마우스 등은 PC 것을 그대로 사용한다. 노트10에 있는 자료를 마우스 몇 번으로 PC로 옮기거나 그 반대로도 할 수 있다. 덱스 모드를 지원하는 앱이 많아지면 노트10의 사용성은 더 좋아질 것으로 보인다. 또 마이크로소프트가 윈도10에 탑재한 ‘사용자 휴대폰’ 기능으로 노트10의 문자, 사진 등을 실시간으로 PC와 연동시킬 수 있다. 문자를 PC에서 바로 보내거나 사진을 실시간으로 확인할 수 있었다. 자체 운영체제(OS)가 없는 삼성전자는 스마트폰과 PC 연동에 어려움을 겪었는데 MS와 협업을 통해 ‘스마트폰-태블릿-PC’등을 자유롭게 넘나드는 갤럭시 생태계 구축이 가능해졌다는 점은 고무적이다. 김준엽 기자 snoopy@kmib.co.kr GoodNews paper ⓒ , 무단전재 및 재배포금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>'공짜야근' 사라지니 6시면 칼퇴… 불켜진 사무실이 없었다[현장르포]</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>게임업계 포괄임금제 폐지 그 후 판교·구로 IT단지 6시반에 찾은 넥슨 본사는 고요..스마일게이트 퇴근은 4시부터 '판교 오징어배''구로 등대' 옛말 업무강도 세지고 시간 준수 엄격 저녁 6시쯤 판교 엔씨소프트 본사 사옥을 직원들이 썰물처럼 빠져나가고 있다. 사진=강현수 인턴기자 '구로의 등대' '판교의 오징어배'라는 별칭이 붙을 정도로 고강도의 야근이 고착화돼 있던 게임업계에 새바람이 불고 있다. 기자가 찾은 판교와 구로 게임사들의 퇴근길 풍경은 그야말로 '천지개벽' 수준이었다. 26일 게임업계에 따르면 넥슨이 이달 포괄임금제를 폐지한 데 이어 넷마블이 3·4분기, 엔씨소프트와 스마일게이트가 10월 중 포괄임금제를 폐지할 예정이다. 포괄임금제는 연봉에 각종 수당이 포함돼 직원들이 초과근무를 하고도 따로 수당을 받지 못하는 경우가 많았지만 포괄임금제가 폐지되면 기존 연봉이 기본급으로 전환돼 기본 근무시간을 초과하는 근무에 대한 수당을 지급해야 한다. ■판교 퇴근시간, 30분만 지나도 '고요' 저녁 6시30분께 포괄임금제가 이달부터 폐지된 넥슨 본사 사옥은 고요했다. 분명히 퇴근시간인데 너무 사람이 없어서 안내데스크에 물어보니 직원들은 이미 거의 다 퇴근을 한 상태. 저녁 6시면 상황 종료란다. 가까스로 퇴근 길 막차에 오른 직원들을 인터뷰할 수 있었다. 넥슨 직원 최경호씨(29·가명)는 "포괄임금제 폐지가 결정되고 회사 분위기는 말그대로 '급격하게' 바뀌었다"며 "야근은 거의 사라졌고 출근은 11시까지만 하면 돼서 아침밥도 먹게 됐다"고 말했다. 인근 스마일게이트의 퇴근시간은 오후 4시부터 시작된다. 스마일게이트는 오전 10시부터 오후 4시를 필수 협업시간으로 정한 뒤 나머지 일정은 개인이 조율해 출퇴근할 수 있다. 스마일게이트 직원 이동현씨(36·가명)는 "특별히 할 일 없으면 다들 4시에 집에 가는데 퇴근할 때 상사한테 보고 안하고 그냥 집에 가는 것이 가장 좋다"며 웃었다. ■개발주기 따라 게임사별 온도차 구로는 판교보다는 퇴근시간이 늦은 편이었다. 구로에 위치한 넷마블에서 만난 문상윤씨(37·가명)는 "포괄임금제 폐지를 앞두고 있지만 이미 정해진 시간에 출퇴근하는 문화가 회사 안에 정착된 지 오래"라며 "다른 데보다는 퇴근이 조금 늦은 것으로 알고있는데 그래도 예전 생각하면 감지덕지"라고 회상했다. 최승우씨(35·가명)는 "아직 할 일이 남은 사람들은 남아서 일을 하기는 하지만 예전처럼 강요나 눈치 주는 건 없다"며 "예전만큼 구로의 등대 수준은 아닌 것 같다"고 평가했다. 칼퇴가 가능한 게임사와 가능하지 않은 게임사의 사정이 다르다는 지적이다. 게임업계 관계자는 "주 52시간 근무제 도입으로 게임 출시 간격이 빠른 게임사 위주로 신작 출시 일정이 밀리면서 타격을 입었다"며 "2~3년 주기로 개발을 하는 게임을 만드는 회사들은 크게 영향을 받지 않는다"고 설명했다. ■업무시간 감시 우려도 다만 포괄임금제 폐지가 마냥 장밋빛 미래만 약속하는 것은 아니다. 관리자들로부터 잦은 간섭에 휘말릴 가능성도 있다. 넥슨 직원 김민주씨(34·가명)는 "딸, 아들 모두 직장 어린이집에 다니는데 일하는 시간이 자유로워져서 애들이 나를 기다리는 시간이 많이 줄어 행복하다"며 "부서 직원들이 다 같이 있는 시간이 줄어들다 보니 관리자급들은 힘들어하는 눈치"라고 우려했다. 게임사에서 관리자급으로 일하고 있는 조바다씨(44·가명)는 "포괄임금제가 폐지되면 업무시간 내에 직원들이 일하는 일거수일투족을 감시하라는 회사측의 압박이 가해질 수도 있다"며 "초과근무가 없어지는 만큼 업무시간이 타이트해질 것"이라고 진단했다. true@fnnews.com 김아름 기자 강현수 인턴기자 ※ 저작권자 ⓒ 파이낸셜뉴스. 무단 전재-재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>삼성전자 '갤럭시S10 선전' 일본시장서 6년來 최고 점유율</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1위 애플 50.8%…삼성 9.8%·샤프 7.2%·소니 7.0% 순 (서울=연합뉴스) 채새롬 기자 = 삼성전자가 올해 2분기 갤럭시S10 시리즈 선전에 힘입어 일본 스마트폰 시장에서 6년 만에 가장 높은 점유율을 기록했다. 일본 도쿄 갤럭시 하라주쿠 [삼성전자 제공] 26일 시장조사업체 스트래티지 애널리틱스(SA)에 따르면 삼성전자는 2분기 일본 스마트폰 시장에서 60만대를 출하해 점유율 9.8%를 기록했다. 애플(50.8%)에 이은 2위였다. 작년 동기 점유율이 애플 45.6%, 삼성전자 8.8%이었던 것과 비교해서 모두 소폭 올랐다. 애플과 삼성전자에 이어서는 샤프(7.2%), 소니(7.0%) 등 일본 기업이 3∼4위를 차지했다. 샤프는 작년 동기(5.1%) 대비 2.1%포인트 올랐고, 소니는 10.3%에서 3.3%포인트 줄었다. 중국 화웨이는 작년 동기 5.9%(4위)에서 올해 2분기 3.3%(5위)로 점유율이 절반 가까이 하락했다. 삼성전자가 10%에 육박한 점유율을 낸 것은 6년만에 최고치다. 삼성전자는 2013년 중반 일본 스마트폰 시장에서 10% 넘는 점유율을 유지하다 애플과 일본 브랜드에 밀려 2014년 5.6%, 2015년 4.3%, 2016년 3.4%로 점유율이 하락했다. 2017년부터 반등을 시작해 5.2%, 2018년 6.4%로 점유율이 오르는 추세다. 2분기 좋은 성적은 상반기 출시한 플래그십 모델 갤럭시S10 시리즈가 일본에서 인기를 끈 덕으로 보인다. 삼성전자는 지난 3월 전 세계 갤럭시 쇼케이스 가운데 최대 규모인 '갤럭시 하라주쿠'를 개관하면서 현지 스마트폰 시장 공략을 본격화했다. 5G 서비스가 처음으로 본격 적용되는 '2020 도쿄 올림픽'을 앞두고 일본 내 5G 네트워크 사업 확대를 위한 기반을 조성하는 동시에 갤럭시 스마트폰 시장점유율 반등의 계기를 마련한다는 전략이다. 삼성전자는 7월에는 2020 도쿄 올림픽을 기념해 갤럭시S10 플러스 올림픽 에디션을 일본에 출시했다. srchae@yna.co.kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>"세계를 바꿀 스타트업"… 한국계 20대 사업가 美서 돌풍</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>[오늘의 세상] 인공지능으로 법안 통과 예측, 美 '피스컬노트' 창업자 팀 황 2800억원 투자 유치 - 美정부·의회·법원의 빅데이터 AI로 실시간 분석해 정보 제공, 우버·맥도널드 등 5000여 고객 야후 창업자·NBA 구단주 등 '흥행보증수표'들 투자 이끌어 이코노미스트 정치 매체 인수… 20대에 언론사 오너 자리에 올라 인공지능(AI)으로 미국 정치판을 흔들겠다는 한국계 젊은 창업자가 미국 스타트업 업계의 주목을 받고 있다. 실리콘밸리에선 '제2의 마크 저커버그(페이스북 창업자)'라는 목소리까지 나온다. 주인공은 데이터 분석 서비스 기업 피스컬노트(FiscalNote) 창업자 겸 CEO(최고경영자)인 팀 황(27·한국명 황태일)이다. 이 20대 청년은 2013년 창업한 이후 야후 창업자인 제리 양, 미국의 억만장자이자 NBA(프로농구) 댈러스 매버릭스의 구단주인 마크 큐번 등 '흥행 보증수표'로 불리는 벤처투자자들로부터 총 2억3000만달러(약 2800억원)의 투자를 이끌어냈다. 2014년 미국 CNN은 피스컬노트를 '세계를 바꿀 10대 스타트업'으로 꼽았다. 2016년 포브스는 황 대표를 '30세 이하 유망주 30인', 세계경제포럼(다보스포럼)은 '기술 선구자'로 선정했다. 지난 23일(현지 시각) 미국 캘리포니아주 산호세에서 열린 한인 스타트업 모임 '82스타트업' 무대에 선 황 대표는 "원래 정치인이 되고 싶었지만, 기술이 정치보다 빠르게 움직이고 모든 것을 바꾸는 것을 보고 창업을 결심했다"고 했다. "나는 정치를 통해 헬스케어 관련 법안을 바꾸려고 노력할 때, 친한 친구는 모바일 앱을 만들어 1년 만에 수만 명의 의사와 환자를 직접 연결하는 것을 보고 '대체 이건 뭐지'란 생각이 들었다"는 것이다. ◇AI로 정치를 예측하다 피스컬노트는 미 연방과 50개 주(州) 정부·의회·법원이 공개한 빅데이터를 실시간으로 끌어와서 인공지능으로 분석한 정보를 제공한다. 이를 통해 현재 의회에 올라온 법안의 세부 내용과 후원자, 상·하원 의원의 과거 투표 성향을 분석해 이들이 찬성 혹은 반대할 것인지, 실제 법안이 통과될 가능성은 얼마인지까지 분석한다. 황 대표는 "법안 통과 예측도는 90% 이상"이라고 했다. 예를 들어 차량 공유 서비스 우버의 대관(對官) 담당자는 현재 미 연방과 50개 주 의회에서 차량 공유와 관련된 어떤 법안이 발의됐고 어떻게 진행되는지를 실시간으로 파악할 수 있다. 주마다 제각각인 법령과 특정 주 법원의 과거 판결문까지 반영한다. 해당 법안은 누가 어떤 의도로 만들었는지, 과연 통과될 것인지를 미리 예측해 관련 기업·시민단체·지역 주민들이 대처하도록 돕는 것이다. 황 대표는 "우버, 존슨앤드존스, 맥도널드 등 5000여 고객이 피스컬노트를 구독한다"며 "현재 미국뿐만 아니라 세계 60국의 공공 데이터를 분석해 제공하고 있다"고 했다. 피스컬노트는 작년 8월 영국의 유력 언론사인 이코노미스트 그룹과 1억8000만달러짜리 계약을 체결했다. 이코노미스트가 보유한 '시큐롤콜(CQ Roll Call)'이란 미국 백악관·의회 소식을 다루는 정치 전문 매체를 인수한 것이다. 대신 이코노미스트는 현금과 피스컬노트의 지분 18%를 받기로 했다. 이코노미스트 그룹의 크리스 스팁스 CEO도 피스컬노트의 이사회 멤버로 합류했고 황 대표는 20대에 언론사의 오너(사주·社主)가 된 것이다. 기술 벤처기업에 유력 매체를 내주면서 한배를 탄 것이다. 황 대표는 "정보를 재판매하는 업(業)인 만큼 고객에게 데이터 분석과 실시간 콘텐츠를 충실하게 제공하기 위한 것"이라고 했다. 팀 황 피스컬노트 창업자/피스컬노트 ◇"정치보다 기술이 세상 더 빠르게 바꿔" 팀 황은 1986년에 미국으로 이민 간 한국인 부부가 낳은 한인 2세다. 1992년 미국 미시간주에서 태어났다. 고등학교 시절이던 16세 때 버락 오바마 민주당 대통령 후보 선거캠프에서 일했다. 이듬해엔 메릴랜드주 몽고메리카운티의 학생 교육위원에 투표로 선출되는 등 학창 시절엔 '정치 유망주'였다. 프린스턴대에 진학해 정치학과 컴퓨터공학을 전공했다. 21세 때 동창생 2명과 함께 창업했다. 그는 "정치와 기술의 교차점에서 창업을 결심했다"며 "창업을 위해 실리콘밸리로 건너온 초창기엔 워낙 돈이 없어 모텔에서 먹고 자며 일했다"고 했다. 황 대표의 목표는 크다. 그는 "현재의 60국을 넘어 전 세계 200여 국가의 모든 법과 규정을 디지털 플랫폼에 담는 것이 목표"라며 "인류 최초의 성문법인 '함무라비 법전'의 다음 버전을 만들고 싶다"고 했다. [실리콘밸리=박순찬 특파원 ideachan@chosun.com] - Copyrights ⓒ 조선일보 &amp;amp; chosun.com, 무단 전재 및 재배포 금지 -</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>"삼성 '갤S10' 일본 열도도 열광?"…日 점유율 '10% 고지' 탈환하나</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>삼성폰, 일본 시장서 2분기 점유율 9.8% 기록 "6년 만에 최고" 삼성전자 IM부문장 고동진 사장이 지난 3월 일본 도쿄에서 열린 갤럭시 쇼케이스 '갤럭시 하라주쿠' 개관식에서 인사말을 하는 모습이다. ‘ (삼성전자 제공) 2019.3.12/뉴스1© 뉴스1 (서울=뉴스1) 김일창 기자 = 삼성전자가 상반기 전략 스마트폰 '갤럭시S10' 시리즈의 판매호조에 일본 스마트폰 시장에서 6년 만에 최고 점유율을 기록했다. 2013년 중반까지만 해도 10%가 넘는 점유율을 유지하다 아이폰에 밀려 '애플 천하'가 된 일본 시장에서 삼성전자가 '10% 점유율' 고지 탈환을 눈앞에 두고 있다. 26일 시장조사업체 스트래티지 애널리틱스(SA)에 따르면 삼성전자는 올해 2분기 약 60만대의 스마트폰을 출하해 점유율 9.8%를 기록했다. 애플은 점유율 50.8%로 일본 시장점유율 1위를 이어갔다. 애플과 삼성전자를 이어서는 샤프와 소니가 각 7.2%·7.0%로 3·4위에 올랐다. 삼성전자의 출하량이 확대한 것은 지난 3월 출시한 갤럭시S10시리즈의 인기 영향으로 풀이된다. SA에 따르면 갤럭시S10시리즈는 올해 1분기 매출 기준으로 전세계에서 가장 많이 팔린 안드로이드 스마트폰이다. 삼성전자의 존재감이 미미한 일본에까지 갤럭시S10 판매효과가 영향을 미친 것으로 분석된다. 삼성전자 스마트폰은 그동안 일본에서 부진을 면치 못했다. 시장조사업체 카날리스에 따르면 삼성전자 스마트폰의 2018년 4분기 일본 시장 점유율은 6.8%다. 60%가 넘는 애플의 점유율과 비교할 때 턱없이 낮은 수준이다. 일본 스마트폰 시장에서 10% 넘는 점유율을 유지한 2013년 이후 줄곧 하락세였다. 그러나 인피니티-O 디스플레이에 지문인식 센서 탑재, 무선충전 기술 등 혁신의 갤럭시S10시리즈를 출시하고 동시에 일본 도쿄 중심가 하라주쿠에 지상 6층·지하 1층 규모의 세계 최대 갤럭시 쇼케이스 '갤럭시 하라주쿠'를 선보이면서 분위기가 바뀌었다. '갤럭시 하라주쿠'는 총 지상 6층·지하 1층 규모로 전세계 갤럭시 쇼케이스 중 최대 규모다. 특히 '5G 올림픽'을 표방하는 2020년 도쿄올림픽을 앞두고 있는 상황에서 삼성전자는 국제올림픽위원회(IOC) 무선통신 및 컴퓨팅 장비 분야 공식 파트너인 만큼, 올림픽 특수 기대감도 높아지고 있다. 삼성전자는 지난달 도쿄 올림픽을 기념해 갤럭시S10+ 올림픽 에디션을 선보였다. 다만, 일본의 경제보복으로 촉발된 양국간 무역갈등이 변수로 남아있다. ickim@news1.kr [© 뉴스1코리아(), 무단 전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>[로봇이 간다]1.5㎏ 의자로봇 입으니···쭈그려 일해도 허리 멀쩡, 생산성은 UP</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>■현대차 웨어러블로봇 4총사 하반신용 '첵스' 연내 양산 추진 가볍고 10~20초면 간편 착용 근로자 피로·부상위험 확 줄어 허리보조 '웩스'도 내년 상용화 사회적 경제비용 절감 효과 커 현대차 로보틱스팀 관계들이 25일 경기도 의왕연구소에서 허리지지형 웨어러블 로봇 웩스(왼쪽)와 의자형 웨어러블 로봇 첵스를 착용한 후 물건 들기와 조립 작업을 시연하고 있다. /권욱기자 [서울경제] 현대자동차는 오는 4·4분기부터 웨어러블 로봇을 시작으로 로봇제품 상용화에 나선다고 현대차 관계자가 25일 서울경제신문에 밝혔다. 현재 연구개발 중인 로봇공학은 3개 분야인데 각각 입는 로봇(웨어러블 로봇), 서비스 로봇, 개인용 소형이동수단(마이크로 모빌리티)이다. 해당 분야에서 모두 8종류의 로봇들이 시험 중이며 이 중 하반신에 입는 ‘첵스(CEX)’부터 연내 상용화된다. 서울경제신문은 경기도 의왕시에 있는 현대차 로보틱스팀의 연구소를 방문해 8종 세트를 취재했다. 총 2편에 걸쳐 보도하는데 그중 ‘웨어러블 로봇 4총사’를 먼저 소개한다. 지난해부터 각각 미국 앨라배마주·조지아주에 있는 현대차와 기아차 북미공장의 생산직 근로자들은 처음 보는 로봇을 입게 됐다. 간편하게 입으면 마치 네발 달린 의자가 된 것처럼 하체의 근력 부담을 덜어주는 하지보조 착용로봇 첵스다. 허리 아래 부분을 곤충의 외골격처럼 감싸주는 형태인데 엉거주춤한 자세로 일하는 경우가 많은 자동차 생산현장에서 일하더라도 허리·무릎·골반에 부담을 주지 않도록 설계됐다. 실제로 현대차가 수개월간 시범 도입한 결과는 성공적이었다. 하루에도 최장 8시간씩 공장 생산라인에 반쯤 쭈그린 자세로 자동차 부품을 조립해야 했던 근로자들은 근골격계 통증과 피로에 시달렸는데 첵스를 입은 후 육체 피로와 부상 위험을 현저히 덜어낼 수 있었다. 생산성 향상을 기대할 수 있음을 시사하는 결과도 데이터로 확보했다고 한다. 첵스는 최근 현대차 국내 공장에도 시범 도입돼 실용성·경제성 등을 가늠하는 절차인 개념증명(proof of concept) 과정을 진행했다. 현동진 현대차 로보틱스팀장은 “첵스는 연내에 양산을 통해 상용화한다”며 “먼저 올해에는 북미공장에서부터 본격 도입되며 내년부터는 국내 공장에도 적용할 계획”이라고 전했다. 양산 제품은 먼저 현대차 내부 수요 물량부터 채운 뒤 다른 자동차 회사를 비롯한 외부 고객들을 대상으로 시판된다. 현대차가 로보틱스팀을 통해 첵스 등의 상용화 준비를 본격화한 것은 2017년 무렵부터였다. 앞서 일본 도요타, 미국 포드사가 상반신 착용 로봇을 자사 공장에 도입하기는 했으나 자체 개발품이 아니라 미국의 웨어러블 전문기업 레비테이트테크놀로지스(LT) 제품 등을 사다 쓴 것이었다. 현대차는 그 정도는 충분히 직접 개발할 수 있다고 판단했다. 이미 웨어러블 로봇 개발을 수년간 연구해왔기 때문이다. 더구나 현대차는 일반 로봇전문기업과 달리 테스트베드 역할을 해줄 대규모 자동차 생산공장을 국내외에 두고 있으니 연구개발 중간중간 생산현장에 시범 적용해 근로자의 의견을 개진할 수 있다는 장점도 갖고 있어 유리했다. 자체 연구진과 생산현장 관계자 등이 소통하며 시제품을 개발해 북미공장에 적용해보니 근로자들의 평가가 좋았다. 현 팀장은 “저희 생산근로자들에게 경쟁사 웨어러블 로봇과 저희 제품을 써보게 했는데, 어느 것이 우리 회사 제품인지 모르도록 블라인드테스트 방식으로 진행했다”며 “그 결과 우리 제품에 대한 사용자들의 만족도가 월등했고, 생산성 개선 효과도 더 좋다는 평가를 들어 자신감을 갖게 됐다”고 전했다. 첵스의 장점은 경량이며 활동성이 자유롭다는 것이다. 또한 별도의 전원·연료가 필요 없이 작동하는 ‘에너지 저장·발산형 패시브방식’이어서 충전 등을 하지 않고 장시간 쓸 수 있다. 자체 하중은 1.5㎏대에 불과하다. 실제로 기자가 실물을 접해보니 약간 두꺼운 책 한 권 정도의 무게밖에 나가지 않았다. 엉덩이에서부터 무릎관절·종아리까지 외골격이 꽉 잡아주면서도 관절의 가동이 매우 부드러워 골반과 무릎을 굽혔다 폈다 반복하며 일할 때 편할 것 같았다. 기자의 체중은 미들급 정도인데 로봇이 워낙 경량이다 보니 혹시나 뒤로 주저앉으면 로봇의 받침 다리가 충격을 버티지 못해 부러지지 않을까 걱정했지만 기우였다. 알고 보니 1.5㎏에 불과한 이 웨어러블은 로봇의 발 하나당 150㎏ 정도씩의 하중도 문제없이 받쳐준다고 한다. 기업과 생산직 근로자들이 웨어러블을 착용해야 하는지 고민할 때 가장 크게 고려하는 요소 중 하나가 탈착 시간과 가격이다. 보통 생산 현장에서 약 45~50분간 일하고 10~15분 쉬는 단위로 일하는 경우가 많은데 입고 벗는 것이 복잡해 5분·10분씩 걸린다면 생산성이 저하되고, 휴식 시간도 그만큼 빼앗겨 착용하기를 꺼릴 수밖에 없다. 첵스는 탈착이 간편하게 이뤄져 20초 정도면 충분히 입거나 벗을 수 있을 것 같았다. 하체를 지지해주는 기존의 주요 외산 웨어러블 제품이 약 3,000달러 안팎의 가격에 시판 중인 데 비해 첵스는 경쟁사 대비 절반 수준으로 전망돼 높은 가성비를 가질 것으로 보인다. 현대차의 웨어러블 로봇 4총사 중에는 ‘첵스’ 외에도 허리보조 로봇 ‘웩스(WEX)’, 하지마비 환자용 의료로봇 ‘멕스(MEX)’, 상체와 팔을 보조해주는 로봇 벡스(VEX)도 포함돼 있다. 이 중 웩스는 주로 서서 무거운 짐 등을 들어 올려 옮기는 근로자를 위해 이르면 내년부터 상용화될 것으로 전망된다. 미국 질병통제예방센터(CDC)에 따르면 팔·허리의 통증·부상 등을 비롯한 근골격계장애(WMDS)를 겪는 미국인 근로자는 연간 약 1억3,000만명(건강보험 적용 기준)에 달한다. WMDS로 인한 미국 사회의 경제적 비용(산재 보상, 임금 손실, 생산성 손실)은 한 해 450억~540억달러에 달한다는 미국 의학연구소의 보고서도 2000년대 초에 나왔다. 2007년 기준 유럽연합(EU) 27개 회원국 근로자 중 근육통증이 보고된 사례는 23%에 달했다는 ‘하중을 줄입시다(Lighten the load)’ 보고서가 유럽산업안전보건청 등을 통해 작성되기도 했다. 국내에서는 아직 WMDS에 대한 공식 통계를 찾기 어려운 상황이지만 제조 및 건설·물류현장 등에서 상당한 근로자들이 관련 질환을 겪고 있을 것으로 추정된다. 따라서 현대차가 자사 생산공장에서 품질과 실용성을 검증한 근로자용 웨어러블 로봇들을 단계적으로 상용화한다면 국내외 근로자들의 보건과 사회적 경제비용 절감에 큰 기여를 할 것으로 기대된다. /의왕=민병권기자 newsroom@sedaily.com | 저작권자 ⓒ 서울경제, 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>한일관계 최악에도…삼성, 日스마트폰 점유율 '6년만에 최고'</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>상반기 출시 '갤럭시S10' 인기 영향 풀이 2분기 점유율 9.8%…두자릿수 회복 보인다 지난 3월 문을 연 갤럭시 하라주쿠. 전 세계 갤럭시 전시장 가운데 규모가 가장 크다. /삼성전자 제공 삼성전자가 올해 2분기 일본 스마트폰 시장에서 6년 만에 가장 높은 점유율을 기록한 것으로 나타났다. 상반기 출시한 프리미엄 스마트폰 '갤럭시S10'의 인기를 누린 영향으로 분석된다. 26일 시장조사업체 스트래티지 애널리틱스(SA)에 따르면 삼성전자는 2분기 일본 스마트폰 시장에서 60만대를 출하했다. 시장 점유율 9.8%로 애플(50.8%)에 이은 2위다. 지난해 2분기 애플 45.6%, 삼성전자 8.8%였던 것과 비교해 모두 소폭 올랐다. 삼성전자는 2013년 중반까지 일본에서 두자릿수 점유율을 유지하다 애플과 일본 브랜드에 밀려 2014년 5.6%, 2015년 4.3%, 2016년 3.4%까지 점유율이 내려앉았다. 그러나 2017년 반등(5.2%)을 시작해 2018년 6.4%로 점유율을 끌어올리고 있다. 애플과 삼성전자에 이어 샤프(7.2%), 소니(7.0%) 등 일본 기업이 3∼4위를 차지했다. 샤프는 전년 동기(5.1%) 대비 2.1%포인트 올랐고, 소니는 10.3%에서 3.3%P 줄었다. 중국 화웨이는 전년 동기 5.9%(4위)에서 2분기 3.3%(5위)로 하락했다. 삼성전자는 일본에서의 점유율 확보 노력을 이어가고 있다. 올 3월 전세계 갤럭시 전시장 가운데 최대 규모인 '갤럭시 하라주쿠'를 개관한 삼성전자는 지난달 2020년 도쿄 올림픽을 기념해 '갤럭시S10 플러스 올림픽 에디션'을 일본에 출시했다. 5세대 이동통신망(5G) 서비스가 처음으로 본격 적용되는 도쿄 올림픽을 앞두고 일본 내 5G 네트워크 사업 확대를 위한 기반을 조성하는 동시에 갤럭시의 시장 점유율 상승 교두보를 마련한다는 복안이다. 노정동 한경닷컴 기자 dong2@hankyung.com ▶ ▶ ▶ ⓒ 한국경제 &amp;amp; , 무단전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>삼성전자, '갤럭시S10'으로 日서 6년만에 최고 점유율…화웨이는 하락</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>삼성전자가 올해 2분기 일본 스마트폰 시장에서 6년 만에 가장 높은 점유율을 기록한 것으로 조사됐다. 상반기 출시한 갤럭시S10 시리즈가 인기를 끌었기 때문으로 분석된다. 반면 화웨이는 작년 동기 대비 점유율이 절반 가까이 하락했다. 26일 시장조사업체 스트래티지 애널리틱스(SA)에 따르면 삼성전자는 2분기 일본 스마트폰 시장에서 60만대를 출하, 점유율 9.8%를 기록했다. 이는 애플(50.8%)에 이은 2위다. 작년 2분기 점유율이 애플 45.6%, 삼성전자 8.8%이었던 것과 비교해 모두 소폭 올랐다. 삼성전자가 10%에 육박한 점유율을 낸 것은 6년만에 최고치다. 삼성전자가 일본 하라주쿠에 문 연 ‘갤럭시 하라주쿠’ 전시관. /삼성전자 제공 삼성전자는 2013년 중반 일본 스마트폰 시장에서 10% 넘는 점유율을 유지하다 애플과 일본 브랜드에 밀려 2014년 5.6%, 2015년 4.3%, 2016년 3.4%로 점유율이 하락했다. 2017년부터 반등을 시작해 5.2%, 2018년 6.4%로 점유율이 상승 중이다. 애플과 삼성전자에 이어 샤프(7.2%), 소니(7.0%) 등 일본 기업이 3∼4위를 차지했다. 샤프는 작년 동기(5.1%) 대비 2.1%포인트 올랐고, 소니는 10.3%에서 3.3%p(포인트) 감소했다. 중국 화웨이는 작년 동기 5.9%(4위)에서 올해 2분기 3.3%(5위)로 하락했다. 한편 삼성전자는 올해 3월 전 세계 갤럭시 쇼케이스 가운데 최대 규모인 ‘갤럭시 하라주쿠’를 개관했다. 5G(5세대) 서비스가 처음으로 본격 적용되는 ‘2020 도쿄 올림픽’을 앞두고 일본 내 5G 네트워크 사업 확대를 위한 기반을 조성하는 동시에 갤럭시 스마트폰 시장점유율 반등의 계기를 마련한다는 전략이다. 삼성전자는 올 7월 2020 도쿄 올림픽을 기념해 갤럭시S10 플러스 올림픽 에디션을 일본에 출시하기도 했다. [이경탁 기자 kt87@chosunbiz.com] chosunbiz.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>헬리콥터도 부르면 온다… '차량 호출 끝판왕' 베트남</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>[세계를 보는 창 NOW] 호출 서비스 '글로벌 각축장' 관광지 투어·스카이웨딩까지 - 출퇴근·음식 배달은 기본 환자 이송·렌터카·택배… 26만원 내면 헬기도 "모십니다" 年 41% 성장, 6년후 20억불 시장 - 싱가포르 '그랩' 작년 진출 후 '셀로' 등 7개 업체 뛰어들어… 베트남 정부 "4차 혁명 총력" 이미지 특파원 베트남 호찌민에 사는 필리핀인 파이샤씨는 하루에 최소 3번은 차량 호출 서비스를 이용한다. 오전에는 오토바이 호출 서비스를 이용해 시내로 출근하고, 낮에는 차량 호출 서비스 앱의 음식 배달 서비스를 이용해 점심밥이나 커피를 시켜 먹는다. 가끔 한밤중에 밖에 나가기 귀찮으면 편의점에서 음료와 간식을 사다주는 서비스를 이용하기도 하고, 외부로 보내야 할 서류나 물품이 있을 때도 차량 호출 서비스 앱부터 연다. 파이샤씨는 "베트남은 다른 나라에 비해 차량 호출 서비스 업체가 많을 뿐 아니라 가격도 저렴하다"며 "택시 서비스 외에도 음식 배달, 택배 등 다양하게 이용하기 좋다"고 말했다. 베트남의 차량 호출 서비스 시장 경쟁이 치열해지고 있다. 작년 초, 글로벌 차량 호출업체인 '우버'가 싱가포르계 차량 호출업체인 '그랩'에 동남아시아 사업 부문을 넘기면서 베트남 차량 호출 시장은 그랩의 독점 체제로 변할 거란 예상이 많았다. 하지만 작년과 올해에만 셀로, 바토, 고비엣 등 7개의 업체가 차량 호출 시장에 새로 뛰어들었다. 업체 간 경쟁이 치열해지면서 시장점유율을 높이기 위해 트럭 호출이나 택배, 음식 배달 같은 다양한 서비스도 속속 등장하고 있다. ◇ 정부의 전폭적 지원과 함께 폭발적으로 성장하는 베트남 시장 베트남의 차량 호출 서비스 시장 규모는 작년 5억달러를 기록했다. 2015년 2억달러에 불과했던 시장이 3년 만에 2.5배로 늘어난 것이다. 성장세는 앞으로 더욱 가팔라질 것으로 보인다. 정부 차원의 전폭적인 지지도 차량 호출 서비스 시장을 키우는 데 일조하고 있다. 응우옌 쑤언 푹 베트남 총리는 직접 "베트남이 혁신적인 기업들을 환영한다는 것을 보여주기 위해서 차량 공유 서비스에 지장을 주는 불필요한 장벽을 제거하라"고 지시했다. 하노이·호찌민 등 대도시 위주로 영업하던 차량 호출 업체들은 전국으로 서비스 범위를 확대하고 있다. 구글·테마섹홀딩스의 2018년 동남아시아 경제보고서에 따르면 베트남의 차량 호출 서비스 시장은 연평균 41%의 성장률을 기록해 2025년 20억달러 규모까지 확대될 전망이다. 차량 호출 서비스의 성장은 버스·택시 등 기존 교통수단 시장을 위협하는 수준에 이르렀다. 브이엔익스프레스 등 현지 언론에 따르면 차량 호출 서비스가 활성화되면서 올해 1~4월 공공 버스를 이용한 탑승객은 전년 동기 대비 8.9% 줄었다. 베트남 교통부에 따르면 작년 버스 탑승객은 목표보다 10% 적었고, 공공버스 운영 업체는 16억달러의 손실을 기록했다. 택시업계도 마찬가지다. 베트남 택시업체인 비나선과 마일린도 앱을 내놓고 차량 호출 서비스 업체에 대응하고 있지만 매출 감소를 막지는 못했다. 이에 비나선은 "그랩 때문에 420억동의 손실을 입었다"며 손해배상 청구 소송을 냈고, 작년 12월 법원은 "그랩은 비나선에 48억동(약 2억5000만원)을 배상하라"고 판결했다. 그랩은 판결에 불복해 항소했지만 다낭 등 다른 지역의 택시협회도 소송을 검토하고 있어 갈등이 예상된다. ◇ 헬리콥터, 트럭 등 영역 넓혀…글로벌 업체도 눈독 차량 호출 업계 간 경쟁도 만만치 않다. 업체들은 기본적으로 제공해온 차량이나 오토바이 택시 서비스 외에 트럭 호출, 렌터카 등 사업 영역을 넓히고 있다. 올해 4월 차량 호출업체 패스트고는 패스트스카이라는 브랜드로 베트남 최초의 '헬리콥터 호출 서비스'를 내놓았다. 하노이 홍강(紅江)이나 할롱베이 같은 관광지를 둘러보는 스카이투어, 웨딩 촬영을 지원하는 스카이웨딩, 응급환자를 이송하는 스카이SOS, 사업가 등이 업무에 필요할 때 쓸 수 있는 스카이플러스 등 4가지로 구성된다. 가격은 1인당 500만동(26만원)부터 시작되고 최대 12명이 함께 이용할 수 있다. 베트남 차량 공유 업체인 패스트고(FastGo)가 올해 새로 출시한 헬리콥터 공유 서비스 홍보물. 헬리콥터가 베트남의 유명 관광지인 할롱베이 상공을 날고 있다. /FastGo 베트남 국방부 산하 업계 1위 통신업체인 비엣텔은 지난 7월 마이고라는 차량 호출 서비스를 내놓으며 트럭 호출 서비스를 시작했다. 총 등록 차량 10만5000대 중 600대가 트럭이다. 트럭 호출 서비스의 등장은 이사나 택배 같은 대규모 배송 업체의 영역까지 넘볼 수 있을 것으로 보인다. 자체 앱에 등록된 오토바이나 차량 기사를 활용한 영역 확장도 활발하다. 오토바이 기사가 음식이나 물품 배달 서비스를 하고, 차량 기사로 등록된 사람이 시간제 렌터카 기사로도 활동하는 식이다. 그랩은 음식 배달 서비스를 시작한 지 1년 만에 주문 건수가 250배 증가했다고 밝혔다. 최근 차량 호출 서비스 업체들은 모바일 결제 시스템 업체들과 손잡고 현금 없는 비용 결제 시스템 구축에도 나서고 있다. 업체들의 경쟁은 더욱 치열해질 것으로 전망된다. 글로벌 업체들까지 속속 베트남 시장에 진출하고 있기 때문이다. 베트남 정부는 2009년부터 스타트업 육성 지원 프로그램을 마련하는 등 4차 산업을 적극 지지하고, 창업을 독려하고 있다. 응우옌 쑤언 푹 총리는 올해 1월 다보스포럼에서 "베트남은 4차 산업 혁명을 기술의 하나가 아닌 '정책 혁명'이라 보고 있다"며 "글로벌 기업들이 베트남에 와서 4차 산업 제품을 생산하길 바란다"고 말했다. [호찌민=이미지 특파원 image0717@chosun.com] - Copyrights ⓒ 조선일보 &amp;amp; chosun.com, 무단 전재 및 재배포 금지 -</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>"렌터카보다 싸게, 리스보다 짧게…중고차 '구독' 하세요"</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>[머니투데이 서진욱 기자] [[인터뷰]전민수 더트라이브 대표 "중고차 구독 '트라이브' 적은 비용, 짧은 계약기간 차별점"] 전민수 더트라이브 대표. /사진제공=더트라이브. "이제 중고차도 '구독'하세요." 정기적으로 사용료를 내고 제품 또는 서비스를 이용하는 ‘구독경제’가 빠르게 퍼지고 있다. 배달음식(요기요), 운동화(나이키), 커피(버거킹, GS25) 등 선결제가 어색하던 영역에서도 구독경제 실험이 한창이다. 자동차 시장에서도 구독 사업모델이 급성장하고 있다. 글로벌 투자은행 크레딧스위스에 따르면 2020년 미국 자동차 구독 시장은 5300억달러(약 642조원) 규모로 커질 것으로 전망된다. 전민수 대표(사진·37)가 이끄는 스타트업(초기 벤처기업) 더트라이브는 중고차 구독 서비스 ‘트라이브’ 앱 출시를 준비 중이다. 신차 대비 저렴한 가격과 장기 렌트 대비 짧은 계약기간을 앞세워 중고차 구독 서비스 대중화를 노린다. 전 대표는 “트라이브는 자동차 구매, 목돈 지출에 대한 부담 없이 차량을 이용할 수 있는 구독 서비스”라며 “이달 중 시범 테스트에 돌입할 예정”이라고 말했다. 트라이브는 다양한 가격대의 구독 서비스를 제공, 사용자가 해당 가격대에 속한 차종 중 자신이 원하는 차종을 선택할 수 있다. 벤츠 E클래스 기준 구독료는 월 70만원(1년 약정) 정도다. 보험료와 취·등록세가 포함된 가격이다. 같은 차량의 렌터카(6개월 약정), 리스(36개월 약정) 비용은 각각 월 250만원, 80만원 정도다. 트라이브는 렌터카보다 저렴한 가격, 리스보다 짧은 계약기간으로 차량을 이용할 수 있다. 전 대표는 “사용자 설문 결과를 바탕으로 중고차 판매가 기준 구독료 공식을 자체 개발했다”며 “공식을 활용해 적절한 구독료를 책정한다”고 말했다. 구독 서비스를 위한 중고차는 자체 상사와 딜러, 다른 업체들과 제휴를 통해 확보할 예정이다. 수원중고차 매매단지에서 중고차 매입 및 판매를 위한 상사를 직접 운영 중이다. 정식 출시 전 10곳 이상 제휴 업체들을 확보해 구독용 중고차를 확보할 계획이다. 전 대표는 “특정 제조사, 차종 구독 모델과 달리 사용자에게 다양한 차종을 제공한다”고 말했다. 트라이브는 세밀한 차량 관리 서비스도 제공한다. 차량진단모듈(OBD)을 활용해 차량 상태와 사고 여부를 진단한다. 정기 점검을 비롯해 사고, 고장 등 문제 발생 시 전담 직원이 처리한다. 세차, 대리, 시승 등 차량 연계 서비스도 제공할 예정이다. 전 대표는 “자동차 시장 패러다임이 소유에서 이용으로 넘어오는 단계”라며 “트라이브로 이용 절차를 단순화해 중고차 구독 시대를 열겠다”고 포부를 밝혔다. 또 “연내에 트라이브 구독자 300명을 확보하는 게 최우선 목표”라며 “쉽고 간편한 중고차 구독 서비스로 발전할 수 있도록 지속적으로 노력하겠다”고 말했다. 한편 더트라이브는 중소벤처기업부의 민간 투자 주도형 기술 창업 지원 프로그램 ‘팁스’ 과제도 수행 중이다. 현대자동차(팁스 운영사)와 함께 인공지능(AI) 기반 자동차 매매 로보어드바이저 기술을 개발하고 있다. AI 기술 기반으로 매입가, 판매가, 수요, 공급 등을 예측할 수 있는 솔루션을 구축하는 게 목표다 서진욱 기자 sjw@mt.co.kr &amp;lt;저작권자 ⓒ '돈이 보이는 리얼타임 뉴스' 머니투데이, 무단전재 및 재배포 금지&amp;gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>활명수 스킨·마데카솔 크림… 제약업계 화장품 바람 솔솔</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>의약품 기술력으로 화장품 사업, 40개사 진출 시장규모 5000억 휴메딕스, 필러 성분 마스크팩… 일동제약 상반기 매출만 99억 중소업체는 유통망 못찾아 고전 주름 개선제의 일종인 필러를 만드는 휴메딕스 는 최근 '아미노 포텐셜 마스크'라는 마스크팩 신제품을 선보였다. 제품에는 필러의 주(主)성분인 히알루론산이 포함됐다. 피부 아래 주입하는 필러는 주름을 펴는 역할을 하며, 이 성분을 피부에 바르면 보습 효과가 있다. 의약품 효과를 활용한 화장품인 셈이다. 회사 관계자는 "2년 전부터 필러 성분을 활용한 30여 가지 신제품을 선보였다"며 "지난해에만 화장품 사업은 매출 30여 억원을 기록한 효자 부업(副業)"이라고 말했다. 휴메딕스의 코스메슈티컬 브랜드 더마 엘라비에. 제약·바이오 회사들이 의약품 개발·생산으로 얻은 기술력을 활용해 화장품 사업에 대거 뛰어들고 있다. 의학적으로 검증된 의약품 성분을 넣은 기능성 화장품을 선보이는 것이다. 이런 화장품이 인기를 끌면서 코스메슈티컬(cosmeceutical)라는 신규 시장이 급부상하고 있다. 화장품(cosmetics)과 의약품(pharmaceutical)을 합한 신조어다. 국내 시장 규모는 5000억원으로 추정된다. 국내 화장품 시장(약 13조원)의 4% 수준이다. 의약품 성분으로 입증된 성분을 쓰다 보니 소비자들의 신뢰도가 높아, 시장은 급팽창하고 있다. GS리테일 이 운영하는 헬스 앤드 뷰티 스토어 '랄라블라'에 따르면 올해 1~7월에 코스메슈티컬 상품 매출은 동기 대비 83% 늘었다. ◇ 40여 제약·바이오社 화장품 진출 동화약품 활명, 동국제약 센텔리안24 제약업계는 최근 2~3년 새 제약·바이오사 40여 곳이 화장품 사업에 진출한 것으로 추정한다. 이미 보유한 의약품 기술을 그대로 활용할 수 있어 화장품 시장 진입이 수월하다. 대표적 제품이 동국제약 이 내놓은 마데카크림이다. 상처 치료제로 잘 알려진 마데카솔의 주 원료로 만들었다. 동국제약은 아예 '센텔리안24'라는 화장품 브랜드도 내놓았다. 소화제 까스활명수로 유명한 동화약품 은 활명수에 쓰는 5가지 생약 성분을 포함한 스킨케어 제품을 내놓고 있다. 줄기세포를 연구 개발하는 차바이오텍 은 노화 방지 크림과 같은 제품을 속속 선보이고 있다. 큐티젠랩 은 세포 배양액을 이용한 주름 개선 기능성 화장품을 내놓았다. 반대로 화장품 회사들은 제약 기술 확보를 위해 제약·바이오 업체들과 손잡고 있다. 국내 화장품 업계의 '빅2'인 LG생활건강 이 2년 전 제약업체 태극제약 을 인수한 게 대표적인 사례다. 태극제약이 올 초 아토피와 같은 피부 질환에도 좋은 크림과 로션을 내놨는데 여기엔 태극제약과 LG생활건강의 노하우가 활용됐다. 화장품 업계 관계자는 "제약사와 화장품 회사의 노하우가 합쳐지면서 이전과 전혀 다른 신개념 제품이 나오고 있다"고 말했다. 화장품 ODM(제조자 개발 생산) 업체인 한국콜마 는 지난해 제약사인 CJ헬스케어 를 인수하기도 했다. ◇ 중소 업체는 유통망 확보 어려워 실제 성공 사례도 나오고 있다. 동국제약은 지난해 화장품 부문에서 매출을 약 540억원 기록했다. 전체 매출 가운데 화장품 비율이 16%다. 일동제약 은 유산균 성분이 들어간 마스크팩이 성공을 거두며, 올 상반기에 화장품 매출이 99억원을 기록했다. 반면 중소 제약 업체는 대부분 섣부르게 진출했다가 가시적 매출 성장을 내지 못하고 있다. 화장품 시장은 제품 효능 못지않게 브랜드 파워와 현장 유통망 확보가 중요하기 때문이다. 중소 제약 업체 대다수는 매출 대부분을 약국에 의약품을 공급하는 B2B(기업 간 거래) 방식에서 얻고 있다. 새로운 유통망 확보에 어려움이 있는 것이다. 중소 제약 업체 관계자는 "아무리 기능성을 강조해도 중소 제약 업체 브랜드는 일반 소비자들에게 낯선 제품에 불과하다"며 "막대한 자본력으로 이미지 마케팅을 벌이는 대형 화장품 브랜드와 경쟁하기 쉽지 않은 게 현실"이라고 말했다. ☞코스메슈티컬(cosmeceutical) 화장품(cosmetics)과 의약품(pharmaceutical)을 합성한 신조어. 화장품에 의학적으로 검증된 성분이 들어간 제품을 말한다. 미백이나 주름 개선 같은 기능성 화장품에 주로 쓰인다. [유지한 기자 jhyoo@chosun.com] - Copyrights ⓒ 조선일보 &amp;amp; chosun.com, 무단 전재 및 재배포 금지 -</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>코오롱티슈진, 턱밑까지 온 상폐 위기…"남은 절차 최선"</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>한국거래소, 기업심사위원회 개최해 상장 폐지 결정 (서울=연합뉴스) 박동주 기자 = 26일 오후 서울 강서구 코오롱생명과학 본사 앞. pdj6635@yna.co.kr (서울=연합뉴스) 김잔디 기자 = '인보사 사태'의 코오롱티슈진은 26일 한국거래소의 상장폐지 결정에 당혹스러움을 감추지 못하면서도 아직 확정되지 않은 만큼 남은 절차에 최선을 다하겠다는 입장을 내놨다. 코오롱티슈진 관계자는 26일 연합뉴스와 통화에서 "아직 코스닥시장위원회 등이 남아있다"며 "남은 절차에서 최선을 다하겠다"고 말했다. 거래소 코스닥시장본부는 이날 기업심사위원회(기심위) 심의 결과 코오롱티슈진의 주권 상장폐지를 결정했다고 밝혔다. 다만 이번 심사는 상장 폐지를 확정하기 위한 절차 중 하나여서 아직 확정된 것은 아니다. 거래소는 앞으로 코스닥시장위원회에서 이를 다시 논의하고, 여기서 상장폐지가 결정돼도 회사의 이의신청을 받아 심사하는 절차가 남아있다. 코오롱티슈진 이런 남은 절차에 사활을 걸겠다는 입장이다. 현재 코오롱티슈진은 인보사 사태로 품목허가가 취소된 것은 물론 미국에서의 임상 중단, 소액주주 소송 등의 악재가 겹겹이 쌓여있는 상황이어서 상장 폐지되면 기업 존립 자체가 어려워지지 않겠느냐는 우려도 나온다. 코오롱티슈진은 인보사 개발과 적응증(치료범위) 확대를 주된 사업으로 꾸려왔는데, 핵심 사업인 인보사의 결함으로 시장에서 퇴출당할 경우 그 여파가 적지 않을 것이라는 분석이다. 인보사의 매출 비중이 미미한 코오롱생명과학과 달리 코오롱티슈진은 사실상 인보사를 위한 회사라고 해도 무방하다. 사업보고서에 따르면 코오롱티슈진은 인보사를 기존에 허가받은 무릎 골관절염 외에도 추간 디스크, 고관절 골관절염, 동물 골관절염 등에 쓰기 위한 연구개발을 진행해왔다. 단 코오롱티슈진은 기심위에서 논의된 내용과 결과를 구체적으로 확인하지 못했다며 향후 대응 방안에 대해서는 밝히지 않았다. 이와 별도로 미국에서의 인보사 임상시험 재개를 위한 준비는 계속 진행하고 있다. 인보사는 주성분이 뒤바뀐 사실이 알려지면서 미국에서 진행되던 임상 3상이 중단됐다. 코오롱티슈진 관계자는 "미국 임상 (재개를 위한)은 이번 사안과는 별개로 서류를 제출할 예정"이라며 "미국 식품의약품청(FDA)의 리뷰를 통해 재개가 결정될 것"이라고 말했다. 인보사는 2017년 국내 첫 유전자 치료제로 식약처 허가를 받았으나, 주성분 중 하나가 허가사항에 기재된 연골세포가 아닌 종양을 유발할 가능성이 있는 신장세포라는 사실이 드러나 허가 취소됐다. 코오롱생명과학의 미국 자회사인 코오롱티슈진이 개발했다. 코오롱생명과학과 코오롱티슈진은 인보사 성분이 뒤바뀌었더라도 그동안 진행돼온 임상시험 결과로 보아 안전성 및 효능에는 문제가 없다고 주장하고 있다. jandi@yna.co.kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>갤노트10, 자급제 물량 풀고 사전예약 개통 연장</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>[디지털데일리 권하영기자] 삼성전자가 당초 26일까지로 예정된 갤럭시노트10 사전예약 개통 기간을 오는 31일까지 연장한다. 자급제폰 물량도 29일부터 시장에 공급하기로 했다. 초반 130만대 사전판매 물량을 확보한 노트10 호조를 이어갈지 주목된다. 26일 삼성전자는 삼성닷컴 공지를 통해 “일부 매장별 컬러·용량 등 재고 불균형 및 불가피한 사정으로 기간 내 개통이 어려운 고객을 위해 전 모델을 대상으로 사전예약자 개통 기간과 사은품 신청 기간을 연장한다”고 밝혔다. 이는 유통 판매처에서 노트10 물량 부족으로 개통이 연기되고 있는 사정을 감안한 결정이다. 일부 판매처에서 과도한 보조금을 약속했다가 개통이 지연되거나 취소되는 사례가 빗발치면서 시장 과열을 바로잡으려는 후속 조치로도 읽힌다. 삼성전자는 앞서 9일부터 19일까지 갤럭시노트10 시리즈 사전예약을 받았다. 이에 따라 고객들은 26일까지 개통을 완료해야 사전예약을 통한 다양한 경품과 혜택을 받을 수 있다. 그런데 사전예약 기간에 일부 판매점이 노트10에 대해 10~20만원대 판매를 약속했다가 취소하는 사례가 속출하면서 문제가 됐다. 이들은 통신사 정책과 판매장려금(리베이트)을 높게 예상했다가 그에 못 미치자 일방적으로 사전예약을 취소하거나 연락을 두절하기 시작한 것. 갤럭시노트10 출고가는 128GB 기준 124만8500원(128GB 기준)이다. 갤럭시노트10을 10~20만원대로 판매하려면 사실상 불법 보조금이 5~60만원대로 지급돼야 한다. 통신3사의 노트10 공시지원금은 고가 요금제를 쓰더라도 당초 예상보다 적은 42~45만원이다. 통신사 관계자는 “일부 판매처에서 하반기 5G 신규폰에 대한 지원금 정책이 좋을 것으로 보고 무리하게 가입자를 확보한 면이 있다”면서 “이들의 사전예약 취소로 기간 내에 정상적으로 개통하지 못한 이용자들이 늘어나고 있다”라고 말했다. 갤럭시노트10에서 새롭게 선보이는 통신사 전용 색상 단말이 예상보다 높은 인기를 끈 점도 배경 중 하나다. 현재 SK텔레콤은 블루, KT는 레드 컬러를 단독 출시한 상태다. 통신사 관계자는 “신규 컬러에 대한 소비자 호응이 좋아 추가 물량을 확보해야 하는 상황”이라고 전했다. 삼성전자는 사전예약 개통기간 연장과 함께 노트10 자급제폰 물량을 오는 29일부터 공급한다. 자급제폰은 통신사 대리점 및 판매점에서 요금제와 연계해 판매하는 것과 달리 유심칩만 끼우면 바로 사용할 수 있는 단말기다. 통신사 약정 기간이나 위약금으로부터 자유롭다. 삼성전자가 자급제 물량 공급과 함께 사전예약 개통 기간을 연장하면서 개통이 지연 또는 취소되거나 원하는 단말을 선택하지 못한 소비자들이 이달 말까지 여유를 가지게 됐다. 노트10 자급제폰은 삼성닷컴·오픈마켓 등 온라인 유통채널과 삼성디지털프라자·롯데하이마트 등 오프라인 유통채널에 본격 공급된다. 공식 출시일인 23일부터 주문을 받고 29일부터 순차 배송할 예정이다. &amp;lt;권하영 기자&amp;gt;kwonhy@ddaily.co.kr &amp;lt;저작권자 © 디지털데일리 무단전재-재배포금지&amp;gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>삼성 판결 D-2, 이재용 부회장 아산서 디스플레이 현장경영</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>이재용 부회장 박근혜 전 대통령과 최순실씨, 이재용 삼성전자 부회장이 연루된 국정농단 사건의 대법원 선고가 이틀 앞으로 다가왔다. 재계도 이 부회장 관련 판결에 촉각을 곤두세우고 있다. 일본의 대 한국 경제 보복, 보호무역주의 강화 등으로 삼성을 둘러싼 대내외 경제 상황이 악화된 가운데 이 부회장의 부재가 가져올 파장이 우려되기 때문이다. 대법원 전원합의체는 오는 29일 오후 박 전 대통령의 특정범죄 가중처벌 등에 관한 법률 위반(뇌물) 등 혐의에 대한 상고심 선고 기일을 연다. 함께 재판에 넘겨진 최씨와 이 부회장 상고심 판단도 같은 날 내려진다. 쟁점은 삼성이 최씨 딸 정유라씨에게 제공한 말 세 마리의 소유권 이전과 '경영권 승계작업' 인정 여부다. 박 전 대통령과 최씨 1·2심은 말 세 마리에 대가성이 있다고 판단, 뇌물로 인정했다. 이 부회장 1심도 같은 취지의 판단을 했다. 그러나 2심에서는 말 세 마리 소유권이 최씨에게 넘어가지 않았다며 뇌물로 인정하지 않았다. 같은 사안에 대해 하급심 판단이 갈렸기 때문에 대법원의 최종 판결에 따라 한쪽은 파기 환송돼 2심을 다시 받을 것으로 예상된다. 세 피고인 모두 항소심을 다시 받을 가능성도 있다. 대법원이 말 소유권 이전과 승계 작업 둘 가운데 하나만 인정할 경우 세 사건 모두 파기 환송돼 재판을 다시 받을 것으로 보인다. 재계의 최대 관심사는 판결 결과다. 이 부회장이 다시 구속된다면 삼성 경영에 불확실성이 추가로 등장하기 때문이다. 이 부회장은 지난해 2월 집행유예로 풀려난 이후 국내외에서 활발한 경영 행보를 펼쳤다. 특히 인공지능(AI), 시스템반도체, 해외 생산 거점 등 미래 먹거리에 집중해서 챙겼다. 시스템반도체 분야에 2030년까지 133조원을 집중 투자, 글로벌 1위를 달성하겠다는 비전도 내놓았다. 이 부회장이 다시 구속되면 삼성의 미래 전략 사업과 혁신 계획이 중단되거나 지연될 수 있다는 우려가 안팎에서 나온다. 특히 최근 일본 경제 보복으로 말미암아 위기가 고조됐을 때 일본과 국내 주요 사업장을 오가며 위기 타개를 위해 노력해 왔다. 수출 중단이 시작되기 전 일본 회사 소재 재고 확보에 나서고, 대체 공급처 발굴과 국산화 추진 등 비상 대책을 주도했다. 이재용 삼성전자 부회장(왼쪽 두번째)이 26일 충남 아산에 위치한 삼성디스플레이 사업장에서 제품을 살펴보고 있다. 이달 들어서는 현장 경영에 박차를 가하고 있다. 이 부회장은 6일 삼성전자 온양·천안사업장을 시작으로 평택사업장(9일), 광주사업장(20일)을 찾은 데 이어 26일에는 디스플레이 아산사업장을 방문해 전자계열사 밸류체인 점검과 미래 신성장 동력 발굴을 위한 현장 경영을 이어 가고 있다. 이날 삼성디스플레이 사업장을 방문한 자리에서는 중장기 사업 전략을 점검하고, 대형 디스플레이 로드맵 등 미래 신기술 전략을 논의했다. 이 자리에는 김기남 삼성전자 DS부문 대표이사 부회장, 이동훈 삼성디스플레이 대표이사 사장, 김성철 중소형디스플레이사업부장 부사장, 남효학 대형디스플레이사업부장 부사장, 곽진오 디스플레이연구소장 부사장 등이 함께했다. 이 부회장은 “위기와 기회는 끊임없이 반복된다. 지금 액정표시장치(LCD) 사업이 어렵다고 해서 대형 디스플레이를 포기해서는 안 된다”면서 “신기술 개발에 박차를 가해 다가올 새로운 미래를 선도해야 하고, 기술만이 살 길”이라고 강조했다. 권건호 전자산업 전문기자 wingh1@etnews.com [Copyright ⓒ 전자신문 &amp;amp; 전자신문인터넷, 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>[단독]세계 2위 모빌리티 中 디디추싱, 내년 상반기 韓 진출</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>-투자전문 회사 미래오성과 합자회사 진출 계약 진행 중 -플랫폼택시·11인승 대형 택시 등 준비 디디추싱 이미지(출처=디디추싱) [헤럴드경제=채상우 기자] 세계 2위 모빌리티 기업인 중국의 디디추싱이 이르면 내년 상반기 한국에 진출한다. 26일 투자전문회사 미래오성그룹에 따르면 최근 디디추싱과 미래오성그룹은 한국 지사 설립 계약을 진행 중이며 이르면 내년 상반기 한국에 지사를 설립할 예정이다. 미래오성그룹 관계자는 "현재 디디추싱과 2020년 한국 진출을 목적으로 긴밀히 얘기 중"이라며 "모바일 플랫폼 구성까지 대략적으로 완료한 상황으로 디디추싱 본사의 결정만 기다리고 있다"고 말했다. 디디추싱은 지난해 일본에 진출할 때도 소프트뱅크와 합자 투자를 하는 방식이었다. 미래오성그룹은 이를 위해 최근 가산디지털단지에 디디추싱 코리아 사무실을 개설했으며, 김범창 미래오성그룹 회장을 디디추싱 코리아 대표로 임의 등록해 놓은 상태다. 디디추싱이 한국에 들어오면 카카오모빌리티와 같이 택시 플랫폼 서비스를 선보일 것으로 예상된다. 아울러 11인승 대형 차량을 이용한 대형 택시 서비스도 준비 중에 있는 것으로 알려졌다. 디디추싱의 한국 진출 배경에는 최근 국토부의 택시-플랫폼 상생안 발표 등으로 국내 모빌리티 시장이 성장기에 돌입했다는 판단 때문으로 분석된다. 업계에서는 디디추싱 한국 진출을 위해 미래오성그룹은 이미 올해 초부터 발빠르게 움직인 것으로 파악하고 있다. 김범창 회장은 올해 4월 중국 상하이에서 개최된 '중국 라이드헤일링 산업 발전 포럼'에 참석해 디디추싱 관계자를 직접 만나 국내 모빌리티 사업에 대해 논의를 했다. 김 회장은 이 자리에서 "중국의 차량공유플랫폼 기업과 손잡고 수년간 플랫폼 사업을 통해 축적한 노하우를 한국에 도입해 한국형 차량공유 플랫폼 사업을 성공시키겠다"고 밝혔다. 2012년 설립한 디디추싱은 기업가치 560억달러(약 67조원)에 달하는 중국업체로 베이징에 본사를 두고 있다. 우버에 이어 세계 2위 모빌리티 기업으로 중국 시장 점유율은 90%에 달한다. 일본과 대만, 동남아, 북미·남미 등 전세계 1000개 도시에서 사업을 운영 중이다. 디디추싱은 최근 세계 1위 기업인 우버를 앞지르기 위해 다양한 국가 진출을 적극적으로 검토 중에 있는 것으로 알려졌다. 올해 초에는 칠레, 페루, 콜롬비아 등 남미 국가에서 마케팅·광고·위기관리·사업 직군 관리자를 채용하며 남미 시장을 공략했다. 한국 역시 세계 진출 방안의 하나로 분석된다. 다만 디디추싱은 한국에서 벌어지고 있는 택시와 모빌리티 간의 갈등을 우려하고 있는 것으로 알려졌다. 업계 관계자는 "디디추싱이 한국 진출에 있어 마지막으로 고민하는 것이 택시와의 갈등 문제로 알려졌다"며 "최근에는 정부 주도로 이 문제가 조금씩 풀리는 양상이 보이고 있지만 여전히 개인택시를 중심으로 해결되지 않은 문제가 존재해 이 부분을 우려하고 있는 것으로 알고 있다"고 말했다. 123@heraldcorp.com - Copyrights ⓒ 헤럴드경제 &amp;amp; heraldbiz.com, 무단 전재 및 재배포 금지 -</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>삼성의 현명한 선택? 美 1%만 이어폰잭 신경쓴다</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>갤럭시노트10 플래그십폰 처음으로 이어폰잭 배제 "무선이어폰의 보편화"로 때가 됐다는 판단 덕분에 미니멀리즘 디자인 도입 성공 "때가 됐다." 강윤제 삼성전자 디자인팀장은 최근 이어폰잭을 없앤 첫 플래그십폰 '갤럭시노트10'을 출시하며 이렇게 말했다. 무선이어폰으로의 급속한 전환 속에 삼성전자도 과감한 선택을 할 때가 됐다는 뜻이었다. 여전히 이어폰잭이 필요하다는 목소리가 있었지만 어쩌면 삼성전자가 현명한 선택을 한 것일지도 모르겠다. 삼성전자의 최대 시장인 미국을 조사한 결과 소비자의 단 1%만이 스마트폰 구매 시 '이어폰잭의 유무'를 중시하는 것으로 나타났다. 25일(현지시간) 미국 알뜰폰 사업자 팅의 설문조사에 따르면 소비자가 스마트폰 구매 시 가장 중요하게 생각하는 요소는 가격이었다. 응답자의 35%는 가격에 따라 구매 여부를 결정한다고 답했다. 팅은 소비자 3600명에게 가장 중시하는 요소 세 가지를 고르게 하는 방식으로 조사를 진행했다. 가격 다음으로는 운영체제(30%), 성능(14%), 화면(5%), 배터리(4%), 디자인(2%)이 중시됐다. 이어폰잭을 중요한 요소 세 가지 중 하나로 꼽은 소비자는 1%에 불과했다. 미국 IT매체 안드로이드 어쏘리티는 "스마트폰 가격이 궁금한 소비자는 많지만 이어폰잭에 관심 있는 사람은 거의 없는 것으로 나타났다"며 "이번 설문조사는 이어폰잭이 사라지는 때가 왔음을 암시하는 또 다른 지표가 될 것"이라고 분석했다. 실제로 무선이어폰은 급속히 확산되는 추세다. 시장조사업체 스트래티지 애널리틱스에 따르면 무선이어폰 시장은 2016년 170만대, 2017년 1510만대, 2018년 3360만대로 성장했다. 특히 애플이 2016년 아이폰7부터 이어폰잭을 없애면서 전체 이어폰 시장에서 무선이어폰이 차지하는 비율은 절반을 넘어섰다. 삼성전자는 유선이어폰을 선호하는 소비자를 위해 이어폰잭을 남겨뒀지만 무선이어폰의 보편화를 감지하고 갤럭시노트10에서 처음으로 변화를 꾀했다. 이를 통해 얇은 디자인 구현이 가능해지기 때문이다. 게다가 이번 조사로 이어폰잭을 중시하는 소비자가 소수에 불과함이 드러난 만큼 삼성전자는 갤럭시S11, 갤럭시노트11의 이어폰잭 역시 배제할 가능성이 높다. 이는 미국에서 3위 점유율을 차지하고 있는 LG전자의 이어폰잭 전략에도 적잖은 영향을 미칠 것으로 보인다. 임온유 기자 ioy@asiae.co.kr &amp;lt;ⓒ경제를 보는 눈, 세계를 보는 창 아시아경제 무단전재 배포금지&amp;gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>삼성 스마트폰, 日 점유율 6년만에 최고…"갤S10 통했다"</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>1위 애플 50.8%, 화웨이 美 제재 영향으로 5위로 하락 (지디넷코리아=이은정 기자)삼성전자가 지난 2분기 일본 스마트폰 시장에서 6년 만에 역대 최고 점유율을 기록한 것으로 나타났다. 26일 스트래티지 애널리틱스(SA)에 따르면, 지난 2분기 일본 스마트폰 시장에서 애플이 전년 동기(45.6%) 대비 증가한 50.8%의 점유율로 1위를 기록했다. 2위 삼성전자는 2분기 일본 스마트폰 시장에서 전년 동기(8.8%)보다 소폭 상승한 9.8%의 점유율로 6년 만에 역대 최고치를 기록했다. 삼성전자는 2013년 두 자릿수의 점유율을 기록했지만 2014년부터 지난해까지 6%대 이하의 점유율을 기록했다. 삼성전자가 점유율 반등에 성공한 데는 갤럭시S10 호조의 영향이 컸다는 분석이 나온다. 삼성전자 갤럭시S10 일본 현지 광고모델 기무라 코우키.(사진 출처= Instagram@koki) 삼성전자 갤럭시S10 일본 현지 광고모델 기무라 코우키.(사진 출처= Instagram@koki) 삼성전자는 갤럭시S10이 출시된 지난 3월 갤럭시 쇼케이스 중 최대 규모인 '갤럭시 하라주쿠'를 도쿄에 개관하고 현지 스마트폰 시장 공략에 집중했다. 이후 2020년 도쿄올림픽을 앞두고 일본 5G 네트워크 사업을 확대를 위한 기반을 조성, 일본에서 갤럭시 스마트폰 시장 점유율 반등에 속도를 내고 있다. 삼성전자에 이어 3~4위는 일본 기업인 샤프와 소니가 차지했다. 샤프는 지난해 같은 기간(5.1%)보다 소폭 오른 7.2%를 기록했으며, 소니는 3.3% 감소한 7.0%의 점유율을 기록했다. 중국 화웨이는 전년 동기(5.9%) 대비 줄어든 3.3%의 점유율로 5위로 하락했다. 이는 미국의 거래중단 제재 조치 여파가 있었던 것으로 풀이된다. 지난 5월 일본 이통사 KDDI와 소프트뱅크, NTT도코모는 미국의 화웨이 장비 사용 금지 행정명령에 따른 영향력을 평가하기 위해 시간이 필요하다며 화웨이의 신규 스마트폰 판매를 연기한 바 있다. 이은정 기자(lejj@zdnet.co.kr) /</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>[단독] MS, 쿠팡·티몬에 경고…"불법 윈도10 팔지마"</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>개인 판매자들, 정품으로 속여 20만원짜리 2500원에 판매 "제품키 판매, 저작권법 위반" 대법 판결 이후 온라인몰 단속 마이크로소프트(MS)의 한국 지사인 한국MS가 윈도10 등 자사의 소프트웨어 불법 판매 단속에 나섰다. 쿠팡, 티몬 등 온라인 쇼핑몰에서 윈도10과 MS오피스 등이 정가의 1%대 수준 가격에 판매되자 ‘철퇴’를 빼들었다. 2500원이면 윈도10 구입 25일 정보기술(IT)업계에 따르면 최근 한국MS는 자사의 소프트웨어가 불법으로 판매되고 있다며 국내 온라인 쇼핑몰 업체에 협조공문을 보냈다. 일부 판매자가 윈도10, MS오피스 등을 정품이라 속이고 제품키를 발송하는 방식으로 팔고 있는 것을 단속해달라는 것. 제품키는 소프트웨어를 설치할 때 사용자가 정품을 사용했다는 것을 인증하기 위해 입력해야 하는 문자 및 숫자로 구성된 고유의 번호다. 윈도10 소프트웨어는 MS 홈페이지에서 다운받고, 정품 제품키를 결제해 입력하면 사용할 수 있다. 쿠팡, 티몬 등에서는 불법 윈도10 등을 파는 판매자가 수백 명에 이른다. 판매 가격은 최저 2500원이다. 정품(20만원)의 100분의 1 수준이다. 이들은 ‘초특가 판매’ ‘정품이 아닐 경우 100% 환불’ ‘제품키 24시간 실시간 발송’ 등의 문구를 앞세워 소비자를 유인했다. 유명 쇼핑몰에서 대놓고 판매하기 때문에 소비자들은 불법 소프트웨어인지 알기 어렵다. 상품 문의 게시판에 정품인지를 묻는 글에 판매자는 정품이 맞다는 답변도 달았다. IT업계 관계자는 “상당수가 비영리 용도나 기업에서 대규모로 구입한 제품 등이 비정상적인 방법으로 유출된 것”이라며 “해당 제품키로 대부분 정품 인증이 가능하기에 판매자 또는 소비자도 불법인지 인지하기 어렵다”고 설명했다. 하지만 이런 방식의 판매는 명백히 불법이다. 지난 6월 한국 대법원은 유출된 제품키를 판매하는 행위는 저작권법 위반이라고 판결했다. 한국MS가 온라인 쇼핑몰업체에 협조공문을 보내는 등 불법 소프트웨어 유통 단속에 나선 것도 이 판결의 영향이 있다. MS 관계자는 “소비자가 사전에 불법을 인지한 것은 물론 의심하다가 제품을 구입했어도 저작권법 위반으로 처벌받을 수 있다”고 말했다. 불법 소프트웨어는 보안에 취약 최근 윈도10 수요가 증가하는 것도 단속의 한 배경이다. MS가 내년 1월부터 윈도7의 공식 기술 지원을 종료할 예정이어서 PC OS(운영체제)를 윈도10으로 업그레이드하려는 수요가 급증했다. 시장조사업체 스탯카운터에 따르면 지난달 기준 국내 PC에서 윈도7의 사용 점유율은 29%에 달한다. 윈도10에 대한 추가 수요가 아직 많다는 뜻이다. MS는 제품키로 구입한 소프트웨어의 안정성이 떨어진다고 설명했다. 제품키로 설치한 소프트웨어는 향후 업그레이드 서비스를 받는 데 한계가 있다. 지난해 MS가 한국 등 아시아 지역 9개 국가를 대상으로 조사한 결과 불법 소프트웨어가 설치된 PC의 84%에서 바이러스 등 멀웨어(악성 소프트웨어)가 발견됐다. 보안업계 관계자는 “불법 소프트웨어를 사용하면 PC 내 금융정보 등이 유출될 가능성이 크고 PC 성능도 떨어진다”고 설명했다. 그러나 한국에서는 정품 소프트웨어를 사용하려는 노력이 아직 부족하다는 지적이 나온다. 미국 비즈니스소프트웨어연합(BSA)은 ‘2018 글로벌 소프트웨어 조사 보고서’를 통해 한국 내 PC에 설치된 소프트웨어 중 32%를 불법으로 추정했다. 일본(16%)의 두 배 수준이다. 불법 이용에 따른 소프트웨어업계의 피해 규모는 5억9800달러(약 6055억원)에 달했다. IT업계 관계자는 “글로벌 IT 업체들이 소프트웨어 판매를 패키지 상품 방식에서 월정액제 방식으로 바꾸고 있는 것도 불법 소프트웨어 유통을 사전에 막으려는 전략”이라고 설명했다. ■ 제품키 product key. 소프트웨어를 설치할 때 사용자가 정품을 사용했다는 것을 인증하기 위해 입력해야 하는 문자 및 숫자로 구성된 고유의 번호. 보통 소프트웨어 패키지 상품에 밀봉된 형태로 제공된다. 온라인으로 불법 소프트웨어를 구입할 경우 판매업자가 제품키를 이메일 등으로 알려준다. 김주완 기자 kjwan@hankyung.com ▶ ▶ ▶ ⓒ 한국경제 &amp;amp; , 무단전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>조국 법무부 장관 후보자 페이스북 글에 지지·응원 글 넘쳐나는 이유</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>"힘내라" 조국 후보자 페이스북엔 응원만 가득 일부 언론 "지지 응원 쏟아진다" 보도 실체는 페친만 댓글 작성 가능 조국, 머리 쓸어넘기며 출근 (사진=연합뉴스) 조국 법무부장관 후보자가 국민들에게는 '용'이 될 생각말고 붕어 가재로 개천에서 행복하게 살라 해놓고 자신의 자녀는 '용'으로 만들어주기 위해 갖은 노력을 하고 있었다는 사실이 드러나면서 분노를 사고 있다. 논문 참여와 고려대 입학, 6차례의 몰빵 장학금, 부산대 의전원까지 구체적으로 드러난 불법사항은 없지만 문제는 조 후보자의 입이었다. 과거 조 후보자는 스스로를 강남 좌파라고 인정했으며 특목고, 특히 외고에 대해서 외국어 공부하러 갔으면 외국어 진로로 가도록 확실하게 규제라든지 이런 게 있어야 된다는 취지의 이야기를 한 적이 있다. 그런데 실체를 들춰보니 조 후보자의 딸은 외고를 나왔는데 딸은 의학전문대학원 다니고 있다. 개인과 정책적인 것은 다르다는 것을 감안해도 그야말로 '내로남불'의 전형적인 케이스로 스스로 당당하기는 조금 어려운 상황이 된 것이다. 아버지로서 철저하지 못하고 안이했다는 자아비판과는 달리 상상을 초월하는 스펙관리 끝에 조 후보자의 딸은 고대 환경생태공학부, 서울대 환경대학원을 거쳐 현재 부산대 의학전문대학원에 다니고 있다. 아들은 미국 조지워싱턴대를 졸업한 뒤 현재 연세대 대학원에서 정치외교학을 전공하고 있는 것으로 알려졌다. 정치적 신념이 확실했던 조 후보자는 국정농단 사태 당시 자신의 페이스북에 정유라의 입시특혜는 물론 논문과 장학금에 대해서도 쓴소리를 남겼으며 지금 고스란히 부메랑이 돼 조 후보자에게 돌아오고 있다. 조 후보자는 2010년 유명환 외교부 장관이 딸 특채 문제로 사퇴를 앞두고 있을 때 고위직이 잘못해서 사과를 하는 걸 파리를 예로 들어 비판했다. 파리가 앞발을 비빌 때는 먹을 준비를 하는 거라며 이때 잡아야 한다는 것이다. 다시 말해 고위직의 진정성 없는 사과를 봐주면 안 된다는 취지였다. 남의 잘못에는 서슬퍼런 비판을 쏟아내던 조 후보자는 자신을 둘러싼 많은 의혹에 연일 사과를 하면서도 청문회까지 심기일전해 맞설 것임을 확실히 했다. 조 후보자의 ‘정치무대’였던 페이스북은 청문회를 앞둔 지금 현재도 우회적으로 자신의 억울함을 항변하는 창구로 이용되고 있다. 자녀 고스펙 문제가 제기된 후 잠시 SNS 활동을 중단했던 조 후보자는 오늘 하루에만도 팩트브리핑이라는 주제의 부정입학 의혹이 거짓이란 게시물 등 10건 이상의 관련 링크를 올렸다. 대부분 자신을 둘러싼 의혹에 대해 긍정적으로 말하는 뉴스 등을 퍼나른 것이다. 이런 상황에서 26일 한 매체는 조 후보자의 페이스북에 오직 지지와 성원의 글이 넘쳐나고 있어 포털사이트의 댓글 분위기와는 전혀 다르다고 보도했다. 그렇다면 왜 이렇게 조 후보자의 행보에 대해 포털사이트와 페이스북 간의 간극이 큰 걸까. 일부 보도에서처럼 조 후보자 딸의 논문 및 입시 특혜 의혹 등은 모두 가짜뉴스기 때문에, 또는 진실된 사과로 인해 마음이 누그러진 국민들이 그를 지지하는 양상으로 바뀐 것일까. 조국 법무부장관 후보자 페이스북 응원글 조 후보자의 페이스북을 보면 바로 답이 나온다. 조 후보자의 페이스북에는 일반인이 댓글을 달거나 비난을 하고 싶어도 남길 수가 없다. 페이스북 자체가 게시물의 공개 대상을 전체공개, 친구 공개, 특정 친구 공개, 나만 보기 등으로 구분지을 수 있으며 조 후보자의 페이스북 또한 친구가 아닌 이상 댓글 쓰기가 불가능하기 때문이다. '조국 사퇴 촉구' 촛불 든 서울대생 (사진=연합뉴스) 네티즌들은 "철저히 기존 지인이나 같은 진영사람들 위주로 친구가 맺어져 있어서 악플달고 싶어도 달수가 없다", "친구들만 댓글을 다는데 당연한 것 아닌가. 비판을 할 수가 없지", "민심을 알고 싶다면 댓글 범위를 전체공개로 열어라", "페친만 댓글 쓸 수 있게 조 후보자가 막아놨다" 등의 반응을 보였다. 듣고싶은 말만 듣겠다고 결정한다면 그렇게 설정할 수 있는 것. 그게 SNS 주인장이 가진 권한이다. "원칙과 상식이 지켜지는 나라, 정의가 살아있는 사회를 위해 조국 후보자의 사퇴를 강력하게 촉구한다"는 서울대 후배들의 촛불집회, "가짜뉴스 만드는 기레기들에 휘둘리지말고 끝까지 힘내라. 응원한다"는 페친들의 댓글. 조 후보자를 바라보는 진정한 민심은 어느 지점에 위치하고 있는 것일까. 이미나 한경닷컴 기자 helper@hankyung.com ▶ ▶ ▶ ⓒ 한국경제 &amp;amp; , 무단전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>삼성 스마트폰, 日서 6년만에 최고 점유율...'갤럭시S10' 인기</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>[한국경제TV 이영호 기자] 삼성전자가 올해 2분기 갤럭시S10 시리즈 선전에 힘입어 일본 스마트폰 시장에서 6년 만에 가장 높은 점유율을 기록했다. 시장조사업체 스트래티지 애널리틱스(SA)에 따르면 삼성전자는 2분기 일본 스마트폰 시장에서 60만대를 출하해 점유율 9.8%를 기록했다. 애플(50.8%)에 이은 2위였다. 작년 동기 점유율이 애플 45.6%, 삼성전자 8.8%이었던 것과 비교해서 모두 소폭 올랐다. 애플과 삼성전자에 이어서는 샤프(7.2%), 소니(7.0%) 등 일본 기업이 3∼4위를 차지했다. 샤프는 작년 동기(5.1%) 대비 2.1%포인트 올랐고, 소니는 10.3%에서 3.3%포인트 줄었다. 중국 화웨이는 작년 동기 5.9%(4위)에서 올해 2분기 3.3%(5위)로 점유율이 절반 가까이 하락했다. 삼성전자가 10%에 육박한 점유율을 낸 것은 6년만에 최고치다. 삼성전자는 2013년 중반 일본 스마트폰 시장에서 10% 넘는 점유율을 유지하다 애플과 일본 브랜드에 밀려 2014년 5.6%, 2015년 4.3%, 2016년 3.4%로 점유율이 하락했다. 2017년부터 반등을 시작해 5.2%, 2018년 6.4%로 점유율이 오르는 추세다. 2분기 좋은 성적은 상반기 출시한 플래그십 모델 갤럭시S10 시리즈가 일본에서 인기를 끈 덕으로 보인다. 삼성전자는 지난 3월 전 세계 갤럭시 쇼케이스 가운데 최대 규모인 '갤럭시 하라주쿠'를 개관하면서 현지 스마트폰 시장 공략을 본격화했다. 5G 서비스가 처음으로 본격 적용되는 '2020 도쿄 올림픽'을 앞두고 일본 내 5G 네트워크 사업 확대를 위한 기반을 조성하는 동시에 갤럭시 스마트폰 시장점유율 반등의 계기를 마련한다는 전략이다. 삼성전자는 7월에는 2020 도쿄 올림픽을 기념해 갤럭시S10 플러스 올림픽 에디션을 일본에 출시했다. 이영호기자 hoya@wowtv.co.kr ▶ ▶ ⓒ 한국경제TV, 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>삼성디스플레이, QD-OLED 신공정에 국산 장비 도입 검토</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>삼성디스플레이가 차세대 대형 디스플레이 기술인 '퀀텀닷-유기발광다이오드(QD-OLED)' 투자를 앞두고 해외 기업이 독점한 핵심 전공정 공급망을 이원화하기 위해 고심하고 있다. 일본 비중이 절대적인 증착기와 미국이 독점한 무기물 형성 박막봉지 공정에 모두 국내 장비사를 참여시키는 방안을 검토하고 있다. 투자를 공식 결정하고 파일럿 라인을 조성한 뒤 양산 투자로 이어질 때 실제 공급망에 어떤 변화가 있을지 업계 기대가 모아진다. 26일 업계에 따르면 삼성디스플레이는 QD-OLED 파일럿 라인 투자를 준비하면서 해외 장비사가 독점한 일부 장비 공급망에 국내 기업을 참여시키는 방안을 모색하고 있다. 우선 일본에 100% 의존하는 증착기는 국내 장비기업 야스와 물밑 협업이 오가고 있다. 최근 일본 정부의 수출 규제로 제품을 제 때 수급하지 못할 가능성이 거론되면서 야스와 협력 가능성이 부상했다. 기술 준비 과정에서 혹시 모를 일본발 리스크에 대비하려면 핵심 공정에서 공급망을 이원화하는 전략이 필요하기 때문이다. 야스는 LG디스플레이에 8세대 OLED 증착기를 납품하는 핵심 협력사이지만 삼성디스플레이와도 협력할 수 있는 가능성을 열게 됐다. 주 고객사인 LG디스플레이가 경쟁사라도 전향적으로 협업을 장려하는 방침을 세웠기 때문이다. 삼성디스플레이는 6세대 OLED 양산에 일본 캐논도키 증착기를 사용한다. 증착기 핵심인 소스 기술은 삼성이 자체 보유했지만 소스를 제외한 증착기는 캐논도키에서 들여왔다. 캐논도키는 세계 중소형 OLED 증착기 시장에서 입지가 독보적이다. 삼성디스플레이는 6세대에 이어 8세대에서도 캐논도키와 협력하고 있다. QD-OLED에 적합한 증착기를 확보하기 위해 캐논도키에 개발을 의뢰했고 일본 현지에서 기술개발과 시제품 장비 제작이 이뤄지고 있다고 파악된다. LG디스플레이는 지난해부터 핵심 협력사를 대상으로 고객사 확대를 주문했다. 중국은 물론 주 경쟁사인 삼성디스플레이도 고객사로 확보해 매출을 다변화하고 규모의 경제를 실현해 생존 체력을 길러야 한다는 취지의 당부를 했다. 자사와 공동 개발했거나 민감한 세부 기술이 아니라면 굳이 제동을 걸 이유가 없다는 입장이다. LG디스플레이 관계자는 “디스플레이 업황이 어려워져 장비 회사가 고객사를 다변화해야만 생존할 수 있게 됐다”며 “LGD 협력사가 경쟁사에서 실력을 인정받고 우리도 기술력 있는 경쟁사 장비를 사용할 수 있어야 패널사와 장비기업 모두 윈윈하는 길”이라고 설명했다. 경쟁사의 핵심 협력사와 협업하는 것은 업계에서 암묵적으로 형성된 '협력사 교차 구매 금지'라는 높은 울타리를 깨는 것이어서 업계 관심이 크다. 최근 반도체와 디스플레이 시장에서 이 관행을 깨는 사례가 소수 생겨나고 있지만 아직 쉬쉬하는 경향이 크다. 유기물 봉지공정에서 무기막을 형성하는데 쓰이는 화학기상증착(CVD) 장비는 원익IPS가 진입할 가능성이 거론되고 있다. 이 공정은 미국 어플라이드머티어리얼즈가 독점한 분야다. 원익IPS는 반도체·디스플레이 공정에 쓰이는 다양한 기능의 CVD 장비를 공급하는 회사다. 유독 디스플레이 봉지공정에서 어플라이드 장벽을 넘지 못했다. 봉지는 유기물을 수분·공기와 닿지 못하게 얇은 막을 여러번 형성해 씌우는 공정이다. 플렉시블 OLED는 기판이 딱딱한 유리가 아닌 유연한 필름 소재를 사용하므로 봉지공정이 더 까다로워진다. 자칫 봉지막이 손상되면 패널 전체 성능에 악영향을 미치므로 상당한 수준의 기술이 요구된다. 어플라이드가 이 분야에서 강력한 기술 입지를 확보한 만큼 새로운 공급사가 진입하는게 쉽지 않았다. 업계 한 관계자는 “발주사인 삼성디스플레이도 어플라이드 눈치를 볼 수밖에 없을 정도로 공급망 다변화가 민감한 공정”이라며 “원익IPS가 아직 요구 성능을 완전히 충족하진 못했지만 양산 투자 시 진입을 목표로 기술개발에 공을 들이고 있다”고 전했다. 배옥진 디스플레이 전문기자 withok@etnews.com [Copyright ⓒ 전자신문 &amp;amp; 전자신문인터넷, 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>삼성, '애플천하' 日 점유율 10%…2013년 이후 최고</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2분기 일본 스마트폰 시장에서 60만대 판매 애플 50%로 압도적 1위지만 현지 업체 모두 제쳐 단 한일 갈등 본격화하기 직전 성적 일본서 아직 출시되지 않은 갤노트10 불매 목소리도 [아시아경제 임온유 기자] 삼성전자가 '애플 천하' 일본 스마트폰 시장에서 갤럭시S10 흥행에 힘입어 6년 만에 가장 높은 점유율을 기록했다. 단 한·일 갈등이 본격화하기 직전인 2분기 성적표다. 26일 시장조사업체 스트래티지 애널리틱스(SA)에 따르면 삼성전자는 지난 2분기 일본에서 스마트폰 60만대를 판매해 점유율 9.8%로 2위에 올랐다. 삼성전자가 10%에 육박하는 점유율을 기록한 것은 2013년 이후 처음이다. 삼성전자는 2013년 일본 스마트폰 시장에서 10% 넘는 점유율을 유지하다 애플과 일본 브랜드에 밀려 2014년 5.6%, 2015년 4.3%, 2016년 3.4%의 점유율로 하락했다. 2017년부터 반등을 시작해 5.2%, 2018년 6.4%로 점유율이 오르는 추세다. 삼성전자의 2분기 우수한 성적표는 갤럭시S10과 중가폰 흥행에 힘입은 것으로 분석된다. 삼성전자는 지난 3월 전 세계 갤럭시 쇼케이스 가운데 최대 규모인 '갤럭시 하라주쿠'를 개관하고 일본 스마트폰 시장 공략을 본격화했다. 5G 서비스가 처음으로 본격 적용되는 '2020 도쿄 올림픽'을 앞두고 일본 내 5G 네트워크 사업 확대를 위한 기반을 조성하는 동시에 스마트폰 시장에서 반전을 일궈낸다는 전략이다. 지난달에는 일본에서 2020 도쿄 올림픽을 기념해 갤럭시S10 플러스 올림픽 에디션을 출시하기도 했다. 다만 2분기는 한·일 갈등이 본격화하기 직전의 시기다. 지난달 아베 신조 일본 총리가 한국에 대한 경제 보복을 시작하면서 양국 관계는 악화일로를 걷고 있다. 한국에서 유니클로, ABC마트 등 일본 브랜드 불매 운동이 격렬하게 벌어지는 가운데 일본에서도 삼성전자를 비롯한 한국 브랜드 불매 운동이 벌어지고 있다. 야후재팬 등 대표 포털 사이트에서는 아직 일본에서 출시되지 않은 갤럭시노트10을 사지 말아야 한다는 목소리까지 나오는 추세다. 이에 3분기 삼성전자의 일본 내 점유율이 변화할 가능성이 제기된다. 임온유 기자 ioy@asiae.co.kr &amp;lt;ⓒ경제를 보는 눈, 세계를 보는 창 아시아경제 무단전재 배포금지&amp;gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>티슈진, 상장폐지 결정...인보사사태 장기전 돌입</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>거래소 "인보사 성분 허위 기재에 품목 취소" 인정 티슈진 이의신청땐 한차례 더 심의...사실상 3심제 이달중 FDA에 임상 재개 위한 서류제출 총력전 [서울경제] 성분이 뒤바뀐 유전자 치료제 ‘인보사케이주(이하 인보사)’ 사태로 최대 위기에 내몰린 코오롱티슈진이 결국 한국거래소로부터 상장폐지 통보를 받았다. 하지만 최종 상장폐지까지는 최대 2년 이상이 소요되는 만큼 인보사 사태는 사실상 장기전에 돌입했다는 분석이 업계에서 나온다. 이 기간 코오롱 측은 미국 임상3상 재개를 위해 총력전을 펼칠 것으로 전망된다. 한국거래소 코스닥시장본부는 26일 기업심사위원회 심의 결과 코오롱티슈진의 주권 상장폐지를 결정했다고 공시했다. 거래소는 이후 15영업일 이내에 코스닥시장위원회를 열어 코오롱티슈진의 상장폐지 여부를 재차 심의·의결하게 된다. 코오롱티슈진이 예상대로 상장 폐지의 수순을 걷게 됐음에도 인보사 사태가 장기화될 것이라는 전망은 최종 결정까지는 2년이 소요되는 데다 이 기간 동안 코오롱측이 마지막 카드로 내세우는 미국 임상 3상 재개와 식약처와 벌이게 될 품목허가 취소 행정소송에 총력적을 펼칠 수 있기 때문이다. 앞서 인보사는 지난 2017년 1액(동종유래 연골세포)과 2액(TGF-β1 유전자삽입 동종유래 연골세포)으로 시판허가를 받았지만 2액의 성분이 알려진 것과 다르다는 사실이 밝혀져 올 7월 식품의약품안전처로부터 최종 품목허가 취소 처분을 받았다. 이에 거래소는 지난달 5일 티슈진 측이 제출한 서류의 내용 중 중요한 사항이 허위기재 또는 누락됐는지를 살펴보기 위해 상장적격성 실질심사 대상으로 정했다. 티슈진은 5월28일부터 주권매매거래가 정지된 상태다. 업계에서는 티슈진이 기술특례상장 형태가 아닌 외국기업으로 상장한 만큼 상장폐지가 불가피했을 것으로 판단하고 있다. 현행 코스닥 상장규정상 4년 연속 영업적자를 기록하면 ‘장기영업손실’ 규정에 따라 관리종목으로 지정된다. 이후 1년 더 영업적자가 나면 상장폐지 실질심사대상이 된다. 기술심사 특례요건으로 상장하면 5년간 장기영업손실 규정 적용이 면제되지만, 티슈진은 해외기업으로 기술심사 특례요건에 해당하지 않았다. 티슈진은 지난 2017년 454억원, 2018년 340억원의 영업적자를 기록했고, 지난 1분기 역시 114억원 영업적자가 났다. 인보사의 판매 혹은 수출 금액의 2%를 매출로 받게 되는 구조상 티슈진이 올해와 내년 매출을 올릴 수 있는 방법은 사실상 전무하다. 거래소가 기심위 심사결과 티슈진이 상장폐지에 해당한다고 판정한 만큼 코오롱은 최악의 시나리오에 직면했다. 이는 거래소가 티슈진이 성분 변경 등 중요사항을 허위로 기재했다는 식약처의 품목허가 취소 처분을 인정했다는 의미다. 물론 거래소가 이번에 상장폐지라고 결론을 내린다고 해도 곧장 상장폐지가 확정되는 것은 아니다. 다시 코스닥시장위원회를 열어 티슈진의 상장폐지 여부를 심의·의결해야 하기 때문이다. 또 코스닥시장위원회에서 상장폐지 결정이 나더라도 티슈진 측이 이의신청을 하면 한 차례 더 심의를 벌이게 된다. 사실상 3심제를 적용하는 만큼 최종적으로 상장폐지가 결정되기까지는 최대 2년 이상의 시간이 소요될 것으로 전망된다. 티슈진 관계자는 “코스닥시장위 결정 이후 회사 측에서 이의신청을 하면 한 차례 더 심의를 하는 것으로 알고 있다”고 말했다. 코오롱 측은 거래소의 상장폐지 결과에도 마지막 남은 카드인 미국 임상3상 재개에 사활을 걸 것으로 보인다. 인보사의 미국 임상3상 재개 여부가 티슈진의 명운을 가를 핵심변수이기 때문이다. 만약 미국에서 임상이 재개된다면 거래소가 상장폐지를 결정하더라도 추후 심사에 긍정적인 영향을 미칠 수 있다는 판단에서다. 티슈진에 따르면 회사는 이달 중 미국 식품의약국(FDA)에 인보사의 임상3상 재개를 위한 서류를 제출할 예정이다. 티슈진 관계자는 “최대한 이른 시일 내에 서류를 제출할 계획”이라며 “이달 안에 FDA에 서류를 낼 것”이라고 말했다. 다음 문제는 자금력이다. 업계에서는 미국 FDA가 설사 임상 재개를 승인하더라도 코오롱 측이 받게 될 자금 부담은 상당할 것이라는 관측이 나온다. 코오롱 측은 티슈진으로 유입되는 자금으로 미 임상을 진행하기 위해 2017년 11월 티슈진을 코스닥에 상장했다. 지난해 11월부터 시작됐다. 현재 중단된 1,000명 규모의 미 임상3상에서 실제로 인보사를 투여한 환자는 10명가량으로 알려졌다. 통상 임상 과정에서 대상자 1인당 1억원이 소요되는 것을 고려하면 코오롱 측은 상장폐지 심사 기간에 1,000억원 이상의 자금을 별도로 마련해야 한다. 금융감독원에 따르면 티슈진의 누적 손실액은 2016년 645억원이었다가 2017년 인보사의 개발비용이 늘면서 1,116억원으로 두 배 가까이 껑충 뛴 후 지난해 말 1,492억원까지 증가했다. 아울러 진행 중인 검찰 수사와 행정소송 결과도 변수가 될 수 있다. 앞서 서울행정법원은 13일 코오롱생명과학이 식약처를 상대로 낸 인보사의 허가취소 처분 집행정치 가처분 신청을 기각한 바 있다. 검찰은 코오롱 측이 성분이 바뀐 것을 알고도 인보사를 판매하고 티슈진을 상장한 의혹 등을 조사하기 위해 코오롱 본사 등에 대해 압수수색을 벌였지만 아직 수사 결과는 나오지 않았다. 업계 관계자는 “티슈진은 한때 시가총액이 4조원까지 갔던 제약바이오주의 상징과도 같은 종목이었다”며 “거래소가 어떤 심사 결과를 내놓더라도 코오롱 측은 인보사의 임상3상 재개를 위해 사력을 다할 수밖에 없을 것”이라고 말했다. /박홍용기자 prodigy@sedaily.com | 저작권자 ⓒ 서울경제, 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>7월 일본여행 얼마나 안 갔나···"로밍 신청 5만명 급감"</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>통신3사 일본 로밍 이용자 수 따져봤더니 인천국제공항 제1여객터미널 일본행 탑승수속 카운터가 한산한 모습을 보이는 반면 동남아행 탑승수속 카운터는 붐비고 있다./영종도=오승현기자 [서울경제] 지난 7월 일본의 수출 규제 이후 일본 제품 불매 운동이 국내에서 퍼지는 가운데, ‘일본 여행객이 얼마나 줄었나’에 대해서도 사람들의 관심이 많다. 지난달 통신 3사의 일본 로밍 신청자 수를 따져 봤더니 작년 같은 기간보다 14.5%(5만 1,231명) 감소한 것으로 집계됐다. 26일 국회 과학기술정보방송통신위원회 노웅래 위원장(더불어민주당)이 과학기술정보통신부로부터 제출받은 자료에 따르면 지난달 통신 3사의 일본 로밍 신청자는 30만1,285명으로 작년 같은 기간 35만2,516명보다 14.5%(5만1,231명) 줄었다. 이는 전달 일본 로밍 이용자 수(33만2,251명)에 비해서도 7.9%(2만8,422명) 적은 수치다. ‘일본 여행 안 가요’ 운동 여파로 7월 일본 휴대전화 로밍 이용자가 급감한 것으로 풀이된다. 1~7월 일본 로밍 이용자 수도 231만279명으로 작년 같은 기간보다 11.6%(30만3,860명) 줄었다. 지난달 일본 로밍 이용자 수 감소율은 일본을 방문한 한국인 여행자 수 감소율( 7.6%)의 1.91배다. 불매 운동의 여파로 일본 여행자 수가 양적으로 줄었을 뿐만 아니라 방문 기간이 단축되는 등 질적인 차원에서도 변화가 이뤄지고 있다는 해석도 나온다. 노웅래 위원장은 “일본 경제침략에 대응하는 국민적 차원의 자발적 불매운동이 지속되고 있다”며 “과거와는 분명히 다른 양상으로 장기화할 가능성이 크다고 본다”고 말했다. 고노 일본 외무상 / 연합뉴스 /강신우기자 seen@sedaily.com | 저작권자 ⓒ 서울경제, 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>화성서 발견된 돌 ‘롤링스톤스’로 명명…아이언맨·믹 재거 감격</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>[서울신문 나우뉴스] 화성서 발견된 돌과 롤링스톤스 무대에 올라 연설 중인 로버트 다우니 주니어. 사진=AP 연합뉴스 골프공보다 약간 큰 화성의 돌에 전설적인 록그룹 롤링스톤스(The Rolling Stones)의 이름을 따 '롤링스톤스'(Rolling Stones Rock)라는 재미있는 이름이 붙었다. 특히 롤링스톤스라는 이름을 명명하는 이벤트를 '아이언맨' 로버트 다우니 주니어가 맡아 큰 화제가 됐다. 공연 중인 롤링스톤스. 사진=AP 연합뉴스 지난 23일(현지시간) AP통신 등 외신은 전날인 22일 캘리포니아주 패서디나 로즈볼 스타디움에서 열린 롤링스톤스의 특별공연에서 롤링스톤스 명명식이 열렸다고 보도했다. 이 돌은 지난해 화성 탐사선 인사이트에 의해 처음 발견된 화성의 암석이다. 흥미로운 점은 인사이트의 자체 추진력 때문에 약 1m 정도 굴러갔다는 점. 이같은 이유로 말 그대로 화성의 돌은 롤링스톤이 됐다. 로버트 다우니 주니어와 인사이트 미션 담당 과학자들 이날 특별공연 무대에 등장한 다우니 주니어는 "과학과 전설적인 록밴드의 만남은 항상 좋은 일"이라면서 "이 이름을 공식화하는 데 이미 6만 명이나 찬성 투표했다”며 너스레를 떨었다. 롤링스톤스 명명에 가장 감격한 사람은 역시 리더 믹 재거(76)였다. 그는 "이번 투어를 축하하는 가장 멋진 방법"이라면서 "이는 우리 밴드의 길고 파란만장한 역사에서도 획기적인 사건으로 미 항공우주국(NASA)의 모든 분들께 감사드린다"며 기뻐했다. NASA 제트추진연구소 지질학자 맷 골롬벡은 “그간 수많은 다른 행성의 암석을 봐왔지만, 이번에 명명된 암석은 어떤 과학 논문에도 존재하지 않는 특별하고 가장 차가운 암석”이라며 의미를 부여했다.　　 지난해 12월 공개된 인사이트의 첫번째 셀카. 사진=NASA/JPL-Caltech 한편 지난해 11월 26일 화성 적도 인근 엘리시움 평원(Elysium Planitia)에 무사히 착륙해 탐사를 이어가고 있는 인사이트는 기존 화성 탐사로봇과는 다르다. 이제까지의 탐사로봇들이 주로 화성 지표면에서 생명의 흔적을 찾는 임무를 수행했다면 인사이트는 ‘땅파기’를 통해 화성 내부를 들여다보기 때문이다. 특히 지난 4월 인사이트는 화성 지진(marsquake)일 가능성이 높은 희미한 진동을 처음으로 포착하는데 성공했다. 박종익 기자 pji@seoul.co.kr ★ ▶ ⓒ 서울신문(www.seoul.co.kr), 무단전재 및 재배포금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>제주도·남부는 ‘가을장마’…최고 300mm 비</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>[앵커] 중부지방은 오늘도 30도 안팎의 늦더위가 계속됐는데요. 제주도와 남부지방은 '가을장마'에 들어가면서 모레까지 최고 300mm의 많은 비가 예보됐습니다. 신방실 기상전문기자가 보도합니다. [리포트] 오늘 새벽, 세찬 빗줄기 속에 호우주의보까지 내려졌던 제주도. 낮 동안 주춤했던 비는 다시 굵어지면서 남해안으로 확대되겠습니다. 내일은 남부 내륙과 충청 남부에도 비가 오겠고 모레까지 제주도에 최고 300 이상, 전남 남해안에도 많게는 100mm의 비가 예보됐습니다. 장마철이 지났는데도 남부에 비가 이어지는 것은 '가을장마', 즉 '2차 장마' 때문입니다. 위성영상을 보면 우리나라 남해상에 동서로 발달한 거대한 구름대가 보입니다. 북서쪽 찬 공기와 남쪽 더운 공기 사이에 또다시 정체전선이 만들어진 건데, 어제 중국에서 소멸한 11호 태풍에서 수증기까지 더해져 비구름의 세력이 강해지고 있습니다. [우진규/기상청 예보분석관 : "앞으로 이 정체전선에 동반된 비구름대는 점차 북상하면서 모레까지 제주도와 남해안을 중심으로 시간당 30mm 이상의 매우 강한 비가 내릴 것으로 예상됩니다."] 여름에서 가을로 계절이 바뀌는 지금 시기엔 찬 공기와 더운 공기의 충돌이 더 강해져 폭이 좁은 비구름이 폭발적으로 발달할 수 있습니다. 제주와 남해안을 중심으로 목요일까지 많은 비가 예보된 만큼 막바지 폭우 피해가 없도록 철저한 대비가 필요합니다. 가을장마를 불러온 정체전선은 다음달 초까지 제주도와 남부지방에 비를 뿌리겠다고 기상청은 내다봤습니다. KBS 뉴스 신방실입니다. 신방실 기자 (weezer@kbs.co.kr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>“공인인증서 폐지..29일, 전자서명 신기술 한자리에”</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>과기정통부, 최신 전자서명 우수사례 설명회 개최 금결원(브라우저), 카카오(페이연동), SKT·아이콘루프(블록체인) 등 다양 [이데일리 김현아 기자] ▲행사 참여 신기술 전자서명 서비스 소개(출처: 과기정통부) 과학기술정보통신부(장관 유영민)가 ‘신기술 전자서명 우수사례 설명회’를 29일 오후 2시, 서울 여의도 켄싱턴호텔에서 개최한다. 이 설명회는 정부의 공인인증서 제도 폐지 방침에 따라 현재 적용 중이거나 적용 예정인 다양한 신기술 전자서명 서비스를 일반 국민과 공공·민간기관 관계자에게 소개해 관련 산업을 활성화하기 위해 마련됐다. 생체인증, 블록체인, 클라우드 등 신기술을 활용한 자사의 최신 전자서명서비스의 특장점을 소개할 예정이다. 금융결제원, 카카오, 한국전자인증, 예티소프트, 아톤, 한국정보인증, 위즈베라, SKT, 시큐브, 라온시큐어, 코스콤, 아이콘루프 등 12개 사업자가 참여한다. 주요 발표 내용으로는 △ 금융결제원의 브라우저 및 클라우드 인증서비스와 △ 모바일 메신저 카카오톡 기반의 카카오페이 인증서비스, △ 한국전자인증의 클라우드 전자서명과 브라우저 전자서명, △ 예티소프트의 웹표준(HTML5) 방식 간편인증 및 간편서명 솔루션 등이 있다. 또 △ 국내은행에 적용 중인 아톤의 간편 전자서명 솔루션 △ 블록체인 기술을 적용한 한국정보인증의 온라인 전자계약서비스, △ 의료분야에 적용 예정인 위즈베라의 간편 전자서명서비스, △ SK텔레콤의 블록체인 기술을 활용한 자기주권형 모바일 전자증명서비스가 소개된다. 아울러 △ 시큐브의 생체 수기서명 인증 기반 전자서명, △ 병무청 민원포털에 적용 예정인 라온시큐어의 블록체인 기반 전자서명 △ 코스콤의 공인·사설 통합인증서비스, △ 아이콘루프의 블록체인 기반 디지털 신원확인·전자서명서비스 등 다양한 기술·서비스를 발표하고, 현장에서 직접 체험할 수 있는 부스를 운영할 예정이다. 과기정통부 오용수 정보보호정책관은 “이번 설명회에서 소개되는 다양하고 편리한 전자서명서비스가 국민들에게 많이 알려지고 시장에 확산될 수 있도록 국회 계류 중인 전자서명법 전부개정안의 조속한 통과를 기대한다”면서 “그렇게 되면, 전자서명시장에 기술·서비스 경쟁이 보다 활성화되어 국민들에게 다양한 인증수단 선택권을 제공하는 등 인터넷 이용환경이 크게 개선될 것으로 전망된다”라고 밝혔다. □ 개 요 o (목적) 정부의 전자서명제도 개편방향에 따른 시장의 다양한 신기술 전자서명서비스 우수사례에 대한 대국민 홍보의 장 마련 o (일시·장소) ’19.8.29(목) 14:00~17:30, 여의도 켄싱턴호텔(15층, 180석 규모) o (행사내용) 신기술 전자서명 우수사례(적용예정 포함) 소개 및 시연 o (주최·주관) 과학기술정보통신부·한국인터넷진흥원(후원:한국전자서명포럼) o (참석자) 전자서명 관련 업계, 공공·민간 수요기관, 언론 등 김현아 (chaos@edaily.co.kr) 네이버 홈에서 ‘이데일리’ 뉴스 꿀잼가득 , 청춘뉘우스~ ＜ⓒ종합 경제정보 미디어 이데일리 - 무단전재 &amp;amp; 재배포 금지＞</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>“S와 다른 새 노트”…삼성 고민 묻어 나오는 갤노트10</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>갤럭시노트10 써보니 갤럭시노트10(왼쪽)은 화면을 둘러싼 테두리 두께를 최소화해 갤럭시노트8과 동일한 크기의 디스플레이를 유지하면서도 전체 크기가 훨씬 작아졌다. 맹하경 기자 ‘노트 맞아?’ 지난 23일 국내에 정식 출시된 삼성전자 ‘갤럭시노트10’(일반형ㆍ화면 6.3인치)을 손에 들었을 때 첫 느낌이다. 갤럭시노트 시리즈는 삼성의 프리미엄 대화면 제품군임에도 노트10은 유독 가볍고, 얇았다. 손이 작은 여성도 한 손에 쏙 쥘 수 있어 노트보다 작은 화면의 갤럭시S 시리즈 못지 않은 느낌을 줬다. 동시에 노트에만 있는 S펜은 카메라 등을 원격으로 조종하는 기능을 강화했다. S펜으로 기존 갤럭시S와의 차별점을 부각하면서도 기존 갤럭시노트에선 찾기 힘들었던 얇고 가벼운 디자인에는 전작들과는 다른, 새로운 스마트폰을 보여주려 했던 삼성의 고민이 담겨 있었다. 이번 갤럭시노트10 디자인을 표현하는 한 단어로는 ‘미니멀리즘’이 어울렸다. 디스플레이를 둘러싼 테두리(베젤)를 최소화했고 이어폰을 꽂는 단자도 없앴으며, 본체 오른쪽에 있던 전원 버튼도 왼쪽으로 옮겨 우측에는 버튼을 한 개도 남기지 않았다. 갤럭시노트10 디자인을 총괄한 강윤제 삼성전자 무선사업부 디자인팀장(전무)은 “‘갤럭시노트9’, ‘갤럭시S10’과도 차별화할 수 있도록 불필요한 부분은 극단적으로 다 없앴다”고 밝힌 바 있다. 갤럭시노트10(아래) 해상도가 갤럭시노트8(위)보다 낮아 같은 밝기에도 전체적으로 어둡고 명암 차이도 잘 드러나지 않는다는 것을 알 수 있다. 맹하경 기자 베젤을 최대한 줄인 덕분에 본체 전체 크기는 ‘갤럭시노트8’(6.3인치)보다 훨씬 작아졌지만 꽉 찬 6.3인치 화면은 그대로 유지할 수 있었다. 무게는 168g에 불과해 노트8(195g), 노트9(201gㆍ6.4인치)보다 훨씬 가벼웠다. 다만, 해상도는 많이 아쉬웠다. 중저가 제품군인 ‘갤럭시S10e’와 같은 2,280×1,080 해상도 때문에 기존 노트보다 전체적으로 어둡고 명암이 제대로 구분되지 않았다. 노트10의 S펜은 앞으로 원격 조종 기능이 더 다양해질 수 있다는 가능성을 보여주는 수준이었다. S펜을 쥐고 움직이는 동작을 카메라가 인식해 전ㆍ후면 카메라 전환, 카메라 모드 변경, 줌인ㆍ줌아웃 등이 가능했다. 하지만 손가락 터치 한번이면 되는 일을 S펜을 쥐고, 버튼을 누르고, 동작을 하는 세 단계까지 늘려야 하기 때문에 카메라를 멀리 두고 찍어야 하는 등 특수한 상황이 아니라면 사용성은 제한될 것으로 보인다. 갤럭시노트10의 'AR 두들' 기능으로 사물을 찍고 있는 화면 위에 이미지를 덧입히면 이미지가 해당 사물을 인식해 따라다니는 콘텐츠를 만들 수 있다. 맹하경 기자 S펜을 활용하는 새 기능이자 노트10의 주요 고객층을 알 수 있는 건 단연 ‘AR(증강현실) 두들’이었다. AR 두들은 카메라를 켠 채로 영상이나 사진을 찍으면서 S펜으로 자유롭게 이미지를 덧입힐 수 있는 기능이다. 사람의 얼굴이나 공간을 인식하기 때문에 덧입힌 이미지가 인식한 사람 얼굴, 사물을 쫓아다니게 된다. 나만의 사진, 영상 콘텐츠를 소통의 수단으로 활용하는 밀레니얼 세대를 공략하려는 전략임을 알 수 있다. 기존 갤럭시노트 시리즈 주 사용자가 남성 중·장년층 고객들이었다면 이번 제품에선 밀레니얼 세대와 여성 고객들까지 포섭하려 한다는 게 업계의 분석이다. 이동통신 3사 중 유일하게 붉은 색상을 단독 판매하며 일반형 판매에 주력 중인 KT 측은 “일반형 예약 구매자 중 절반이 여성으로 기존 노트 시리즈 여성 사용자 평균인 40%를 훌쩍 넘겼고, 노트9 때보다 20대 구매자 비중도 25% 이상 늘었다”고 밝혔다. 맹하경 기자 hkm07@hankookilbo.com ▶</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>중국 디디추싱, '한국행' 준비 중</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>중국 모빌리티 기업 디디추싱이 한국 진출을 검토하고 있다. 8월26일 업계에 따르면 디디추싱은 올해 초부터 국내 업체들을 만나 한국내 모빌리티 사업을 논의해왔다. 국내 규제 상황에 따라 이르면 내년 상반기 본격적으로 한국 시장에 뛰어들 가능성도 있는 것으로 알려졌다. 디디추싱은 ‘카카오택시’처럼 택시호출을 중개하는 방식으로 국내 진출을 검토하고 있다. 브이씨엔씨(VCNC) ‘타다 베이직’처럼 자체 서비스를 하는 것이 아니라, 한국의 기존 택시산업을 최대한 활용한다는 방침이다. 구체적인 운영 형태는 정해지지 않았다. 국내 모빌리티 시장은 초기 단계다. 여물지 않은 시장임에도 디디추싱이 한국행을 고려한 이유는 폭넓은 시장을 확보하기 위해서다. 2012년 중국에서 설립된 디디추싱은 중국 시장 점유율 90%를 확보하고 있다. 이용자 수만 4억명 이상. 미국 시장조사업체 CB인사이트에 따르면 기업가치는 560억달러(약 67조원)에 달한다. 전세계 1천개 도시에 진출하며 중국 바깥으로 영향력을 빠르게 확대해가고 있다. 디디추싱이 한국에 진출하는 또 다른 유인은 중국인 관광객이다. 한국관광공사에 따르면 한국을 찾는 외국인 관광객의 국적은 중국이 압도적이다. 지난달 한국을 방문한 중국인 관광객만 51만9132명에 이른다. 디디추싱과 접촉한 투자전문업체 관계자는 “한국에서 수익성을 보고 있다거나 큰 이점이 있어 진출하려는 것은 아니다”라면서도 “중국인 여행객이 제일 많은 시장이고, 중국인도 한국에 와서 디디를 찾기 때문에 수요는 있다”라고 귀띔했다. 이에 따르면 국내 진출 초반 중국인 관광객을 대상으로 수요를 확보하고 이후 국내 승객을 단계적으로 공략하는 전략을 취할 가능성이 있어 보인다. 다만 디디추싱은 규제의 불확실성을 우려하고 있다. 올해 초만 해도 연내 한국 진출을 염두에 뒀지만, 택시산업과 모빌리티 업계 갈등을 지켜보며 한 발 물러선 상태다. 내년 상반기로 진출 시기를 미룬 이유도 이 때문이다. 국토부가 지난달 발표한 ‘택시제도 개편방안’이 구체화되기 전까지는 신중을 기할 전망이다. 투자전문업체 관계자는 “사실 디디추싱은 한국 시장 자체가 작기도 하고, 굳이 이 시점에 들어와야 하는지 망설이고 있다”라며 “초반에는 활발하게 논의했지만 (내부적으로) 검토하다 보니 굳이 빨리 (진출)해야 하느냐는 의문이 있는 것”이라고 말했다. [새소식] 기사 내용과 관련해 디디추싱 측 입장을 다음과 같이 덧붙입니다. 디디추싱 대변인은 이메일을 통해 &amp;lt;블로터&amp;gt;에 "일련의 보도는 정확하지 않은 것으로, 한국에는 (진출) 의도가 없다"라는 입장을 밝혔다. Thank you for getting in touch. Those media reports are inaccurate. DiDi has no such intention in Korea. Please attribute this to DiDi or DiDi spokesperson. - 업데이트 2019년 8월26일 오후 7시15분 김인경 기자(shippo@bloter.net) ▶ ▶ 저작권자 ⓒ(주)블로터앤미디어, 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>"군 병사 월평균 데이터 38GB 사용"..일반인보다 4배 많아</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>군장병 요금제 사실상 무제한 데이터이기 때문 와이파이 없는 군대 환경도 영향 일반인 LTE는 월평균 9.6GB 사용 고립감 줄었지만 일탈 행위도..방통위·국방부 윤리교육 SKT ‘0히어로’ 12만 돌파, 군 병사 가입자 수 1위 [이데일리 김현아 기자] SK텔레콤 홍보모델들이 ‘0히어로’ 흥행 기념으로 이벤트 당첨자들에게 제공할 푸드트럭과 각종 선물을 소개하고 있는 모습이다 SK텔레콤 제공 올해 4월부터 스마트폰 사용이 전 군 장병 대상으로 확대되면서 이동통신사와 알뜰폰 회사들이 군 병사를 대상으로 하는 LTE 요금제를 잇따라 출시했다. 병사들도 평일 오후 6시에서 10시, 휴일은 아침 7시부터 밤 10시까지 부대 안에서 보안 취약 구역을 제외하고는 스마트폰을 쓸 수 있게 된 것이다. 군인들은 한 달에 데이터를 얼마나 쓸까. 언뜻 보기에는 일반인들보다 적게 쓸 것 같지만 결과는 달랐다. ◇군인 월평균 38GB, 일반인은 9.6GB..데이터 혜택, 와이파이가 없기 때문 지난 4월 군 병사 전용 요금제 ‘0히어로’를 출시한 SK텔레콤에 따르면 군 병사들의 월평균 데이터 사용량은 38GB나 됐다. 이는 과학기술정보통신부의 2019년 6월 무선데이터 트래픽 통계기준상 LTE 일반인 평균 사용량(9.6GB)의 4배에 달하는 수치다. 이는 통신사들이 내놓은 군인 대상 요금제가 사실상 무제한에 가까운 데이터 혜택을 주기 때문으로 보인다. 군대에는 와이파이가없어 이를 고려해야 한다는 평가도 있다. 현재 가입자 12만 명을 모아 군 병사 요금제 중 1위를 기록한 ‘0히어로’만 봐도 일반 요금제보다 데이터 혜택이 풍성하다. ‘0플랜 히어로(월33,000원)’는 기본 제공량 6GB(+1Mbps 속도제어) 이외에도 평일 18~22시와 휴일에 매일 2GB(+3Mbps 속도제어)를 무료로 제공하며, ‘0플랜 슈퍼히어로(월55,000원)’는 기본 제공량 100GB(+5Mbps 속도제어)와 VIP 멤버십 등급 등의 추가 혜택을 준다. 월 3만 원 대 요금제에 가입해도 군인들이 많이 쓰는 평일 저녁이나 휴일에 2GB씩 무료로 주니 병사들의 데이터 사용량이 큰 폭으로 증가한 것이다. 이는 다른 이통사들도 마찬가지다. 실제로 병사들은 일과가 끝난 평일 18~22시와 휴일에 집중적으로 스마트폰을 이용하고 있으며, 특히 평일보다 휴일에 데이터 사용량이 많았다. ‘0플랜 히어로’에 가입한 군 병사들의 일평균 데이터 사용량은 평일 18~22시 0.65GB, 휴일 1.77GB를 기록했다. ◇고립감 줄었지만 일탈 행위도..방통위·국방부 윤리교육 일각에선 우려의 시선도 있다. 군인들이 너무 많이 스마트폰을 보지 않을까 하는 우려다. 군인들도 개인 여가는 필요하고 고립감이 줄어 군 생활에 도움이 되기도 하지만, 휴대전화를 이용해 불법도박을 하는 등 일탈 행위도 발견되고 있다. 이에따라 국방부와 방송통신위원회는 군 장병 대상 인터넷 윤리교육을 진행하고 있다. 방송통신위원회와 국방부가 군 장병들에게 건전한 인터넷 윤리문화를 정착시키기 위해 5월 24일 국방부에서 업무협약(사진. 방통위)을 체결하고 인터넷 윤리 시범교육을 실시했다. 왼쪽부터 이효성 방송통신위원장과 정경두 국방부장관이다. 방통위 제공 ◇택시할인, 무료 쿠폰 등 인기..SKT 푸드트럭 이벤트 중 한편 SK텔레콤에 따르면 ‘0히어로’가 제공하고 있는 군 생활 맞춤 혜택도 꾸준히 인기다. 휴가, 외박 시에 유용한 T맵택시 10% 할인 혜택은 현재까지 6천명이 이용할 정도로 반응이 좋다. ‘0(영)한동’ 앱에서 제공하는 무료 쿠폰 이용자는 누적 3만명을 넘었다. SK텔레콤은 지난 7월 ‘0히어로’ 흥행 기념으로 군 생활 응원 메시지 모집 이벤트를 진행했으며, 이번 달부터 당첨자들을 직접 찾아가 푸드트럭과 POOQ/FLO 이용권 등 각종 선물을 제공하고 있다. 방문 이벤트는 9월까지 진행될 예정이다. 한명진 SK텔레콤 MNO사업지원그룹장은 “군 병사들의 통신 혜택을 강화하기 위해 넉넉한 데이터와 다양한 생활 맞춤 혜택을 제공했던 것이 흥행 요인”이라며 미래 고객인 군 병사들에게 더 좋은 혜택으로 보답할 것”이라고 강조했다. 김현아 (chaos@edaily.co.kr) 네이버 홈에서 ‘이데일리’ 뉴스 꿀잼가득 , 청춘뉘우스~ ＜ⓒ종합 경제정보 미디어 이데일리 - 무단전재 &amp;amp; 재배포 금지＞</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>[위클리 스마트] 갤노트10 기본·플러스 모델 뭐가 다를까 "실제 써보니…"</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>"화면 크기 외 사양 차이는 체감 적어"…KT 레드·SKT 블루 컬러 매력 (서울=연합뉴스) 채새롬 기자 = 23일 출시된 갤럭시노트10 기본 모델과 플러스 모델을 며칠간 사용해 본 느낌은 기존 팬층은 물론 그동안 노트 시리즈를 써보지 않은 사용자에게도 매력 어필이 되게끔 화면 크기가 잘 나뉘었다는 것이다. 갤럭시노트10(좌측)과 갤럭시노트10플러스[촬영 채새롬] 갤럭시노트10은 시리즈 처음으로 6.3인치 일반 모델과 6.8인치 플러스 모델로 나뉘어 나왔다. 플러스 모델이 기존 노트 팬층을 공략한 모델이라면 일반 모델은 컴팩트한 사이즈를 좋아하는 소비자를 노린 모델이다. 두 모델은 화면 크기 외에도 화면 해상도 차이, 저장 용량 옵션 차이, ToF 카메라 유무 등 스펙에서 차이 나지만, 실제 사용할 때 화면 크기 외에 특별히 느껴지는 사양 차이는 없었다. 램 용량(12GB)·칩셋이 같고, S펜 에어액션 등 신기능을 동일하게 이용할 수 있기 때문이다. 일단 일반 모델은 한 손에 쏙 들어오는 사이즈가 가장 큰 장점이다. 기존 갤럭시노트 시리즈는 크고 둔탁해 보여 '아저씨폰' 느낌이 강했는데 일반 모델은 손이 작은 기자도 휴대가 편리하고 가벼워 매력적이었다. 화면 크기가 6.3인치로 절대적인 크기도 작지 않다. 플러스 모델이 WQHD(2960×1440) 해상도를 지원하는 데 비해 일반 모델이 FHD+(2220×1080)를 지원한다는 스펙 차이가 존재하긴 하지만 '막 눈'인 기자에겐 차이를 느끼지 못하는 수준이었다. 아이패드 미니5(위쪽)와 갤럭시노트10플러스로 재생한 동영상[촬영 채새롬] 일반 모델과 구별되는 플러스의 장점 역시 화면 크기다. 노트 필기를 좋아하는 사용자라면 더 넓은 화면을 자유롭게 쓸 수 있는 플러스 모델의 이점이 분명하다. 화면 크기가 커지다 보니 동영상 등 콘텐츠를 볼 때도 몰입감이 확 높아졌다. 아이패드 미니 5와 유튜브에서 같은 영상을 틀어봤더니 플러스 모델과 아이패드 미니에서 각각 재생되는 영상의 체감 크기는 큰 차이가 없었다. 아이패드 미니 화면이 7.9인치로 더 크지만, 아이패드에서는 유튜브 영상이 화면 비율에 맞게 축소되는 데 비해 갤럭시노트10에서는 영상을 베젤 끝까지 확장해서 꽉 채운 화면으로 볼 수 있기 때문이다. 카메라 측면에서는 기본 모델과 트리플 카메라 구성이 동일하고, ToF 카메라를 사용해 쓸 수 있는 전용 기능도 많지 않아 구별되는 이점을 크게 느끼지 못했다. 화면 크기를 기본으로 고려한 뒤 용량 차이, ToF 카메라로 이용할 수 있는 3D 스캐너 기능이 필요한지를 추가로 검토해서 일반 모델을 구매할지 플러스 모델을 구매할지 선택하면 될 것 같다. 갤럭시노트10 레드와 갤럭시노트10플러스 블루[촬영 채새롬] 특히 이번 갤럭시노트10 시리즈는 국내에서는 KT가 기본 모델 '레드'를, SK텔레콤이 플러스 모델 '블루'를 전용 색상으로 제공하는데, 색상도 선택의 이유 중 하나가 될 수 있겠다는 생각이 들었다. 두 색상 모두 글라스를 기본으로 한 빨간색, 파란색인데, 쨍하면서도 차분한 느낌이 있어 색깔이 오묘하고 매력적이다. 빛이 반사될 때마다 총천연색을 발하는 시그니처 컬러 '아우라 글로우'와는 확실히 다른 매력이 있다. 링크 투 윈도 기능[촬영 채새롬] 이밖에 직접 사용할 때 눈에 띈 기능 중 하나는 노트 시리즈에 새로 추가된 '링크 투 윈도'다. 마이크로소프트 계정을 폰과 윈도우10 PC에서 로그인한 상태로 PC의 마이크로소프트 스토어에서 '사용자 휴대폰' 앱을 내려받으면 내 갤럭시노트10의 사진, 알림, 문자메시지를 한눈에 볼 수 있다. 카카오톡을 기본 메신저로 PC와 연동해 쓰다 보니 휴대폰으로 오는 문자 메시지를 놓치는 경우가 많았는데, 문자가 올 때마다 PC에 알림을 주고 바로 답장을 할 수 있게 돼 있어 편리했다. 그동안 폰에서 찍은 사진을 공유하려면 USB를 연결하거나 메신저로 공유하는 등 과정을 거쳐야 했는데 갤럭시노트10으로 찍은 사진을 실시간으로 컴퓨터로 볼 수 있다는 점도 좋았다. 언팩 행사 당시 잠깐 써봤을 때 적응하기 어려웠던 S펜의 에어 액션은 하루 정도 사용하니 손에 익었다. S펜의 버튼을 눌렀다 떼는 시점을 체득하는 것이 적응의 포인트였다. 다만 상하좌우로 움직이는 것은 용이했지만, 시계 방향이나 반시계방향으로 돌리는 것은 며칠이 돼도 적응되지 않았다. 사진 촬영 시 줌 인, 줌 아웃 등은 좀처럼 동작 인식이 되지 않아 손으로 하는 게 더 마음이 편했다. S펜으로 쓴 손글씨를 텍스트로 바꿔주는 기능은 정확한 글자 인식이라고 하기에는 미흡하지만, 초벌 변환 용도로는 충분한 수준이다. srchae@yna.co.kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>지구상 최고 빌딩 크기 ‘소행성’ 다가온다…다음달 14일 스친다</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>[서울신문 나우뉴스] 지구에 접근하는 소행성 상상도 지구상에서 가장 높은 빌딩 높이에 맞먹는 소행성이 지구를 향해 날아오고 있다. 미 항공우주국(NASA)에 따르면, 아랍에미리트 두바이에 위치한 세계에서 가장 높은 건물인 부르즈 할리파의 높이와 거의 비슷한 소행성이 한 달 안에 지구로 접근할 것이라고 한다. 부르즈 할리파의 높이는 얼마나 될까? 전체 높이는 829.84m이다. 한국의 삼성물산이 시공사로 참여해 건축한 이 초고층 건물은 마지막 층이 160층으로 높이 630m이며, 나머지 부분은 첨탑이다. '2000 QW7'로 불리는 이 소행성은 지름이 290~650m 사이로, 부르즈 할리파보다는 약간 작지만, 이제껏 지구 근처를 지난 여느 소행성에 비해서는 엄청난 덩치를 자랑한다. 참고로, 6600만 년 전 멕시코 유카탄 반도 북부 칙술루브에 떨어져 공룡을 멸종시킨 소행성의 지름은 12㎞였다. 미국 캘리포니아 패서디나에 있는 제트추진 연구소의 한 부서인 지구근접물체연구센터(CNEOS·Center for Near Earth Object Studies)에 따르면, 소행성 2000 QW7는 9월 14일(현지시간) 우리의 푸른 행성 지구 옆을 스쳐지나갈 것으로 예상된다. CNEOS에 따르면, 이 소행성이 지구를 위협할 만한 거리까지 접근하지는 않을 것으로 보인다. 소행성의 속도는 지구에 의해 가속되어 시속 2만3100㎞, 초속으로는 6.4㎞에 달하는 엄청난 속도에 이를 것으로 예측되지만, 지구에 가장 근접할 때의 거리는 약 530만㎞로, 이는 지구-달 사이 거리의 약 14배에 이른다. 그러나 우주적인 척도로 보자면 거의 스치듯이 지나간다는 표현이 과장은 아니다. 지구-태양 간 거리 1억 5000만㎞를 1천문단위(AU)라 하는데, 지구 근처를 지나는 소행성 등의 천체가 지구와의 거리가 1.3AU 이내에 들면 지구 근접 천체로 간주된다. 소행성 2000 QW7은 지구와 마찬가지로 태양을 공전한다. 그러나 궤도는 지구 궤도와 산발적으로 교차한다. 제트추진 연구소에 따르면, 이 소행성이 지구에 마지막으로 접근한 때는 2000년 9월 1일이다. 오는 9월 14일 이후 다음 번 지나칠 것으로 예상되는 시간은 19년 후인 2038년 10월 19일로 예측된다. 이광식 칼럼니스트 joand999@naver.com　 ★ ▶ ⓒ 서울신문(www.seoul.co.kr), 무단전재 및 재배포금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>조국 딸 "3주간 인턴했다더니"…정부 연구기관 기록엔 '닷새짜리 결석생'</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>정부 출연연 KIST 단기연수 지원하고 5일만에 그만 둬 조씨 자소서에는 "3주간 인턴근무하며 실험 준비" 밝혀 조국 법무부 장관 후보자가 23일 오후 서울 종로구 적선현대빌딩에서 논란이 일고 있는 사모펀드와 사학재단 웅동학원을 사회에 환원하겠다고 밝히고 있다. 2019.8.23/뉴스1 © News1 안은나 기자 (서울=뉴스1) 최소망 기자 = "3주간 인턴으로 근무하면서 성인병 관련 약물 실험을 준비했다." 조국(54) 법무부 장관 후보자의 딸 조모(28)씨가 부산대 의학전문대학원 입학 전형에 제출한 자기소개서에 밝힌 한국과학기술연구원(KIST) '3주간 인턴십' 경력이 실은 '닷새짜리 결석생'의 허위 스펙인 것으로 드러나 논란이다. 정부출연연구기관인 KIST에서 당시 조국 딸을 담당했던 한 관계자는 25일 &amp;lt;뉴스1&amp;gt;과의 통화에서 "10년 가량 지나서 잘 기억이 나진 않지만 잘 나오지 않았던 것으로 기억한다"며 "5일 정도 나왔다"고 말했다. 조 후보자의 딸 조씨는 지난 2010년 고려대 환경생태공학부에 입학했다. 이후 2011년 7월 KIST에 '단기연수프로그램'으로 인턴 근무를 시작했다. 1개월 간의 정규 과정이었다. 실제로 조씨가 한 유료 논문 판매 사이트에 올리면서 드러난 부산대 합격 자기소개서에도 "3주간 인턴으로 근무했다"고 기록돼있다. 하지만 KIST의 기록에 따르면 조씨가 연구실에 나온 기간은 2011년 7월 18일부터 22일까지 총 5일에 불과하다. 당시 조씨를 담당한 KIST 관계자는 "5일 정도 나온 것으로 기억한다"면서 "최근에 그 아이가 그 아이(조국 딸)이라는 것을 알고 놀랐다"고 말했다. 또 다른 관계자도 "당시 학생이 며칠 만에 본인 의지로 하기 싫다면서 나간 것으로 알고 있다"고 설명했다. 나라에서 지원하는 1달짜리 단기연수프로그램에 참여해 5일만 참가하고는 대학 자기소개서에는 "3주간 참가했다"고 부풀린 것이다. 결석으로 얼룩진 단기연수프로그램이 의학전문대학원 입학을 위한 스펙으로 포장됐다는 지적이 나온다. KIST 관계자는 "KIST가 국가 연구기관인 만큼 어린 학생들에게 대학원을 진학하거나 취업할 때 이런 곳이 있다는 것을 알리기 위해 인턴제도 등을 많이 도입하고 있다"며 "(조씨가 참여한 단기연수프로그램도) 그 일환이었다"고 설명했다. 이 과정에서 누군가는 기회를 박탈당했을 우려도 제기된다. 한 청년 과학자는 "누군가에게는 소중한 기회이거나 한번밖에 없는 기회일 수도 있었는데 다른 사람이 기회를 박탈당한 게 아닐지 조금 안타깝다"고 털어놓았다. somangchoi@news1.kr [© 뉴스1코리아(), 무단 전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>이통요금 25% 할인 가입자 2천500만명 돌파…5G 후 증가세 둔화</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>약정할인 월평균 가입자 5G 상용화 전 72만명→상용화 후 54만명 LGU+ 선택약정할인 위약금 경감 개시일 타사보다 4개월 늦어 (서울=연합뉴스) 최현석 기자 = 이동통신 가입 때 통신사의 공시지원금 대신 25% 요금할인을 선택한 가입자가 2천500만명을 넘어섰다. 25일 과학기술정보통신부와 통신업계 등에 따르면 휴대전화 요금이 25% 할인되는 선택약정할인 가입자는 지난달 말 현재 2천511만명을 기록했다. 2017년 12월 560여만명에서 작년 말 2천77만명으로 급증한 데 이어 7개월간 추가로 434만명 늘었다. 25% 요금할인 가입자가 19개월 새 4.5배로 급증한 것은 2017년 9월 요금할인율이 20%에서 25%로 상향된 이후 공시지원금을 받고 통신사를 바꾸기보다 기존 통신사의 요금할인을 선택하는 가입자가 늘었기 때문으로 분석된다. 다만 지난 4월 5세대(5G) 이동통신 상용화 후에는 증가세가 둔화하는 양상이다. 월평균 요금할인 가입자는 1~3월 72만명이었지만 5G가 상용화된 3~7월에는 54만명으로 감소했다. 통신사들이 5G 활성화를 위해 공시지원금을 최고 70만원대로 높여 최고 40만원대인 25% 요금할인 혜택과 격차가 벌어진 데 따른 것으로 보인다. 25% 할인을 선택한 가입자가 늘었지만 중도 해지 시 위약금은 통신사별로 큰 차이를 보여 주의가 요구된다. 24개월 선택약정할인으로 LG유플러스에 가입할 경우 16개월 이상 사용해야 위약금이 줄어들기 시작한다. 이는 12개월이 지난 시점부터 위약금이 줄어드는 SK텔레콤과 KT에 비해 4개월이나 늦다. 12개월 약정도 사정이 비슷하다. SK텔레콤과 KT는 6개월 경과 시점부터 위약금이 감소하지만 LG유플러스는 9개월이 지나야 위약금이 줄어든다. 이에 따라 월정액 9만5천원 요금제에 24개월 선택약정(월 2만3천750원 할인)으로 가입한 경우 가입 8개월 차부터 LG유플러스의 위약금이 타사보다 많아지기 시작해 23개월 차에는 17만8천원까지 차이가 확대된다. LG유플러스 선택약정할인 가입자는 3사 가입자의 30% 수준인 750만명에 달할 것으로 추산된다. 타사와 동일하게 25% 할인 혜택을 제공하면서 더 많은 위약금을 청구하는 것은 문제가 있어 개선이 필요하다는 지적이 나온다. LG유플러스는 "기기변경 때 위약금을 면제하는 정책을 가장 먼저 채택하는 등 고객 혜택 수준이 타사보다 높은 경우도 많다"며 "약정할인 위약금은 타사와 마찬가지로 변경하는 것을 검토하고 있다"고 반박했다. 광진구 집단상가 내 이동전화 판매점[촬영 최현석] harrison@yna.co.kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>애플 진입 노리는 中 BOE 실력은…"韓 따라잡는건 시간문제"</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>BOE, B7 가동하면서 B11·B12·B15 패널 공장 동시 투자 "생산량 곧 삼성 추월, 수율도 2~3년 뒤 70% 올라올 듯" 2020년형 아이폰부터는 삼성·LG 패널과 함께 들어갈 듯 국내 유기발광다이오드(OLED) 장비업체 A사는 중국 최대 디스플레이 회사 BOE와 계약서를 쓰고 관련 장비를 설계·제작하고 있다. 중국 몐양에 있는 모바일 OLED 패널 공장 ‘B11’에 들어갈 장비다. A사 관계자는 "삼성·LG디스플레이의 투자가 무기한 중단된 상황에서 BOE는 모바일 OLED 패널 공장 투자를 동시다발적으로 하고 있다"면서 "올해 하반기 BOE의 ‘B12(중국 충칭)’에서도 장비 발주가 있을 것으로 예상되고, 최근 건설 계획을 발표한 ‘B15(중국 푸저우)’도 투자 계획을 이미 다 짜놓고 중국 고객사 판매 동향·수율(완제품 비율)을 보며 시기를 저울질하고 있는 것으로 알고 있다"고 전했다. 중국 BOE가 첫 모바일 OLED 패널 공장인 ‘B7’에서 만든 패널이 탑재된 화웨이의 ‘메이트 20 프로’. / 블룸버그 25일 디스플레이 업계에 따르면, 중국 정부의 지원을 받아 액정표시장치(LCD) 시장을 빠르게 장악한 BOE가 ‘물량 공세’ 방식으로 모바일 OLED 시장에도 뛰어들고 있는 것으로 나타났다. 중국 청두에 있는 첫 OLED 패널 공장인 ‘B7’을 가동하면서 동시에 B11·B12·B15에 투자하거나 투자를 검토하고 있는 것이다. 시장조사기관 스톤파트너스에 따르면, 4개 공장을 모두 가동할 경우 전체 패널 생산량은 월 18만장 수준으로 현재 모바일 OLED 1위인 삼성디스플레이(16만5000장)를 훌쩍 넘어서게 될 전망이다. 4개 공장이 모두 돌아가는 시기는 2023년으로 점쳐진다. 업계에서는 현재 BOE의 모바일 OLED 수율을 50% 수준으로 보고 있다. 이충훈 유비리서치 대표는 "이미 BOE의 패널 품질은 빠르게 올라가고 있는 것으로 파악되고 있다"며 "수율은 2~3년 안에 70% 이상으로 올라갈 것"이라고 예상했다. 윤주호 메리츠종금증권 연구원은 "‘수율’보다 더 중요한 것은 ‘수요’"라면서 "BOE는 LCD 때도 일단 많이 만든 다음 품질이 좋은 것은 세트업체에 팔고, 그렇지 않은 것은 장난감 회사에 파는 식으로 대응해 수율을 끌어올려 왔다. OLED에서도 생산 여력을 늘려 일단 이런 저런 수요에 대응하면서 수율도 금세 올릴 것"으로 내다봤다. 현재 BOE의 모바일 OLED 패널 수요 대부분은 화웨이를 비롯한 중국 스마트폰 제조사다. 여기에 애플도 내년 아이폰 채용을 목표로 BOE의 OLED 패널 품질을 테스트 중인 것으로 알려졌다. 애플은 패널의 안정적 공급, 저렴한 구매단가를 위해 공급선 다변화에 수년간 공을 들여왔다. 여기에 2020년 아이폰부터는 LCD 패널을 아예 쓰지 않고, OLED 패널 제품으로만 내놓기 위한 계산도 깔려 있다. 지난해 판매 대수 기준으로 아이폰 중 OLED 모델은 58% 수준이었고, 전량을 삼성디스플레이로부터 구입해 왔었다. 올해 신작부터는 LG디스플레이도 일부 물량(약 600만대) 패널을 공급한다. 한 디스플레이 업계 관계자는 "LG디스플레이도 품질 테스트에서 한 번에 통과하지 못했을 정도로 애플의 기준이 매우 높은 것으로 알고 있다"면서 "다만, BOE가 LCD 수율도 보란 듯 끌어올렸던 경험이 있고 국내 OLED 전문가들을 대거 영입해 기술력을 끌어올리고 있어 2020년, 늦어도 2021년에는 애플에도 납품할 수 있을 것으로 본다"고 말했다. 그래픽=송윤혜 시장조사업체 IHS마킷이 집계한 올해 1분기(1~3월) 모바일 OLED의 글로벌 시장 점유율을 보면 삼성디스플레이의 점유율은 88.0%로 지난해 같은 기간(95.7%)보다 7.7%포인트나 줄어든 것으로 나타났다. 반면 중국 BOE는 0.1%에서 5.4%로 점유율을 확 늘리며 삼성디스플레이에 이어 2위에 이름을 올렸다. 에버디스플레이(중국), LG디스플레이, 비전옥스(중국)가 그 뒤를 이었다. [장우정 기자 woo@chosunbiz.com] chosunbiz.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>삼성, 벨기에서 EUV용 포토레지스트 조달…SK하이닉스도 이미 거래 중</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>삼성전자가 극자외선(EUV)용 포토레지스트(PR)를 벨기에에서 조달하고 있는 것으로 파악됐다. 일본 정부의 대 한국 수출 규제에 따른 대응으로 수입 노선이 추가됐다. 25일 업계에 따르면 삼성전자는 지난 7월 일본 수출 규제 조치가 시행된 후 일본에서 수입해 온 EUV PR 일부를 벨기에에서 조달하고 있다. 이 EUV PR는 A사가 일본에서 생산, 공급한 것이었다. 그러나 삼성전자는 7월 이후 이 일본산 EUV PR와 동일한 제품을 벨기에 B사에서 수급하고 있다. 삼성전자가 벨기에에 위치한 B사에서 품질이 같은 EUV PR를 공수할 수 있었던 것은 B사가 A사가 만든 합작사기 때문이다. A사는 지난 2015년 반도체 전문 연구소와 함께 B사를 설립했다. 이 사안에 정통한 관계자는 “규제 시행 이후 제품 공급처가 일본에서 벨기에로 이전됐다”면서 “쉽게 말해서 같은 EUV PR가 벨기에를 통해 들어오고 있다고 보면 된다”고 설명했다. 삼성전자 화성 파운드리 공장 전경(자료: 삼성전자) 업계에 따르면 삼성전자가 사용 중인 EUV PR는 A사를 포함한 일본 3개 회사 제품이다. 이 가운데 2개 회사 소재는 7나노(㎚) 로직 디바이스를 제조하는 데 쓰이고 나머지는 D램 연구용이다. 삼성전자는 아직 D램에 EUV를 적용하지 않아 현재 제조 현장에서 사용되는 EUV PR는 7㎚ 로직 디바이스용이었다. 이 때문에 일본의 수출 규제 시행으로 여파가 우려된 것은 7㎚ 반도체 제조에 필요한 EUV PR의 수급이었지만 삼성은 일단 A사와의 사전 공조를 통해 대비책을 마련한 것으로 풀이된다. 그동안 벨기에가 일본 소재 수출 제한의 우회로 및 대처 방안 가운데 하나로 거론돼 왔지만 구체적인 내용이 파악된 건 처음이다. 업계에 따르면 지난 7월 한 달 동안 일본에선 수출 승인이 한 건도 없었음에도 삼성전자는 이미 벨기에에서 EUV PR를 받은 것으로 전해졌다. A사 외 7㎚ 로직 디바이스에 사용되는 또 다른 일본 회사 C사의 EUV PR는 현재 일본 내에서만 생산되고 있다. 따라서 이 소재는 일본 정부의 승인을 받아야만 한국에 들어올 수 있다. 삼성전자는 수출 승인이 불확실하고, 벨기에가 대체 공급선으로 떠올라 C사 EUV PR를 벨기에 제품으로 교체하는 방안을 검토 중인 것으로 전해졌다. 일본산 EUV PR 한국 수출은 이달 들어 간간이 승인됐다. 지난 7일과 19일이다. 일본 정부가 다른 소재는 제외하고 EUV PR만 두 차례 승인한 이유가 명확하지 않아 배경에 관심이 쏠리기도 했다. 그러나 벨기에를 통한 EUV PR 공급 사실이 알려지면서 다른 일본 소재 회사들이 정부 승인을 촉구했을 가능성이 있어보인다. 한편 삼성전자뿐만 아니라 SK하이닉스도 벨기에에서 EUV PR를 공급 받고 있는 것으로 파악됐다. SK하이닉스는 일본에서 벨기에로 전환한 삼성전자와 달리 일본 수출 규제와 무관하게 이전부터 벨기에와 거래해 왔다. SK하이닉스는 EUV 양산 전이고, 벨기에에 거래처를 두고 있어 일본의 EUV PR 수출 규제와 관련해 삼성전자보다는 영향이 덜하다는 평가다. 삼성 서초사옥에 전시된 반도체 웨이퍼. &amp;lt;전자신문 DB&amp;gt; 윤건일 전자/부품 전문기자 benyun@etnews.com [Copyright ⓒ 전자신문 &amp;amp; 전자신문인터넷, 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>결국 10만원짜리 갤럭시노트10은 없었다</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>개통 후 첫 주말 실구매가 주중보다는 내려가 사전판매 시 약속했던 수준보다는 높아 제2의 빵집 대란 기다리며 관망하는 소비자 늘어나 삼성전자가 20일 '갤럭시노트10' 국내 사전 판매량이 지난 17일 기준 100만대를 넘겼다고 밝혔다. 최종 사전 판매 물량은 130만대 이상으로 추정된다. 이는 전작 대비 2배 이상 증가한 수치다. 이날 한 시민이 서울 강남구 삼성전자 딜라이트샵을 찾고 있다. /문호남 기자 munonam@ [아시아경제 임온유 기자] 결국 10만원짜리 갤럭시노트10은 없었다. 고로 대란도 없었다. 주말에도 불법보조금 규모가 신통치 않자 휴대폰 집단상가에서는 소비자가 갤럭시노트10 구매에 선뜻 나서지 않는 풍경이 그려졌다. 방송통신위원회-이동통신사-휴대폰판매점-소비자 간의 눈치싸움이 지속되면서 판매열기가 갤럭시S10 5G 첫 주말에 미치지 못하는 것으로 보인다. 물론 기다림에 지쳐 '졸업'을 선언하는 이들도 적잖게 등장했다. 졸업이란 휴대폰 커뮤니티에서 쓰이는 은어로, 구매를 완료했다는 뜻이다. 이 와중에 갤럭시노트10 플러스 512GB 아우라 블랙, SK텔레콤 전용인 갤럭시노트10 플러스 256GB 아우라 블루 등 특정 모델의 물량 부족 현상까지 이어지면서 시장 상황이 매우 복잡하게 돌아가고 있다. 삼성전자가 20일 '갤럭시노트10' 국내 사전 판매량이 지난 17일 기준 100만대를 넘겼다고 밝혔다. 최종 사전 판매 물량은 130만대 이상으로 추정된다. 이는 전작 대비 2배 이상 증가한 수치다. 이날 서울 강남구 삼성전자 딜라이트샵을 찾은 시민들이 제품을 살펴보고 있다. /문호남 기자 munonam@ 삼성전자 갤럭시노트10이 출시된 이후 첫 주말인 24일 최저 실구매가는 일반형(124만8500원)의 경우 30만원 초반대, 플러스형(256GB 139만7000원, 512GB 149만6000원)의 경우 40만~50만원대에서 책정됐다. 갤럭시노트10 개통일인 20일을 포함한 주중보다는 나아졌지만 당초 휴대폰판매점이 약속했던 수준(10만~30만원대)에는 크게 못미치는 금액대다. 이에 첫 주말을 기다리자며 관망적 자세를 취해온 사전예약자들이 다시 한번 고민에 빠졌다. 한 휴대폰 유통업계 관계자는 "신도림 휴대폰 집단상가의 경우 예비 구매자로 북적이긴 했지만 실구매까지 이어지는 비율이 낮은 것으로 분석된다"고 말했다. 갤럭시노트10 실구매가는 공식판매가에 비하면 매우 낮은 수준이다. 그럼에도 구매를 망설이는 이유는 소비자가 상반기 LG전자 V50 씽큐의 '빵집' 대란을 떠올리고 있기 때문이다. 빵집이란 실구매가 0인 폰을 뜻한다. 당시 이동통신3사는 5G 초기 가입자를 유치하기 위해 막대한 보조금으로 경쟁한 바 있다. 결국 갤럭시노트10을 사려는 소비자의 망설임은 과거 이통3사의 과도했던 보조금 때문인 셈이다. 갤럭시노트10의 사전판매량은 130만대로 전작 갤럭시노트9의 두배에 이르렀다. 이에 업계는 일찌감치 갤럭시노트10의 흥행을 점쳤다. 그러나 낮은 보조금으로 실구매율이 목표치에 도달하지 못하자 업계는 흥행에 제동이 걸릴까 우려하고 있다. 일부 소비자는 결국 대란은 터질 것이라며 계속 버티겠다는 의지를 드러냈다. 그러나 방통위의 감시 아래 이통3사가 시장 안정화에 방점을 찍으면서 당분간 대란은 없을 가능성이 높다. 임온유 기자 ioy@asiae.co.kr &amp;lt;ⓒ경제를 보는 눈, 세계를 보는 창 아시아경제 무단전재 배포금지&amp;gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>삼성전자, 갤노트10 핵심 서비스로 블록체인 앱 '림포' 소개</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>삼성전자가 최신 스마트폰 갤럭시노트10을 출시하면서 블록체인 애플리케이션(앱)을 핵심 서비스로 홍보하고 있어 눈길을 끈다. 유력 스마트폰 제조사 가운데 가장 먼저 블록체인 지갑 서비스를 탑재하면서 블록체인 생태계 조성에 힘쓰고 있다는 것을 강조하기 위한 것으로 풀이된다. ■갤노트10 체험관 갤럭시스튜디오에서 블록체인 앱 ‘림포’ 만난다 삼성전자는 지난 23일 공식 출시한 갤럭시노트10을 홍보하기 위해 전국 주요 지역 ‘갤럭시노트10 5G’와 ‘갤럭시노트10 플러스 5G’를 체험할 수 있는 갤럭시스튜디오를 마련했다. 갤럭시스튜디오에서는 이용자들이 자유롭게 갤럭시노트10을 체험해볼 수 있다. 서울 종로구 익선동에 위치한 갤럭시스튜디오에서 갤럭시노트10 5G를 체험해볼 수 있다. 특히 삼성전자는 이용자들이 갤럭시노트10을 통해 이용할 수 있는 다양한 혁신 서비스들을 미리 만나볼 수 있도록 했다. 이 혁신 서비스 가운데 블록체인 기술이 적용된 앱이 있다. 주인공은 바로 운동한만큼 암호화폐 보상을 주는 앱 ‘림포’다. 서울 종로구 익선동에 위치한 갤럭시스튜디오에서 갤럭시노트10과 ‘림포’ 앱을 만날 수 있었다. 갤럭시스튜디오의 안내직원에게 블록체인 앱을 살펴볼 수 있다고 해서 왔다고 했더니 바로 림포 앱을 구동시켜 준다. ■운동미션 수행하면 암호화폐 주는 ‘림포’ 림포는 리투아니아 블록체인 프로젝트가 개발한 앱이다. 매일 이용자에게 걷기나 뛰기 미션을 주고 이 미션을 완수할때마다 이용자에게 보상으로 림포토큰을 제공한다. 이 림포토큰으로 림포 앱 내의 림포샵에서 다양한 전자기기나 운동화, 운동복 등을 구매할 수 있다. 갤럭시스튜디오에서 갤럭시노트10 5G로 체험한 블록체인 기반 애플리케이션(앱)인 '림포' 갤럭시스튜디오에서는 림포 앱이 어떻게 이용되는지만 확인할 수 있었다. 미션을 수행하고 받은 림포토큰을 삼성 블록체인 월렛을 통해 출금하는 체험이 가능했다. 출금은 출금권을 구매하는 형태로 이뤄진다. 1000림포토큰을 출금하려면 100림포토큰이 수수료로 필요하다. 출금권을 구매하면 1000림포토큰을 삼성 블록체인 월렛으로 이동시킬 수 있다. 이렇게 삼성 블록체인 월렛으로 이동한 림포토큰을 다시 림포토큰이 상장된 암호화폐 거래소 지갑으로 이동시키면 현금으로 바꿀 수 있다. 수수료가 아깝다면 그냥 림포샵에서 다른 상품권이나 제품을 구매하면 된다. 체험버전에서는 신세계백화점 1만원 상품권이 1000림포토큰으로 판매된다고 안내돼 있다. 갤럭시버즈와 같은 제품과 스타벅스 교환권 등도 구매할 수 있다. ■림포 한국 이용자 2만명 넘어, 보상액도 1억원 돌파 림포 앱은 구글 플레이스토어 등 앱스토어를 통해 내려받을 수 있다. 갤럭시노트10이 아니더라도 다른 스마트폰에서 이용할 수 있다. 다만 삼성 블록체인 월렛이 탑재된 갤럭시노트10과 갤럭시S10이 아니면 출금권을 활용한 암호화폐 출금이 불가능하다. 현재 림포 앱 이용자 수는 글로벌 기준 23만명이고, 이 가운데 2만명이 한국인이다. 한국이용자들이 수행한 미션이 100만건을 돌파했고 보상액도 1억원을 넘겼다. 업계 한 관계자는 “최근 여러 블록체인 기반 서비스가 출시되고 있지만 가장 많이 이용되고 있는 앱이 림포일 것”이라며 “실생활에서 블록체인 기술을 직접 활용할 수 있다는 점을 증명한 앱이기 때문에 삼성전자도 림포 앱을 블록체인 기술 홍보용으로 선택했을 것”이라고 전했다. 한편 갤럭시스튜디오에서 체험한 갤럭시노트10의 또다른 앱 가운데 하나인 ‘삼성글로벌골스’도 눈길을 끌었다. 이 앱은 이용자들이 유엔개발계획에 직접 기부를 할 수 있도록 지원하는 앱이다. 최근 블록체인 기술이 투명한 기부문화를 만들 수 있다는 점에서 주목받고 있는 만큼, 향후 이 앱에도 블록체인 기술이 적용될 가능성이 높아 보인다. jjoony@fnnews.com 허준 기자 ※ 저작권자 ⓒ 파이낸셜뉴스. 무단 전재-재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>물 만난 ‘청불’ 보드게임, 애플 인기순위 점령</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>25일 애플 앱스토어 인기 순위(게볼루션 집계) - 맞고·포커 등 애플 앱스토어 진입하자 인기 상위 직행 - 향후 거래소 갖춘 대형 RPG, 애플 앱스토어 대응 촉각 [디지털데일리 이대호기자] 국내 애플 앱스토어에서 만 18세 이상 이용가인 청소년이용불가(청불) 게임 유통을 할 수 있게 되자 맞고·포커 등 성인 대상의 보드게임이 인기를 끌고 있다. 25일 애플 앱스토어 무료 인기 순위(게볼루션 집계)를 보면 1위 한게임 섯다, 3위 피망 뉴맞고, 4위 피망 섯다, 6위 한게임 신맞고, 7위 한게임 포커 등이 올라와 순위 전반을 재편한 상황이다. 간단한 보드게임 특성 상 시장 대응이 가장 빨랐고 성인 이용자들도 iOS 플랫폼에서 즐길 수 있는 보드게임에 반색하는 분위기다. 맞고·포커 등의 모바일 보드게임은 지난 23일 일제히 출시됐다. 업계에선 구글플레이처럼 애플 앱스토어에서도 보드게임들이 꾸준한 매출 순위를 유지할지에 관심을 보이고 있다. 구글플레이에선 보드게임 2강 업체인 네오위즈 대비해 한게임이 약세를 보였으나 애플 앱스토어에선 각축을 벌일지 주목된다. 애플 앱스토어의 순위 재편은 현재 진행형이다. 향후 아이템 거래소를 갖춘 대형 역할수행게임(RPG)들이 애플 앱스토어에 진입, 매출 순위를 뒤흔들지도 기대를 모은다. 앞서 게임물관리위원회 판단으로 유료 캐시를 활용한 아이템 거래소 콘텐츠 유무에 따라 청불 또는 청소년이용가 등급이 나뉜 바 있다. 리니지M 등이 대표적으로 청불과 12세 이용가로 나눠 서비스 중이다. 리니지M 청불 등급은 출시 이후 2년이 넘게 구글플레이 매출 1위 붙박이인 상황이다. 이를 감안하면 리니지M 성인 이용자층을 겨냥한 애플 앱스토어 대응은 시간문제라는 관측이 나온다. 올 하반기엔 리니지M의 적통을 잇는 리니지2M도 출시를 앞뒀다. 한편 한국모바일산업연합회(MOIBA)가 발간한 ‘2018년 대한민국 모바일 콘텐츠산업 현황’ 보고서에 따르면 그해 구글플레이 매출액은 5조4098억원(전년비 10.8%↑)으로 전체 63.2%를 차지했다. 애플 앱스토어 매출액은 2조1211억원(전년비 9.4%↑)으로 24.8% 비중을 보였다. 성인 게임물 유통으로 애플 앱스토어 매출액 비중에 변화가 찾아올지 주목된다. &amp;lt;이대호 기자&amp;gt;ldhdd@ddaily.co.kr &amp;lt;저작권자 © 디지털데일리 무단전재-재배포금지&amp;gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[영상] 애플 아이폰 11 vs 삼성 갤럭시 폴드, 9월 맞장 뜬다 </t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>(지디넷코리아=유회현 기자) 삼성전자 폴더블 스마트폰 갤럭시 폴드가 9월 출시 예정이다. 지난 2월 앞서 공개한 갤럭시 폴드는 일부 결함이 발견되면서 여론의 뭇매를 맞았다. 하지만 삼성전자는 4월 출시 일정을 무기한 연기하고 힌지 부분의 들뜸 현상과 필름처럼 보이는 디스플레이 부품 등 내구성 개선을 위한 개발에 착수했다. 2019년 하반기 새로운 아이폰 출시가 예고된 가운데 결함을 고치고 새롭게 돌아온 갤럭시 폴드가 2천 달러 대의 가격대로 선전 할 수 있을지 지켜봐야 할 듯하다. 유회현 기자(lusy33@zdnet.co.kr) /</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>‘명불허전’ 갤노트10 출시 첫 주말 “재고가 없어요”</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>하반기 기대작 갤노트10, 20일 선개통·23일 공식출시 첫주말 대리점·판매점 모두 "재고 없어 못 판다" 사전 예약물량도 해소 안돼 물량부족 이어질 듯 "번이 혜택도 그닥…가격 오히려 더 오를 수 있다" [이데일리 장영은 기자] “갤노트10 플러스요? 우린 물건이 없어요” 갤럭시노트(갤노트)10 출시 첫 주말, 강변 테크노마트 내 휴대폰 집단상가의 분위기는 ‘역대 최대’ 수준이라는 사전 예약 열기를 실감케 했다. 갤노트10은 지난 20일부터 사전예약자 대상 선개통이 시작됐으며 23일 공식출시 됐다. 20일 서울 종로구 LG유플러스 종각직영점에서 열린 삼성전자 5G폰 ‘갤럭시노트 10’ 출시 기념행사에서 고객이 갤럭시노트10을 받고 있다. (사진= 뉴시스) ◇ 개통 대기 서류 줄줄이 밀려…“열에 아홉은 갤노트10” 공식 출시 당일인 23일에도 분위기를 보고자 방문했지만 주말은 확실히 달랐다. 평일인 전날은 휴대폰 판매점이 모여 있는 6층 전체에 20여명 정도의 사람들이 휴대폰을 ‘보러’ 다니는 수준이었고, 간간이 (계약) 서류를 쓰고 있는 모습이 보였다. 24일은 늦은 오후 시간에 방문했음에도 거의 모든 판매점마다 상담을 하거나 서류를 쓰는 사람이 있을 정도였고, 일부 ‘인기’ 매장은 서너명씩 기다리기까지 했다. 판매점 10곳을 돌며 갤노트10 가격과 반응을 알아본 결과 4곳은 갤노트10 플러스는 아예 물량이 없다며 손을 내저었다. 나머지 판매점들도 “재고를 확인해 봐야 한다”며 바로 개통이 힘들 수도 있다고 전했다. ‘ㄷ’ 판매점 매장 직원은 “일단 원하는 색깔 순서를 말해주면 창고에 가서 확인해 보겠다”면서 “블랙이랑 화이트가 있을 가능성이 가장 높고 블루랑 아우라 글로우는 솔직히 언제 될지 모르겠다. 사전 예약자들도 못 받고 있는 상황”이라고 말했다. 매장에 옮겨 놓은 물량은 이미 오전에 다 나갔고 사겠단 사람이 있을 때만 재고를 확인해 가지고 오는 식이었다. 재고가 있으면 기기는 바로 받아갈 수 있지만 개통도 지연될 수 있다는 게 매장측 설명이었다. 이 직원은 “지금 마감 시간까지 2시간도 채 안 남았는데 오늘 개통물량이 엄청 밀려 있다”면서 “오늘 8시까지 안 되면 내일은 휴일이라 월요일 아침에 될텐데 그 정도는 생각하고 계셔야 한다”고 설명했다. 개통 대기 물량 대부분이 갤노트10 이라고 덧붙였다. 갤럭시노트10 플러스 아우라 글로우 색상. (사진= 삼성전자) ◇ 사전 예약 물량도 아직 해소 안돼…“가격 오히려 더 오를 수도” 이같은 인기에도 가격 경쟁은 그다지 과열되지 않는 분위기였다. 가격 문의를 한 매장 중 3곳은 “알아본 가격이 얼마냐”며 내민 계산기에 40만원대 중반의 가격을 찍,자 “우리는 이 가격에 맞춰줄 수 없다”면서 ‘협상’ 자체를 포기했다. 나머지 3곳도 “그 정도가 지금 마지노선”이라며 새롭게 가격을 제시하진 않았다. 지난 23일 신분증을 맡기는 조건으로 갤노트10 플러스 모델을 30만원대 후반까지 제시했던 것을 감안하면, 사려는 사람은 늘었지만 판매 경쟁은 오히려 냉담해진 셈이다. ‘S’ 판매점 직원은 “지금 분위기가 막 (현금 지원을) 쏘고 이럴 수 없다”면서 “번이(번호이동)를 해도 가격 차이가 많이 해봐야 5만원인데, 그나마 이건 물량이 없어서 신분증 맡겨놓고 가셔야 한다”고 했다. 직영 대리점도 상황은 비슷했다. 서울 종로구에 위치한 한 KT 대리점에서는 “공시지원금과 카드 사용을 통한 할인 혜택 외에는 지원해 드릴 수 있는 부분이 없다”며 “번호이동 추가 지원은 없다”고 딱 잘라 말했다. 서울 송파구의 한 SKT 대리점은 “요금제에 따른 공시지원금이 다 이긴 한데 이번 주말에만 특별히 ‘89’(8만9000원)요금제로 하실 경우 30만원 페이백을 해드린다”고 안내했다. 전날까지만 해도 가격이 더 떨어질 수도 있다는 판매점이 꽤 있었으나, 물량 부족에 실 구매자들의 방문이 이어지면서 오히려 가격이 오를 것 같다는 전망이 우세했다. 매장에서 만난 30대 회사원 최모씨는 “사전 예약했다가 그 가격엔 도저히 안 될 것 같다는 얘기를 듣고 매장을 방문했다”면서 “괜히 나중에 9월에 가격 더 내고 (사전예약) 사은품도 못 받게 될 것 같아서 지금 받아가려고 온 것”이라고 말했다. [이데일리 이동훈 기자]갤럭시노트10 일반 모델과 플러스 모델 사양비교. 장영은 (bluerain@edaily.co.kr) 네이버 홈에서 ‘이데일리’ 뉴스 꿀잼가득 , 청춘뉘우스~ ＜ⓒ종합 경제정보 미디어 이데일리 - 무단전재 &amp;amp; 재배포 금지＞</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 시험을 잘 보려면 시험을 자주 봐야 한다? </t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>[ 토요판] 정수근의 기억실험실 ⑨ 공부 잘하는 법 반복학습은 암기에 도움되지만 들인 노력에 비하면 효과는 적어 한번 공부한 뒤 연습시험 통해 끄집어내 떠올리면 더 오래가 좌뇌형-우뇌형, 시각형-청각형… 말 많지만 검증된 학습법 아직 없어 ‘깊게 이해, 문제 풀고, 적절한 수면’ 평범하지만 최선인 공부의 길 배운 내용을 잘 이해하더라도 이해한 것을 기억하지 못한다면 소용이 없을 것이다. 하지만 단지 반복해서 읽고 쓰는 암기법만으로는 공부한 내용을 오래 기억하는 데 한계가 있다. 게티이미지뱅크 고등학생 시절에 영어 단어를 외우기 위해 종이에 단어를 한가득 채워 쓰곤 했다. ‘깜지’ 또는 ‘빽빽이’라고도 불리는 이 공부법은 이른바 ‘암기과목’을 공부하는 대표적인 방법이었다. ‘깜지’를 하느라 다 쓴 볼펜을 자랑스럽게 모아놓는 친구도 있었다. 하지만 안타깝게도 쌓여가는 볼펜의 개수가 꼭 높은 성적으로 이어지는 것은 아니었다. 그래도 공부를 잘하려면 암기도 잘해야 하는 것은 사실이다. 아무리 배운 내용을 잘 이해하더라도 기억하지 못한다면 소용이 없을 것이다. 오랜 시간 여러번 반복하는 게 능사가 아니라면 과학적으로 검증된 ‘공부 잘하는 방법’이 따로 있을까? 반복학습보다 인출연습 가장 보편적인 공부법은 아마도 ‘반복해서 읽기’일 것이다. 이미 많은 사람이 알고 있겠지만 단지 교과서를 여러번 되풀이해서 읽거나 ‘깜지’를 쓰는 방법은 들인 노력에 비해 효과가 그리 크지는 않다. 사실 얼마나 많이 반복하는가보다는 한번을 하더라도 얼마나 제대로 공부하느냐가 중요하다. 1975년에 이를 보여주는 연구 결과가 발표됐다. 캐나다 토론토대학 연구진은 실험 참가자들에게 여러 단어를 제시하면서 단어에 관한 몇가지 과제를 주었다. 단어의 글자가 대문자인지 소문자인지(시각적 처리 과제), 단어가 다른 단어랑 운율이 맞는지(청각적 처리 과제), 단어가 문장의 빈칸에 들어가도 되는지(의미적 처리 과제)를 판단하게 했다. 실험 참가자들에게 단어를 외우라는 지시를 하지는 않았다. 연구진은 단어 처리 과제를 마친 실험 참가자들에게 예고하지 않은 깜짝 테스트를 시행해서 얼마나 많은 단어를 기억하는지 조사했다. 결과는 아마 쉽게 예상할 수 있을 것이다. 사람들은 시각 또는 청각으로 정보를 처리했던 단어보다 의미를 따져 처리한 단어를 더 잘 기억할 수 있었다. 즉, 더 복잡하고 의미 있는 정보 처리를 할수록 더 오래 기억할 수 있다는 것이다. 그렇다면 의미를 되새기며 교과서를 여러번 되풀이해 읽으면 기억에 도움이 될까? 연구에 따르면, 그저 반복해 공부하는 것보다는 중간에 시험을 치르는 게 훨씬 효과적일 수 있다. 미국 세인트루이스 워싱턴대학의 헨리 로디거 교수가 2006년 이와 관련한 실험을 했다. 그는 실험에 참가한 학생들에게 과학 내용이 담긴 교재 자료를 제시하고서 공부하게 했다. 일부 학생들은 자료를 두번 반복해서 공부했고, 다른 학생들은 한번 공부하고 연습시험을 한번 치렀다. 5분 뒤 자료 내용을 얼마나 잘 기억하는지 검사한 결과에서는, 반복 학습한 학생들이 더 높은 점수를 받은 것으로 나타났다. 그러나 일주일 뒤 다시 시행한 검사에서는 결과가 뒤집혔다. 한번 공부하고 연습시험을 봤던 학생들이 시험 없이 반복 학습만 했던 학생들보다 실제 시험에서 더 좋은 점수를 받은 것이다. 즉, 반복 학습을 통해 정보를 여러번 저장하는 것과 비교해, 저장된 정보를 시험문제 풀이를 통해 인출하는(끄집어내어 떠올리는) 연습을 하는 게 더 효과적일 수 있다. 연습시험이 그저 시험에 적응하는 데 도움을 주었을 뿐은 아닐까? 다른 연구에서는 실제 시험과 연습시험의 형식이 다르더라도 연습시험이 반복 학습보다 더 나은 공부법이라는 결과가 제시됐다. 공부한 내용을 다시 읽으면 뇌에서는 이전에 저장된 정보만이 다시 활성화될 가능성이 높다. 하지만 시험문제를 풀면서 답을 떠올릴 때는 저장했던 정보와 함께 관련된 다른 정보도 함께 활성화될 수 있다. 이 과정에서 기존 지식과 새로 배운 정보가 통합되기도 하고, 관련이 없어 방해되는 정보는 억제되기도 한다. 그래서 인출 연습을 한 정보는 좀 더 정교화되고 잘 기억될 수 있다. 반복해 읽는 학습법은 ‘많이 공부했다’는 만족감을 준다. 반면에 연습시험 문제를 풀다 보면 모르는 게 많다고 느껴질 수 있다. 하지만 많은 연구들은 일단 학습을 한 다음에는 반복 학습보다 반복 인출 연습이 기억을 더 오래가게 한다는 점을 보여주고 있다. 그렇다면 앞으로 공부할 때 다음 몇 가지를 시도해볼 만하다. 교재에서 한 챕터가 끝나는 곳에 연습문제가 실려 있다면 그냥 넘어가지 말고 꼭 풀어보기 바란다. 챕터를 반복해 공부하는 것보다 효과가 더 좋을 것이다. 연습문제가 없다면 직접 질문을 만들고 답해보거나, 배운 내용을 차례로 다시 떠올려보는 인출 연습을 해봐도 좋다. 배웠던 모든 내용을 다 기억해내지 않아도 괜찮다. 로디거 교수의 다른 연구에서는 인출 연습을 한 정보뿐만 아니라 시험에서 다뤄지지 않은 다른 관련 정보의 기억도 덩달아 향상되었다. 학생을 가르치는 선생님이라면, 중간고사와 기말고사만 치르기보다는 학기 중에 쪽지시험을 여러번 보는 것도 배운 내용을 잊지 않게 하는 좋은 방법이다. 현재로선 여러 연구에서 검증된 효과적 학습법은 생각보다 평범하다. 주의 깊게 공부하고, 배운 내용을 시험해 보고, 적절한 수면을 취하는 게 좋다. 게티이미지뱅크 좌뇌형은 분석적, 우뇌형은 창의적 반복 학습이건 인출 연습이건 간에 공부에 쓸 수 있는 시간은 한정되어 있다. 당장 내일이 시험이라면 밤을 새워 한 글자라도 더 머릿속에 담고 싶을 것이다. 하지만 이미 이전 연재 글에서 다뤘듯이 뇌는 잠자는 동안에 공부한 내용을 복습한다.(5월16일치, ‘4당5락? 잠자는 동안 뇌는 낮에 공부한 내용 복습한다’) 잠을 자지 않으면 학습한 내용이 장기기억으로 전환되기 어렵다. 적절한 수면의 중요성을 보여주는 또 다른 사례가 있다. 혹시 ‘서머타임’(일광시간 절약제)을 기억하는가? 낮이 긴 여름에는 표준시를 1시간 당기고 낮이 짧은 겨울엔 시간을 되돌리는 제도이다. 우리나라에서도 몇번 시행되다가 1988년 이후에 사라진 제도이지만, 미국에서는 여전히 여름마다 시간을 1시간 당기고 있다. 미국의 모든 지역에서 서머타임을 시행하지는 않기 때문에, 같은 주 안에서도 서머타임을 시행하는 곳과 시행하지 않는 곳이 나뉘기도 한다. 이를 이용해 연구자들이 재밌는 비교를 해봤다. 미국 인디애나주에서 서머타임을 시행한 카운티의 학생들은 1시간 일찍 일어나야 했기에 일주기 리듬(생체시계)이 흐트러지게 되었다. 이 학생들은 미국의 대입 수능시험 격인 에스에이티(SAT) 시험에서 서머타임 제도를 시행하지 않은 카운티의 학생들보다 약 16점이 낮은 점수를 받았다. 서머타임으로 단순히 일어나는 시간만 빨라지는 게 아니다. 서머타임 시행 직후에는 일주기 리듬이 바뀌고 잠 시간이 줄어 주의 집중의 기능도 떨어질 수 있다. 학습 효율을 높인다고 알려진 여러 방법이 있다. 하지만 널리 알려진 학습법 중에도 과학적 근거가 부족한 것들이 있다. 대표적인 예가 ‘좌뇌형-우뇌형’ 학습 유형일 것이다. 뇌에는 좌반구와 우반구가 있고, 일부 기능은 좌뇌 또는 우뇌에 편중되어 있는 것은 사실이다. 하지만 ‘창의적인 사람은 어느 쪽 뇌가 우세하다’거나 ‘어느 한쪽 뇌 위주의 사고를 하는 사람이 더 직관적’이라는 등의 주장은 과학적인 근거가 없다. 실제로 미국 유타대학 연구진이 2013년 기능적 자기공명영상으로 1000여명의 뇌를 조사한 결과에서는 이른바 ‘좌뇌형’과 ‘우뇌형’ 활성화 패턴이 따로 존재하지 않는 것으로 나타났다. 그런데도 사람들의 뇌를 존재하지 않는 좌뇌형-우뇌형으로 나눈다면, ‘나는 한쪽 뇌가 더 우세하니 덜 창의적이야’라거나 ‘나는 이쪽 뇌가 우세하니 감성적인 면이 강하고 분석적인 면은 약해’라며 지레짐작으로 자신의 가능성을 제한해버릴 위험이 있다. 또 다른 널리 알려진 학습법으로 ‘시각형-청각형-신체감각형’ 학습 유형이 있다. 이름 그대로 시각형 학습자는 시각자료로 공부했을 때, 청각형 학습자는 정보를 소리로 들었을 때, 신체감각형은 몸을 움직여 경험했을 때 더 잘 배울 수 있고, 그래서 각자 자신이 선호하는 유형으로 공부하는 게 더 효율적이라는 것이다. 언뜻 그럴듯해 보이지만 샌디에이고 캘리포니아대학의 해럴드 패슐러 교수가 2008년에 이런 학습 유형에 대한 기존의 연구 결과들을 검토했더니, 선호하는 유형에 맞춰 공부하더라도 학습효과가 좋아지지 않는다는 결과가 더 많았다고 한다. 사람마다 시각이나 청각, 신체감각 정보 중 특정 유형을 다른 유형보다 선호할 수는 있다. 또한 어떤 정보는 특정 유형으로 제시될 때 이해하기도 쉽고 기억하기도 쉽다. 그러나 둘 사이에 뚜렷한 상관관계는 없었다. 시각형 정보를 더 좋아하는 사람은 있을 수 있지만, 그렇다고 그 사람이 늘 시각적으로 공부했을 때 학습 효율이 특별히 더 높지는 않았다는 것이다. 이렇게 보면, 내가 어떤 유형의 정보를 선호하는가보다는 배워야 할 내용이 어떤 유형에 적합한가가 더 중요하다. 예를 들어 내가 시각보다 청각을 선호한다고 하더라도 ‘뇌의 구조’를 배운다면 ‘청각적’으로 설명을 듣는 것보다 ‘시각적’으로 직접 각 뇌 영역의 위치를 보는 것이 더 효과적일 것이다. 영어 단어를 어떻게 발음하는지 배우기 위해서 발음기호를 ‘시각’으로 볼 수도 있겠지만 ‘청각’으로 듣고, ‘신체감각’으로 직접 발음해 보는 게 훨씬 낫다. 과학적으로 검증된 완벽한 공부법을 연구자들이 언젠가 찾아낼지도 모르겠다. 하지만 현재로선 여러 연구에서 검증된 효과적 학습법은 생각보다 평범하다. 주의 깊게 공부하고, 배운 내용을 시험해 보고, 적절한 수면을 취하는 게 좋다. 유산소 운동도 기억을 향상시키는 데 효과가 크다.(6월15일치 ‘운동하면 기억력이 좋아진다’) 마치 과일과 채소를 많이 먹고 운동을 열심히 하면 건강에 좋다는 말처럼 뻔한 얘기처럼 들릴 것이다. 하지만 방법을 안다고 해서 모두가 건강해지고, 모두가 효과적으로 공부하게 되진 않는다. 나 역시 ‘기억 인출 연습’을 하면 기억을 더 잘할 수 있다는 것을 알면서도 나중에 다시 찾아보면 그만이라는 생각에 그 연습을 소홀히 해, 애써 공부한 자료를 다반사로 잊어버린다. 운동과 잠이 중요하다는 글을 쓰는 지금도 졸린 눈을 비비며 거북목을 한 채 몇시간째 자리에서 움직이지 않고 있다. 아는 것과 실천하는 것은 다른 문제다. 정 수근 한국뇌연구원 선임연구원(심리학) [ⓒ한겨레신문 : 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">카카오톡과 라이언, 나이키와 달린다 </t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>톡비즈 솔루션과 카카오 '인기 IP' 라이언, 글로벌 브랜드와 첫 협업 카카오톡 배너 클릭하면 광고영상, 톡으로 간편가입서비스 달리는 라이언 아이템도 제공   카카오가 나이키 코리아와 손잡고 카카오톡과 인기 지적재산권(IP)인 라이언과 공동 마케팅을 진행한다고 24일 밝혔다. 이번 마케팅은 4600만 이용자가 있는 국민 메신저 플랫폼 카카오톡과 카카오 콘텐츠, 글로벌 브랜드와 새로운 협업을 시도한 사례다. 카카오톡이 지난 2·4분기에 베타서비스로 선보인 톡보드 최상단 배너를 클릭하면 #탭의 브랜드탭을 통해 라이언과 박나래의 유쾌한 광고 영상을 만날 수 있다. 또 카카오톡 간편가입 서비스를 통해 나이키 제품을 쉽게 볼 수 있는 이용자 동선을 마련했다. 아울러 카카오 계정으로 나이키닷컴에 로그인하면 선착순으로 한정판 이모티콘을 받을 수 있다. '조이런 마블 게임' 참여자에게는 카카오프렌즈 홍대 플래그십 스토어 지하 체험 공간 초대권도 제공한다. 아울러 카카오톡 프로필에서 '달리는 라이언' 스티커와 배경화면 등 프로필 아이템이 무료로 제공된다. 카카오 오프라인 접점을 통한 마케팅도 선보인다. 나이키 조이라이드 이노베이션과 디지털 인터랙티브 게임 등 다양한 경험을 할 수 있는 제품 체험 공간이 카카오프렌즈 홍대 플래그십 스토어 지하에 마련됐다. 이와 함께 한정판 카카오프렌즈 제품도 8월 말부터 강남, 홍대, 부산 카카오프렌즈 플래그십스토어와 DDP점, 카카오프렌즈 온라인몰에서 만나볼 수 있다. 카카오 관계자는 "이번 나이키 코리아와 협업은 카카오톡의 접근성과 인기 캐릭터 라이언의 친숙함을 기반으로 이용자에게 차별화된 가치와 경험을 제공하고자 한 것"이라며 "앞으로도 카카오 자산을 활용한 다양한 형태의 브랜드 간 협업을 이어갈 계획"이라고 말했다. gogosing@fnnews.com 박소현 기자 ※ 저작권자 ⓒ 파이낸셜뉴스. 무단 전재-재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>트럼프, 지소미아 종료 첫 언급.."무슨 일 있을 지 지켜보겠다"</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>23일 G7 참석차 출국 전 기자단과 질의응답 "문 대통령도 나의 좋은 친구..한국 지켜보자" "북한과 좋은 관계..김정은 내게 매우 솔직해" [이데일리 김혜미 기자] 도널드 트럼프 미국 대통령이 ‘한일군사정보보호협정(GSOMIA·지소미아) 종료 결정과 관련해 “앞으로 무슨 일이 있을 지 지켜볼 것(We’re going to see what happens)”이라고 말했다. 지소미아 종료에 대한 첫 공식 발언이다. 23일(현지시간) 미 의회방송 C-SPAN에 따르면 트럼프 대통령은 주요 7개국(G7) 정상회의 참석차 프랑스로 출발하기 전 기자들과 만난 자리에서 “한국의 지소미아 종료 결정을 우려하는가”라는 질문에 “앞으로 무슨 일이 일어날 지 지켜볼 것이다. 문(재인) 대통령 역시 나의 좋은 친구다. 한국에 무슨 일이 일어날지 지켜보자”고 언급했다. 이는 앞서 미 국무부가 지소미아 종료에 대해 ‘실망했다’는 입장을 보인 것과 다소 차이를 보인 것이다. 마이크 폼페이오 미 국무장관은 지난 22일 “한국이 정보공유 합의에 대해 내린 결정에 실망했다”며 “한국과 일본이 대화를 통해 ‘옳은 곳’으로 관계를 되돌리기 바란다”고 언급한 바 있다. 이에 따라 추후 미 정부의 정책 기조가 달라질 수 있을 지 주목된다. 트럼프 대통령은 이날 아베 신조 일본 총리에 대해서도 “아주 좋은 친구”라며 G7 회의에서 만남을 기대하고 있다고 밝혔다. 같은 자리에서 트럼프 대통령은 김정은 북한 국무위원장에 대해서도 “좋은 친구”라고 언급해 눈길을 끌었다. 한미 연합군사훈련이 종료된 20일 이후인 24일(한국시각) 오전 북한이 탄도미사일로 추정되는 발사체 2발을 동해상으로 발사했다는 소식이 전해진 뒤에도 크게 개의치 않는 모습이다. 트럼프 대통령은 이날 “미국 정부는 북한과 매우 좋은 관계를 맺고 있다. 김정은 북한 국무위원장이 지금까지 나에게 아주 솔직했다고 생각한다”며 “김정은 위원장은 미사일 테스트를 좋아한다. 양측은 단거리 미사일 제한에 합의한 적이 없다. 무슨 일이 일어나는지 지켜볼 것”이라고 말했다. 이는 북한의 미사일 발사에 대한 미국의 태도가 크게 달라지지 않을 것임을 시사하는 것으로 해석된다. 폼페이오 미 국무장관은 최근 미국의소리(VOA) 인터뷰에서 “우리가 가장 크게 신경쓰는 것은 장거리 미사일 시험”이라면서 “김정은 위원장이 비핵화에 전념하고 있고, 그가 이를 실행할 수 있도록 방법을 찾고 있다는 데 희망을 두고 있다”고 언급한 바 있다. 도널드 트럼프 미국 대통령. 사진 : 뉴시스 김혜미 (pinnster@edaily.co.kr) 네이버 홈에서 ‘이데일리’ 뉴스 꿀잼가득 , 청춘뉘우스~ ＜ⓒ종합 경제정보 미디어 이데일리 - 무단전재 &amp;amp; 재배포 금지＞</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>배터리 핵심광물 '코발트 가격' 2주 만에 20% 급등</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>글렌코어 무탄다 구리 코발트 광산. (사진=글렌코어) 배터리 핵심 원재료 광물인 코발트 가격이 세계 최대 공급업체의 감산 발표로 2주 만에 20% 이상 상승했다. 런던금속거래소(LME)에서 이달 초 톤당 2만5000달러에 거래되던 코발트 가격은 22% 올라 22일(현지시간) 현재 톤당 3만500달러를 유지하고 있다. 최근 코발트 가격 급등은 세계 최대 광산업체인 글렌코어가 최대 코발트 산지인 콩고민주공화국 내 무탄다 광산 운영을 2021년까지 중단하겠다고 발표했기 때문이다. 무탄다 광산은 세계 최대 코발트 광산 중 하나로 전 세계 코발트 생산량의 약 20% 담당하고 있다는 점을 감안하면 시장에 미치는 파급력이 크다. 글렌코어가 광산 가동 중단을 결정한 이유는 코발트 가격 하락에 따른 경제성 악화 때문이다. 지난해 3월 톤당 최고 9만5500달러까지 치솟았던 코발트 가격은 올해 톤당 2만달러대로 급락했다. 세계 최대 코발트 정련업체인 화유코발트 역시 코발트 가격 폭락으로 최근 콩고민주공화국 소재 코발트 광산에 대한 6630만달러 규모 투자 철회를 결정했다. 코발트는 전기차용 리튬이온 배터리 양극재를 만드는데 필수 원재료 가운데 하나다. 전기차 시장 확대에 대한 기대감으로 지난해 가격이 300% 이상 급등하면서 신규 광산 프로젝트가 다수 시작됐다. 하지만 이후 공급 과잉 등 영향으로 가격이 폭락하면서 경제성이 악화되면서 신규 프로젝트가 줄줄이 취소되는 상황이다. 역설적으로 전문가들은 신규 프로젝트 중단에 따른 공급 감소 영향으로 안정되던 코발트 가격이 수년내 다시 상승할 가능성이 높다고 전망하고 있다. 여기에 전기차 시장이 본격 확대되며 수요가 급증할 것으로 예상돼 리튬, 코발트, 니켈 등 주요 원재료 가격이 장기적으로는 상승할 가능성이 높다는 전망이다. 영국 캐피탈이코노믹스는 최근 보고서에서 지난 2015년 아연 시장에서 글렌코어가 비슷한 조치를 취하면서 아연 가격이 3년내 2배가량 상승했던 사실을 언급하며 “이번 광산 가동 중단으로 내년 말까지 코발트 가격이 톤당 4만달러에 도달하고 2021년 말에는 5만달러대로 추가 상승할 것”이라고 내다봤다. 원재료 가격이 오르면 LG화학, 삼성SDI, SK이노베이션 등 배터리 업체에는 원가 부담으로 작용. 반대로 에코프로비엠, 엘앤에프, 포스코케미칼, 코스모신소재 등 양극재 제조사에게는 매출 확대 요소가 된다. 정현정 배터리/부품 전문기자 iam@etnews.com [Copyright ⓒ 전자신문 &amp;amp; 전자신문인터넷, 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>서울서 3,000대 우버택시 달린다...韓 공략 속도 높이는 우버</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>■ 택시호출 적극 마케팅 막강한 자금력 앞세워 파격 서비스 서울서 우버택시 3,000대로 늘어 ■ 택시·스타트업과 협업 택시조합과 플랫폼택시 협의나서 코리아스타트업포럼 특별회원 가입 [서울경제] 지난 2013년 승차공유 ‘우버 엑스(X)’로 국내 진출을 위한 문을 두드렸다가 좌절을 맛본 우버가 6년 만에 한국 모빌리티 시장에서 기지개를 펴고 있다. 올해 4월 서울에서 시작한 택시 호출 서비스가 빠르게 확대되고 있는데다 택시 조합·스타트업과의 협업도 시동을 걸고 있는 상황이다. 업계에선 국토교통부의 ‘혁신성장과 상생발전을 위한 택시제도 개편방안(상생안)’의 세부 내용이 확정돼 국내 모빌리티 시장의 불확실성이 사라지면 우버의 사업확대가 본격화될 것으로 전망한다. ◇마케팅 총공세에 우버택시 3,000대로 늘어 = 현재 우버가 국내에서 가장 공을 들이는 사업은 택시호출 서비스 ‘우버택시’다. 지난 4월 처음 출시됐을 때만 하더라도 우버택시를 불러도 잡기 힘들다는 평가가 나왔지만 최근엔 3,000대까지 규모를 확대했다. 3,000대는 모두 개인택시 기사들이며 아직 법인택시와의 협업은 시작하지 않았다. 택시 업계의 강한 반발을 불어왔던 승차공유 ‘우버X’와 달리 우버택시는 우버 플랫폼에서 택시를 부를 수 있도록 중개하는 서비스이기 때문에 택시기사들도 긍정적인 평가를 내리고 있다. 우버가 빠르게 택시기사들을 끌어들일 수 있었던 배경은 적극적인 마케팅에 있다. 택시기사들은 우버택시를 시작할 때와 일정 횟수씩 우버 앱의 콜을 수락할 때마다 우버로부터 일정 금액을 받을 수 있다. 우버택시를 운행하는 한 택시기사는 “주변 택시기사들이 소개를 해줘 우버택시를 시작하게 됐다”라며 “카카오T와 티맵도 함께 하고 있지만 최근엔 우버쪽의 콜도 자주 받는 편”이라고 밝혔다. 이용자들을 대상으로 한 마케팅도 활발하게 이뤄지고 있다. 지난 4월 출시부터 현재까지 4개월이 넘는 기간 동안 우버택시를 처음 이용하면 운임의 50%, 이후부터는 탈 때마다 운임의 20%씩 할인 혜택을 제공 중이다. ◇택시조합·스타트업 협업 위해 문 두드려 = 우버가 국내에서 펼치는 모빌리티 서비스는 앞으로 계속 확장할 것으로 보인다. 이미 우버는 지난달 서울개인택시운송조합에 플랫폼 택시 파트너사 선정을 위한 제안서를 제출한 뒤 함께 협의를 진행하고 있다. 서울개인택시조합 관계자는 “우버에서 택시 호출쪽도 프로모션을 제시하며 노력하고 있고 여러 유형으로 (사업을) 하기 위해 서로 입장을 전달한 상황”이라고 전했다. 서울개인택시조합은 우버 등 모빌리티 업체들과 협업을 통해 오는 11~12월경 5,000명 규모의 플랫폼 택시를 3~4개 출범시키는 방향을 고심 중인 것으로 알려졌다. 만약 우버가 서울개인택시조합과 플랫폼 택시를 출범하게 되면 중개 서비스를 넘어 ‘우버’ 브랜드를 디자인 등에 내걸 수 있는 가맹 서비스까지 확장하게 되는 셈이다. 스타트업과의 접점을 늘리기 위해 최근엔 코리아스타트업포럼에 특별회원으로 가입하기도 했다. 코리아스타트업포럼은 우아한형제들·비바리퍼블리카 등 유니콘(기업 가치 1조원 이상 비상장기업) 기업부터 스타트업까지 1,000여개 기업들이 가입돼있는 국내 스타트업 대표 단체다. 우버는 스타트업을 지원하고 공동기획 사업 등을 추진할 수 있는 특별회원 자격이다. ◇택시부터 음식까지 ‘카풀’ 빼고 다해 = 우버는 현재 호출 서비스인 우버택시 이외에도 외국인용 택시 ‘인터내셔널 택시’와 고급 택시 서비스 ‘우버블랙’, 교통 약자를 지원하는 ‘우버 어시스트’ 등을 운영하고 있다. 이밖에 음식 배달 서비스인 ‘우버이츠’도 출범 2주년을 맞기도 했다. 다만 다양한 사업에 더해 택시를 기반으로 한 서비스 확대까지 모색하고 있지만 막상 본래 서비스인 승차공유는 다시 운행하기 어려울 것으로 보인다. 국내에선 카풀(승차공유)을 출퇴근 2시간으로만 제한하는 법안이 마련되면서 카풀 업체들이 어려움을 겪고 있다. 토종 모빌리티 업체들을 위협하는 글로벌 업체라는 인식도 극복해야 할 요소다. 실제로 국내 모빌리티 스타트업들은 정부의 상생안 마련 이후 우버가 막대한 자금력으로 시장을 장악할 수 있다는 우려를 제기하고 있다. 한 모빌리티 업체 관계자는 “상생안이 오히려 규제의 불확실성을 없애주면서 자금력이 있는 우버가 적극적으로 움직이고 있다”라며 “스타트업 입장에선 대기업들이 주도하는 판에 끼어들어가기 어려운 환경”이라고 말했다. /권경원기자 nahere@sedaily.com | 저작권자 ⓒ 서울경제, 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>[WiFi카페] 먹방이 바꾼 치킨·피자…"튀어야 알려진다"</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>소비자 호기심 자극하기 위한 이색 메뉴 선봬 주머니 사정 넉넉지 못한 중견·중소업체 중심 '활발' 협찬방송과 순수 리뷰 방송 간 구분 필요 [이데일리 김유성 기자] ‘호기심을 자극해 자연스러운 입소문이 나도록 하라.’ 유튜브의 대중화, 먹방의 발달은 식품업계 광고·마케팅 방식을 바꾸고 있습니다. TV 등을 통해 일방적으로 광고 영상을 전달하기보다, 사용자 스스로가 영상 콘텐츠를 만들고 입소문이 나도록 하는 식입니다. 바이럴(입소문)만 잘되면 큰 비용 들이지 않고도 제품을 알릴 수 있죠. 삼양식품의 불닭볶음면이 대표적인 예입니다. 이 라면은 매운맛이 특징인 덕분에 여러 화제를 낳았습니다. 매운맛 좋아하는 한국인도 도전하게끔 만드는 라면이었죠. 불닭볶음면을 먹은 외국인들의 반응도 콘텐츠가 됐습니다. 불닭볶음면은 단일 라면 브랜드로는 어느새 국내 최대 수출 라면이 됐습니다. 외식 업계도 이런 바이럴 마케팅이 유행하고 있습니다. 상반된 재료를 쓴 음식 메뉴를 개발하거나 극단적으로 맵거나 짠 음식으로 소비자들의 호기심을 자아내는 식입니다. 특히나 대중적인 메뉴인 치킨과 피자 업계에서 이런 경향이 두드러지고 있습니다. 마케팅 주머니 사정이 넉넉하지 못한 중견·중소기업일수록 이런 마케팅에 더 의존할 수 밖에 없습니다. 페리카나 누꼬진짬뽕 리뷰 영상 채널 모음 캡처 그래서 몇 개 업체를 추려봤습니다. 홍보 업계에서 회자되는 기업들입니다. 저랑 해당 기업 내부 마케팅 담당자들과는 일면식이 없다는 점 알려드립니다. 1982년 문을 연 국내 원조급 치킨 프랜차이즈 페리카나는 진한 해물맛 소스를 치킨과 어울리도록 한 ‘누꼬진짬뽕’을 선보였습니다. 치킨과 함께 진한 국물의 짬뽕을 같이 먹는 메뉴입니다. 참고로 페리카나는 치킨 CF 원조 기업이기도 합니다. 개그맨 최양락 씨가 광고하던 1980년대 후반에는 꽤 인기를 끌었죠. 1990년대 비슷비슷한 업체들이 많이 나오다보니 2000년대 들어 고만고만한 치킨 프랜차이즈로 가라앉았고요. 누꼬진짬뽕은 짬뽕을 치킨과 함께 먹는다는 콘셉트입니다. 몇몇 먹방 유튜버가 소개하면서 화제가 되기도 했고요. 치킨과 짬뽕의 부조화 때문일까요, 호평과 혹평이 오가고 있습니다. 모든 조합이 환영받는 것은 아니죠. 치킨에 과자를 얹어 먹는 제품도 나왔습니다. 치킨에 붙는 땅콩 부스러기처럼 과자 토핑이 올라간 제품입니다. 맘스터치가 만든 ‘매콤소이팝’입니다. 과자 제조업체 오리온과 함께 ‘치킨팝 땡초찜닭맛’ 과자가 토핑처럼 올라가 있습니다. 누꼬진짬뽕보다는 긍정적인 의견은 많아 보입니다. 김치와 치킨을 조합한 치킨도 있습니다. 멕시카나치킨인데요, 멕시카나도 지금은 중견 기업 정도지만, 1990년대 국내 치킨 업계를 풍미했습니다. 선두 업체들과 비교해 대규모 마케팅을 한다거나 TV CF를 하기에는 무리죠. 멕시카나치킨은 김치를 조합했습니다. 대상의 김치 브랜드 ‘종가집’과 협업해 김치를 소스로 한 ‘미스터 김치킨’을 출시했습니다. 후라이드 치킨에 볶음 김치 맛을 양념으로 해서 새콤달콤한 맛을 냈습니다. 멕시카나는 앞서 언급한 페리카나와 맘스터치보다는 비용을 더 들인듯 합니다. 유명 먹방 유튜버 ‘밴쯔’를 섭외해 리뷰 영상을 제작한 덕분이죠. 비용대비 효과는 좋아 보입니다. 김치킨 등 멕시카나 치킨 메뉴를 리뷰하는 먹방 유튜버 벤쯔 (유튜브 캡처) 불닭 소스를 입힌 피자도 나왔습니다. 불닭볶음면의 유명세가 피자로까지 확장된 셈입니다. 파파존스의 붉닭 피자는 ‘불닭 핫 치킨 바베큐’와 ‘붉닭 크림치즈 소스’ 2종으로 구성됐습니다. 파파존스 전 제품을 통틀어 가장 매운 맛입니다. 시즌 한정 메뉴로 출시됐던 불닭피자는 소비자들의 요청에 따라 정식 메뉴가 됐습니다. 토종 피자 프랜차이즈 피자마루는 피자와 떡볶이를 같이 먹는 메뉴를 출시했습니다. 피자 위에 떡볶이를 부어 먹거나, 피자를 떡볶이 소스에 찍어 먹는 식입니다. 식품 업계에서는 음식 유행 주기가 점점 짧아지고 있다고 전합니다. 큰 비용을 광고와 홍보에 들이기에는 망설일 수 밖에 없습니다. 자금 사정이 넉넉지 못한 면도 크고요. 그래서 이들 업체들이 선택한 게 유튜브나 소셜미디어이고 바이럴입니다. 다만 반짝 이슈에 그치지 않게 하려면 소비자들이 직접 콘텐츠를 만들게 해야 합니다. 소비자들이 먹으면서 재미있게 영상을 만들어 올릴 수 있는 마당을 마련해주는 것이지요. 앞으로도 이런 경향은 더 강해질 것으로 보입니다. 먹방은 비용을 이유로 TV나 신문 등 전통 매체에서 소외됐던 중견·중소 식품기업들 입장에서 마케팅의 장이 됩니다. 주시청자들이 먹을 것에 관심 많은 젊은 층들이기 때문이겠죠. 그러나 먹방에 있어 광고·협찬을 받고 찍는 영상인지, 순수 리뷰 영상인지는 구분해줄 필요가 있습니다. 그래야 순수하게 리뷰를 하면서 소비자들에게 정보를 주는 먹방 콘텐츠가 빛을 발할 수 있겠죠. 그 순수성이 신뢰를 얻을 때 콘텐츠는 지속력을 갖게 됩니다. 지금의 먹방이 제품 알리기에는 좋아 보입니다만, 소비자들의 신뢰를 얻을만큼의 노력이 전제돼 있을까요? 여러분은 어떻게 생각하시나요? 김유성 (kys401@edaily.co.kr) 네이버 홈에서 ‘이데일리’ 뉴스 꿀잼가득 , 청춘뉘우스~ ＜ⓒ종합 경제정보 미디어 이데일리 - 무단전재 &amp;amp; 재배포 금지＞</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>같은 약 6社가 복제…바이오시밀러 경쟁 격화</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>국내 바이오·제약사 잇따라 황반변성 시밀러 개발나서 퍼스트무버 지위 확보위해 출혈경쟁·수익성 악화 우려 중간에 기술 수출 나서거나 바이오베터로 차별화 필요 국내 기업 간 바이오시밀러(바이오의약품 복제약) 출시 경쟁이 격화되고 있다. 얼마 전까지만 해도 대기업과 중소 제약사가 개발하는 바이오시밀러가 달랐지만, 이제는 회사 규모와 관계없이 개발 제품이 중복되는 사례가 늘면서 수익성 악화에 대한 우려가 커지고 있다. 업계 관계자는 "바이오시밀러가 오리지널 못지않게 약효를 인정받으면서 국내외 기업들이 대거 바이오시밀러 시장에 뛰어들고 있다"며 "특히 블록버스터급 오리지널 약을 바이오시밀러로 개발하는 데 국내 기업 간 경쟁이 치열해지고 있다"고 최근 바이오시밀러 시장 분위기를 전했다. 국내 기업의 참여가 많은 바이오시밀러 분야 중 하나는 시력장애를 동반한 고령화 질환인 황반변성 치료제다. 오리지널 약인 독일 바이엘 '아일리아'와 스위스 노바티스 '루센티스'를 복제한 바이오시밀러 시장을 잡기 위해 국내 5~6개 업체가 뛰어들었다. 시장조사 기관인 아이큐비아 등에 따르면 지난해 전 세계적으로 아일리아와 루센티스 판매액은 각각 8조원, 4조원에 달했다. 내년 물질특허 만료를 앞둔 루센티스에 대한 바이오시밀러 개발에는 삼성바이오에피스를 비롯해 종근당, 일동제약 등이 뛰어들었다. 아일리아의 바이오시밀러에는 알테오젠과 삼천당제약이 도전장을 냈다. 삼성바이오에피스는 이미 루센티스의 바이오시밀러 제품 'SB11'에 대해 글로벌 임상 3상을 진행 중이다. 제약사 중에서 바이오시밀러 사업이 활발한 종근당도 'CKD-701'이란 바이오시밀러 제품에 대해 서울대병원, 삼성서울병원 등 25곳에서 국내 임상 3상을 진행하고 있다. 일동제약도 노인성 황반변성 치료제로 쓰일 바이오시밀러 'IDB0062'를 개발하고 있다. 아일리아 쪽은 알테오젠이 국내에서 임상 1상을 하고 있고, 전임상 단계인 삼천당제약은 지난 4월 유럽의약품청(EMA)으로부터 글로벌 임상을 위한 최종 검토의견서를 수령했다. 아일리아의 물질특허는 일본 미국 유럽에서 2022~2025년 종료되지만, 물질을 안정화시키는 제형과 제제에 대한 특허가 남아 있어 아일리아 바이오시밀러는 2027~2030년이 돼야 출시될 것으로 보인다. 알테오젠 관계자는 "아일리아 관련 특허 장벽이 높고 해외 제약사들도 바이오시밀러 개발에 나서고 있어 경쟁이 센 편"이라며 "판매도 10년이 지나야 가능한 만큼 임상 3상 단계에서 기술 수출을 진행할 것"이라고 밝혔다. 희귀 질환 치료제인 '솔리리스'의 바이오시밀러는 전 세계에서 3곳이 개발하고 있는데, 이 중 2곳이 국내 업체다. 솔리리스는 미국 제약사 알렉시온이 만든 발작성 야간 혈색소뇨증(PNH) 치료제로 지난해 전 세계적으로 35억6300만달러( 약4조3000억원)의 매출을 올렸다. 국내에서는 삼성바이오에피스가 지난 3월 'SB12'란 프로젝트로 글로벌 임상 1상을 마쳤고 임상 3상에 들어갔다. 경쟁사는 같은 임상 3상 단계에 있는 글로벌 제약사 암젠 외에 국내 기업인 이수앱지스가 있다. 이수앱지스는 호주와 뉴질랜드에서 진행하고 있는 임상 1상을 연내 완료한 뒤 내년부터 임상 3상에 진입할 계획이다. 이수앱지스 관계자는 "정상적인 임상 진행과 함께 해외 기업에 기술 수출을 하는 것도 추진 중"이라고 밝혔다. 지난해 전 세계 매출액이 69억5700만달러(약 8조2000억원)에 달해 전 세계 4위 의약품에 이름을 올린 대장암 치료제 '아바스틴' 바이오시밀러는 삼성바이오에피스가 지난달 중순 유럽에 판매허가를 신청했고, 미국에는 하반기 신청을 예정하고 있다. 셀트리온은 아바스틴의 바이오시밀러인 'CT-P16'에 대해 글로벌 임상 3상을 진행하고 있다. 업계 인사는 "오리지널 바이오의약품 특허 기간이 끝난 뒤 가장 먼저 바이어시밀러 제품을 내놓는 '퍼스트 무버'가 되려면 과거에는 해외 기업 동향만 살피면 됐지만, 이제는 국내 업체들도 경쟁 상대로 부상하고 있다"며 "비용 절감 등을 위해 기술 수출을 하거나 기존 제품에 효능을 추가한 바이오베터를 만드는 등 차별화가 필요하다"고 주문했다. [김병호 기자] [ⓒ 매일경제 &amp;amp; mk.co.kr, 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>국내 연구진, 암세포 공격력 강화 세포치료제 기술 개발</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>한국연구재단은 차의과학대 박경순·박우람·한동근 교수 공동연구팀이 생체재료 기반 나노 기술을 이용, 암세포에 구멍을 내 죽이는 자연살해세포가 암세포를 보다 잘 공격하도록 만드는 세포치료제 제작기술을 개발했다고 25일 밝혔다. 우리 몸에 선천적으로 존재하는 자연살해세포는 바이러스에 감염된 세포나 암세포를 선택적으로 인식한 후 즉각 파괴한다. 다른 면역세포와 달리 면역거부반응이 적어 건강한 사람의 세포를 환자에게 사용할 수 있다. 하지만 자연살해세포의 자체방어기작 때문에 외부에서 인식강화유전자를 도입하기가 쉽지 않다. 바이러스를 이용해 암세포 인식강화 유전자를 자연살해세포 내로 전달하려는 방식은 바이러스를 매개체로 한다는 점에서 안전성 측면에서 다소 불리하다. 차의과학대 연구팀은 바이러스 대신 형광을 띠는 자성 나노입자를 암세포 인식강화 유전자와 함께 전달함으로써 자연살해세포 내로 유전자가 전달되는 효율을 높였다. 고분자 생체재료를 나노입자 위에 겹겹이 쌓는 삼중코팅 방식을 통해 자연살해세포의 자체 방어기작을 회피하도록 설계했다. 나노입자의 도움으로 자연살해세포 표면에 암세포 인식강화 단백질이 정상적으로 만들어지는 것과 악성유방암세포벽에 구멍을 내 파괴하는 능력이 향상된 것을 확인했다. 과학기술정보통신부·한국연구재단 개인기초연구 사업과 보건복지부 연구중심병원육성과제 지원으로 수행된 연구 성과는 국제학술지 '바이오머티리얼스‘에 이번달 9일 게재됐다. 박경순 교수는 "차세대 항암면역세포로 주목받는 자연살해세포를 자유자재로 엔지니어링할 수 있는 기술을 개발했다"고 설명했다. [설성인 기자 seol@chosunbiz.com] chosunbiz.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>KT, “갤노트10+ 배터리 이용시간 4시간21분 증가”</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>[디지털데일리 최민지기자] KT 이용자는 5G 배터리 절감 기술(C-DRX)로 삼성전자 ‘갤럭시노트10플러스’를 4시간21분 더 사용할 수 있다. KT(대표 황창규)는 서울·수도권, 강원, 부산, 울산, 경남 등에 우선적으로 5G C-DRX 기술을 적용한 데 이어 8월1일 기준 전국망 확대 적용을 완료했다고 25일 밝혔다. 한국정보통신기술협회(TTA)가 갤럭시노트10플러스로 5G C-DRX 기술 적용 전후 배터리 사용시간을 테스트한 결과, 사용시간이 최대 4시간21분 증가한 것으로 확인됐다. 동일한 환경에서 같은 서비스를 이용해 배터리 소모 시간을 측정했는데, C-DRX를 도입했을 때 배터리가 최대 11시간4분, 최소 10시간24분간 지속한 반면 C-DRX를 탑재하지 않은 경우 최대 6시간57분, 최소 6시간43분간 동작했다. 이는 배터리 사용시간이 약 65% 증가한 것으로 ‘갤럭시S10 5G’에 C-DRX를 적용했을 때보다 4% 가량 효과가 늘어난 결과다. KT 네트워크연구기술지원단장 이수길 상무는 “KT는 LTE에 이어 5G에서도 가장 먼저 C-DRX 기술을 전국 확대 적용해 전국 어디서나 고객들이 배터리 절감효과를 누릴 수 있게 됐다”고 말했다. &amp;lt;최민지 기자&amp;gt;cmj@ddaily.co.kr &amp;lt;저작권자 © 디지털데일리 무단전재-재배포금지&amp;gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>[주말N수학]피보나치도 울고 갈 파인애플 볶음밥</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>열대과일 파인애플에 피보나치 수열이 숨어 있다.게티이미지뱅크 달콤새콤한 열대과일 파인애플에도 피보나치 수열이 숨어있습니다. 피보나치 수열은 이탈리아 수학자 레오나르도 피보나치의 이름을 딴 수열입니다. 1, 1, 2, 3, 5, 8, 13, 21, 34, 55, 89, 144…처럼 두 개의 1로 시작해서 연이은 두 수를 더해 다음 항을 만드는 수열입니다. 피보나치의 이름을 따르긴 했지만, 피보나치 수열을 처음 생각해낸 건 피보나치가 아닙니다. 피보나치 수열이 처음 문헌에 등장한 건 기원전 5세기 인도 수학자 핑갈라의 책에서였고, 그보다 훨씬 전부터 쓰였을 가능성이 높습니다. 하지만 피보나치가 자신의 책 ‘산술의 서’ 12장에서 토끼 번식에 관한 문제로 피보나치 수를 설명하면서 유명세를 타서 피보나치 수열이라 불리게 되었습니다. 피보나치 수열은 매우 간단하지만 수학 전반에 걸쳐 등장하는 중요한 개념입니다. 기하학, 대수학, 정수론 등 다양한 수학 분야에서 쓰일 뿐 아니라, 자연 속에서도 아주 쉽게 발견할 수 있습니다. 해바라기, 솔방울, 나뭇가지 배열, 수벌의 가계도 등 자연의 모습이나 식물의 생장을 설명할 때 피보나치 수열은 빼놓을 수 없습니다. 파인애플 역시 그 예시 중 하나입니다. 파인애플 껍질은 육각형 알맹이들이 서로 다른 3종류의 나선 방향으로 얽혀 이뤄져 있습니다. 피보나치 수열은 이 나선의 개수에서 찾을 수 있습니다. 같은 방향의 나선의 수가 꼭 5, 8, 13, 21 같은 피보나치 수가 되기 때문입니다. 아래 그림처럼 전체 껍질을 펼쳤을 때, 같은 육각형 알맹이를 기준으로 ①번 방향 나선은 5줄이 나오고, ②번 방향 나선은 8줄, ③번 방향 나선은 13줄이 나옵니다. 수학동아 제공 이런 특징은 다른 식물에서도 관찰할 수 있습니다. 솔방울 역시 나선으로 이뤄져 있는데, 각 방향을 따라 생성된 나선의 개수는 대부분 연속한 피보나치 수고, 해바라기 씨의 나선도 피보나치 수를 따릅니다. 식물의 나선뿐만 아니라 꽃잎의 수나 잎사귀의 배열에서도 피보나치 수열을 발견할 수 있습니다. 식물의 줄기에 붙어있는 잎의 배열을 살펴봅시다. 한 줄기의 가장 낮은 위치에 있는 잎사귀에서 관찰을 시작합니다. 첫 번째 잎에서 시작해 줄기를 기준으로 회전하며 올라가 이 잎사귀와 완전히 똑같은 방향에 있는 잎사귀를 찾을 때까지 개수를 세는 겁니다. 그러면 신기하게도 같은 방향에 있는 잎사귀에 도착할 때까지 회전한 횟수가 피보나치 수가 되고 이 두 잎 사이의 잎사귀 개수 역시 피보나치 수가 됩니다! 특히 야자수에서 이와 같은 피보나치 수열을 흔히 발견할 수 있습니다. 수학동아 제공 식물의 생장 비밀은 '피보나치 수열' 이 정도면 식물들이 그야말로 피보나치 수열을 바탕으로 자라고 있다고 말할 수 있겠습니다. 그러면 왜 이런 현상이 나타나는 걸까요? 식물 생장의 비밀을 찾기 위해 수학자, 식물학자 등 많은 사람이 연구를 해오고 있지만 아직 확실한 결론을 얻지는 못했습니다. 다만 식물의 씨앗을 고르게 배열하기 위한 최적의 분포가 피보나치 수열을 따르기 때문일 거라 추측하고 있습니다. 너무 중앙에만 몰려 있거나 가장자리로 갈수록 듬성듬성해지면 생장과 번식에 효율적이지 못하기 때문입니다. 알프레드 포사멘티어 미국 뉴욕시립대 수학교육과 교수와 잉그마 레만 독일 베를린 훔볼트대 수학과 교수는 도서 '피보나치 넘버스'에서 "야자수 각각의 잎사귀가 차지하는 공간이 최대한 충분하고 빛을 많이 받게끔 하는 배열과 관련이 있을 것"이라고 추측하며 "오랜 세대를 거치면서 생존에 유리한 방향으로 진화한 것이 아닐까"라고 덧붙였습니다. 이들은 식물의 기하학적 배열에 대한 가장 '괄목할 만한 결과'로 1992년 발표한 프랑스 수리물리학자 스테판 두아디와 이브 쿠더의 논문을 꼽았습니다. 두아디와 쿠더는 컴퓨터 모델링을 이용해 식물의 생장에 작용하는 이론을 발전시켰고, 피보나치 패턴과 관련된 실험을 진행했습니다. 그들은 식물에 숨겨진 황금각(137.5도)을 동역학으로 설명하기도 했습니다. 이 결과는 식물학만으로 설명하기 어려웠던 식물의 배열을 새로운 관점에서 바라보게 했고 이후로도 오랫동안 ‘두아디와 쿠더 방정식’은 식물 생장 연구의 모형으로 쓰였습니다. 식물 생장 패턴까지 포함한 방정식 발견 그런데 최근 두아디와 쿠더의 방정식을 보완한 새로운 방정식이 등장했습니다. 2019년 6월 스기야마 무네타카 일본 도쿄대 교수팀은 두아디와 쿠더의 방정식으로 설명하지 못했던 식물까지 포함하는 변형된 방정식을 발표했습니다. 피보나치 수열을 따르지 않는 식물 종이 어떻게 배열 패턴을 나타내는지 알아낸 것입니다. 상산나무는 기존의 식물 생장 모델로는 배열 패턴을 만들지 못했던 식물입니다. 연구팀은 예외라고 여겨졌던 상산나무 역시 식물 생장 모형을 이용해 나타낼 수 있으리라 생각했고 기존에 쓰이던 모형에 새로운 변수를 추가해 상산나무가 어떻게 자랄지 예측했습니다. 결과는 실제 상산나무의 모습과 일치했습니다. 이 방정식은 상산나무 하나만이 아니라 상산나무와 비슷한 종류의 다른 식물에도 적용할 수 있습니다. 연구를 이끈 스기야마 교수는 “우리의 모형은 잎이 둘러서 나는 모든 주요 식물의 잎사귀 배열 패턴을 생성할 수 있다”며 “또한 다른 자연에서 나타나는 여러 종류의 패턴에도 잘 맞는다”고 새로운 방정식의 우수성을 설명했습니다. 그러나 아직 과제는 남아있습니다. 기하학적 계산을 통해 식물이 어떻게 자랄지 예상할 수는 있지만, 왜 그런 모양으로 자라는지는 여전히 정확히 알지 못하기 때문입니다. 무작위로 자라는 것 같았던 식물들이 아주 정확한 규칙을 지키며 자라고 있다니 정말 놀랍습니다. 관련기사 수학동아 8월호, [수數 셰프의 맛있는 수학] 피보나치도 울고 갈 파인애플 볶음밥 참고자료 알프레드 포사멘티어, 잉그마 레만 ‘피보나치 넘버스’, Takaaki Yonekura ‘Mathematical model studies of the comprehensive generation of major and minor phyllotactic patterns in plants with a predominant focus on orixate phyllotaxis’ [박현선 기자 tempus1218@donga.com]</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>한경연 “日 반·디 소재 R&amp;D 비용, 韓 대비 41배”</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>[디지털데일리 김도현기자] 한국 반도체·디스플레이 핵심 소재·부품 기업의 연구개발(R&amp;amp;D) 지출액이 일본보다 적은 것으로 나타났다. 25일 한국경제연구원(이하 한경연)은 한국과 일본의 소재·부품기업 1만117개사(한국 2787곳, 일본 7330곳)를 분석, 이같은 결과가 나왔다고 밝혔다. 한경연은 “소재 생산기업 5곳 중 3곳 꼴로 일본 기업의 R&amp;amp;D가 한국보다 많았다”며 “부품 업체의 평균 R&amp;amp;D 지출액은 양국 기업이 서로 비슷했다”고 설명했다. 소재부문에서 일본 기업의 평균 R&amp;amp;D 지출액은 한국 기업의 1.6배였다. 세부 품목별로는 1차 금속 5.3배, 섬유 5.1배, 화합물 및 화학제품 3.1배였다. 이 가운데 반도체·디스플레이 화학소재 기업만 분석하면 일본이 한국의 40.9배였다. 부품부문은 다른 양상을 보였다. 일본 기업의 R&amp;amp;D 지출액이 한국의 40%에 불과했다. 반도체 등 전자부품에서 한국 기업의 R&amp;amp;D 지출액이 일본의 8.2배에 달했다. 다만 정밀기기부품은 일본의 평균 R&amp;amp;D 지출액이 한국에 비해 7.0배, 수송기계부품은 2.3배, 전기장비부품은 2.0배 컸다. 한경연은 전자부품 품목에서 반도체 착시효과가 있다고 분석했다. 반도체를 제외할 경우 전체 부품 부문에서 일본 기업이 60% 많다. 유환익 한경연 혁신성장실장은 “한국 소재·부품산업은 반도체 쏠림이 심한 반면 화학, 정밀부품 등 다른 핵심 소재·부품에서 갈 길이 멀다”면서 “꾸준한 R&amp;amp;D 지원과 화평법, 화관법 등 화학물질 관련 규제 및 노동 관련 규제 개선이 필요하다”고 지적했다. &amp;lt;김도현 기자&amp;gt;dobest@ddaily.co.kr &amp;lt;저작권자 © 디지털데일리 무단전재-재배포금지&amp;gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>LG유플러스, KB알뜰폰에 '5G+LTE' 망 공급 확정</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>LG유플러스 CI KB국민은행 CI LG유플러스가 KB국민은행 알뜰폰 'KB알뜰폰'(가칭)에 롱텀에벌루션(LTE)과 5세대(5G) 이동통신 망 공급을 확정했다. KB알뜰폰은 이통사가 알뜰폰에 5G 망을 공급하는 첫 사례일 뿐만 아니라 거대 금융사업자인 KB국민은행의 알뜰폰 시장 진출로 주목받고 있다. 5G 알뜰폰 첫 단말은 10월 출시 예정인 보급형 5G폰 단말 '갤럭시A90 5G'가 유력하게 거론된다. LG유플러스 관계자는 25일 “망 공급을 확정짓고 도매대가 협의가 마무리 절차를 밟고 있다”면서 “다음 달 양측 간 최종 확정 사항을 발표할 것”이라고 말했다. LG유플러스는 알뜰폰 시장 지원과 자사 회선 가입자 확대가 KB알뜰폰 5G 도매 공급 배경이라고 밝혔다. LG유플러스 내부에서도 KB알뜰폰이 단순 알뜰폰이 아니라 금융·통신 혁신 서비스로 적절하다는 공감대가 이뤄진 것으로 알려졌다. KB알뜰폰은 양측 간 요금제, 유통 방식에 대한 논의가 끝난 후 10월께 출시될 것으로 전망된다. LG유플러스 관계자는 “출시 시기와 요금제, 유통 방식은 KB국민은행 의지에 달렸다”면서 “우리는 도매 제공에 따른 전산 개발, 요금제 개발 등을 지원할 것”이라고 밝혔다. KB알뜰폰용 스마트폰으로는 보급형 스마트폰 갤럭시A90뿐만 아니라 기존 갤럭시S10 5G와 갤럭시노트10 시리즈도 거론된다. 보급형 단말뿐만 아니라 플래그십을 위한 프로모션도 준비, 저가나 중고 단말 위주로 형성된 알뜰폰 이미지를 불식시킨다는 전략이다. 과학기술정보통신부는 LG유플러스의 5G 공급 결정에 환영 의사를 표시했다. 과기정통부 관계자는 “이통사가 아닌 다양한 사업자가 알뜰폰 시장에 진출해 여러 서비스를 내놓고 마케팅을 적극 펼친다면 알뜰폰 시장 활성화에도 도움이 될 것”이라면서 “다만 기존 5G 요금제 가격대가 높은 만큼 얼마나 알뜰폰 시장에 적절한 요금이 나와 줄지가 관건”이라고 평가했다. 자료. 게티이미지뱅크 KB알뜰폰이 타 알뜰폰이 공급하는 LTE에 더해 5G 망까지 확보하면 거대 알뜰폰 사업자가 될 공산이 크다. KB알뜰폰은 알뜰폰에 은행·증권·보험 등 계열사 서비스를 연계한 차별화 서비스를 선보일 예정으로, 기존 KB 고객이 통신요금 할인과 인증서·애플리케이션(앱)을 통한 금융 서비스를 동시에 누릴 수 있어 큰 호응이 예상된다. 거대 알뜰폰 사업자 출현에 따른 중소 알뜰폰 사업자 위기를 우려하는 시각도 있다. 지금도 CJ헬로와 이통 자회사인 SK텔링크, KT엠모바일 등이 알뜰폰 가입자 대다수를 차지하고 있기 때문이다. 통신업계 관계자는 “거대 금융사업자가 가세해 5G 요금제를 통해 과도한 가입자 뺏기 등이 진행되면 중소 알뜰폰은 생존이 어려워질 수 있다”고 말했다. 정예린기자 yeslin@etnews.com [Copyright ⓒ 전자신문 &amp;amp; 전자신문인터넷, 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>국내 시스템반도체 설계 업계, 상반기도 '우울'</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>반도체 웨이퍼. &amp;lt;사진=SEMI 코리아&amp;gt; 국내 시스템 반도체 기업 2019년 상반기 영업이익 분석. &amp;lt;전자신문 DB&amp;gt; 국내 시스템반도체 설계 기업들이 상반기 우울한 실적을 기록했다. 중국 업체들의 저가 공세, 미-중 무역분쟁 심화 등으로 규모가 작은 설계 업체들이 버티기 힘들었다는 지적이다. 25일 국내 매출 상위 20개(2018년 기준) 시스템반도체 설계 회사 영업이익 실적을 종합한 결과, 9개 기업이 적자를 기록한 것으로 나타났다. 영업이익이 작년보다 감소한 기업은 11개였다. LG그룹 계열 시스템반도체 회사이자 업계 1위인 실리콘웍스 영업이익은 작년 상반기 136억8600만원에서 41.57% 감소한 79억9600만원을 기록했다. 보급형 메모리 설계 양산으로 지난해 실적 상승세를 기록했던 제주반도체는 올 상반기 14억600만원으로 지난해 같은 기간보다 83.18% 급감했다. 이밖에 아나패스, 크로바하이텍, 아이에이, 픽셀플러스 등 적자 폭은 더욱 늘어난 것으로 나타났다. 시스템반도체 설계 업체들은 반도체 칩 설계를 주로 담당하는 곳이다. IT 기기에 필요한 칩 구조를 설계하면 삼성전자, DB하이텍, 대만 TSMC 등 파운드리에서 칩을 만든다. 설계 업체들은 이 반도체를 스마트폰, TV 제조사들에 공급한다. 사물인터넷(IoT), 인공지능(AI) 시대 개화로 시스템반도체가 각광받고 있지만 국내 기업은 제한된 수요 등으로 고전하고 있다. 특히 올 상반기는 미-중 무역분쟁 장기화로 더욱 고전한 것이라는 분석이다. 업계 관계자는 “지난해 말부터 일어났던 미국과 중국 간 무역 분쟁이 길어지면서 실적에도 적잖은 영향을 줬다”고 전했다. 메모리 시장에서의 더딘 가격 회복세도 범용 메모리를 생산하는 제주반도체에도 악영향을 미친 것으로 풀이된다. 아울러 중국 시스템반도체 업계 확장도 국내 기업의 설자리를 좁게 만들고 있다. 이미 중국에는 1800개 이상 반도체 설계 기업이 있고 이들은 한국의 기술과 비슷하거나 이미 한 수 넘어섰다는 평가다. 중국 구딕스는 네덜란드 시스템반도체 업체 NXP 오디오솔루션 사업부를 인수하는 등 덩치를 키우고 있다. 올해 국내 파운드리 및 시스템반도체 패키징 업체 실적 증가와 공장 '풀가동'은 국내 설계 업체들의 약진이라기보다 중화권 업체들의 수주 증대가 크게 작용했다는 분석이다. 실제 DB하이텍의 2015년 반기 내수 매출은 1715억원으로 전체 매출 60%가량 차지했지만 올 상반기는 734억원으로 내수 매출이 20%에 불과하다. 4년 만에 상황이 뒤집힌 것이다. 업계 관계자는 “국내 파운드리 호황은 삼성전자 시스템LSI사업부와 중화권 물량이 늘어났기 때문으로 보인다”고 전했다. 하반기에도 설계 업체들의 고전은 지속될 것으로 보인다. 한 시스템반도체 업체 대표는 “상반기와 크게 달라지지 않을 것으로 본다”고 말했다. 또 “지난 4월 정부가 발표한 시스템반도체 지원 효과는 시간이 지나야 효과를 볼 수 있을 것”이라고 덧붙였다. 쉽지 않은 상황에서도 실적 증가를 기록한 기업들도 있다. 차량용 반도체 전문 업체인 텔레칩스는 상반기 매출이 34.25% 증가한 35억7100만원을 기록했다. 중국 시장 물량이 증가한 동운아나텍은 지난 2분기 흑자전환으로 작년 동기 대비 83% 증가하면서 적자폭을 크게 줄였다. 강해령기자 kang@etnews.com [Copyright ⓒ 전자신문 &amp;amp; 전자신문인터넷, 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>저녁부터 16시간 굶으면, 정크물질 분해돼 살 빠져</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>식후 12시간 되면 ‘굶는 상황’ 신호 세포 청소 안 될 땐 정크물질 쌓여 신호전달 막아 치매·파킨슨 생겨 ‘아침은 왕, 저녁엔 거지처럼’ 식사 단식 땐 대장 줄기세포도 젊어져 완벽한 효과 보려면 3~4일 굶어야 ━ 김은기의 바이오토크 성인 3명 중 1명이 비만, 즉 체질량지수(BMI) 25 이상이다. 뱃살 줄이는 방법으로 가끔 굶는 소위 ‘간헐적 단식’이 유행이다. 덜 먹으니 체중 주는 건 당연하다. 하지만 단식 진수는 다른 데 있다. 바로 디톡스다. 굶으면 몸에 쌓인 독소가 제거, 회춘한다. 굶는 건 세포 영양분이 떨어지는 악재인데 이게 왜 건강에 호재일까. 어릴 적 기르던 개가 무얼 잘못 먹었는지 토하더니 도통 밥을 안 먹었다. 걱정스러워 이것저것 챙겨주지만 입도 안 댄다. 주위 어른들은 “나으려고 저런다. 놔두어라”고 한다. 이틀 굶은 개는 다시 먹기 시작했다. 굶는 단식이 치유효과가 있는 걸까. 고대 이집트에서는 매년 30일씩 단식으로 몸을 다스렸다. 현대의학 대부 그리스 히포크라테스는 “자연치유력이 최고다. 아플 때 먹는 것은 질병을 키우는 것”이라며 단식을 강조했다. 한두 끼 굶는 것이 건강 증진 효과를 낼까. 최근 과학이 속을 들여다보았다. 답은 ‘그렇다’이다. 가끔 한 끼 굶으면 뱃살은 금방 줄지 않는다. 하지만 몸에서는 금방 정크단백질을 분해하고 새로운 물질을 만든다. 이게 잘되면 줄기세포도 젊어진다. 잘 안되면 치매· 파킨슨·당뇨가 생긴다. 노벨 생리의학상을 받은 자가소화(autophagy), 즉 ‘스스로(auto) 먹어 버리는(phagy)’ 원리다. 이 원리를 알면 어떻게 다이어트를 해야 할지 감이 잡힌다. 핵심은 저녁-아침 사이 긴 공복으로 정크물질을 분해, 리사이클시키는 거다. 1 히포크라테스 “아플 때 먹으면 질병 키워” 한국 외환 위기 당시 다수의 회사는 구조조정에 들어갔다. 회사 내 불필요한 조직을 분해해서 새로운 팀을 만들었다. 음식을 굶는 건 동물들에게는 가장 큰 위협이다. 길어지면 굶어 죽는다. 몸은 어떻게 대응하고 어떤 효과가 날까. 올해 하버드의대 연구진은 굶는 단식이 어떻게 질병(치매·파킨슨)을 예방·치유할 수 있는지 분자수준에서 조사했다. 식사 후 12시간이 지나자 쥐는 ‘굶는 상황’이라는 비상 신호를 발신한다. 이 신호를 받은 세포들은 분주해진다. 모든 물질을 조사해서 불필요한 놈들, 특히 잘못 만들어진 단백질들에게 ‘딱지’를 붙였다. 딱지 붙은 놈들을 전담팀이 트럭에 실어 ‘리사이클 공장’으로 옮겨가 분해한다. 이걸로 다시 정상 단백질을 조립한다. ‘굶는 신호’를 받은 지 5분 만에 시작, 1시간이면 리사이클 과정이 끝난다. 이런 재생작업은 매일 계속된다. 이것이 제대로 안되면 체내에 정크물질이 쌓인다. 알츠하이머 치매나 파킨슨은 정크단백질(베타아밀로이드·타우·알파시누클린)이 신호전달을 막아 생긴다. 올해 캘리포니아대 연구팀은 정크단백질 자체보다도 이놈들을 분해해야 할 리사이클 공장(라이소좀)이 제대로 작동되지 않아 치매가 생긴다고 발표했다. 이런 두뇌 리사이클 작업은 주로 잠잘 때 일어난다. 잠을 제대로 못 자거나 정크단백질을 제대로 분해, 리사이클하지 못하면 치매·파킨슨이 생긴다. 단식으로 리사이클되는 게 하나 더 있다. 세균·바이러스도 딱지를 붙여 청소차에 실어 재활용센터로 보내 버린다. 물론 균 침입 시 면역도 작동한다. 하지만 리사이클 방법이 면역부작용(과한 염증, 자가면역)이 없어 더 안전하다. 올해 독일 연구진은 이를 분자수준에서 확인했다. 살모넬라 등 병원균 56종을 감염시켰더니 대장상피세포가 침입균 단백질에 딱지를 붙여 리사이클시킬 수 있음을 확인했다. 어릴 적 보았던 아픈 개도 식중독균 감염 속에서 스스로 살아남는 법을 알고 있었던 셈이다. 단식으로 병을 고치는 비결이 리사이클이다. 비결이 하나 더 있다. 리셋이다. 단식은 제2 시계를 리셋시킨다. 제1 시계는 두뇌 속 생체시계다. 새로 발견된 제2 시계는 배꼽시계다. 즉 간·근육 등 신체말단조직 유전자들이 배꼽시계에 맞추어 일사분란하게 움직인다. 배꼽시계와 두뇌생체시계는 독립적이지만 서로 연관되어 있다. 아침 7시에 기상한다면 두뇌 생체시계는 4시쯤 심장박동을 조절하고 수면호르몬인 멜라토닌도 낮춘다. 반면 배꼽시계 유전자는 매번 들어오던 식사 시간에 맞추어 간·근육세포를 미리 준비시킨다. 실제로 간·근육 유전자 중 73%는 식사에만 반응하는 순수 배꼽시계 유전자, 나머지는 두뇌생체시계와 연관되어 있다(2019, 셀리포트). 문제는 이 두 시계가 서로 엉켰을 때다. 식사시간이 불규칙해지면 배꼽시계 유전자가 헝클어진다. 식사가 들어왔는데도 인슐린이 준비되지 않는다. 헝클어진 배꼽시계는 대사질환을 일으킨다. PC 프로그램이 엉키면 PC를 리셋시켜야 한다. 시차로 틀어진 두뇌생체시계는 햇볕 쬐는 것으로 리셋한다. 헝클어진 배꼽시계 리셋방법은 단식이다. 배꼽시계가 리셋되고 생체물질이 리사이클되면 몸에 무슨 효과가 있을까. ‘자가소화’ 리사이클은 굶은 상태가 핵심 이슬람 5대 의무 중에 라마단 금식이 있다. 굶는 극기로 신앙심을 높인다. 일 년에 한 달간, 해 뜰 무렵부터 질 때까지, 15시간씩 금식이다. 단식자들 혈액을 검사하니 인슐린 민감성을 높이고 대사질환을 낮추는 물질들(TPM)이 모두 높아져 있었다. 라마단 단식이 정신뿐만 아니라 육체도 젊게 만든 셈이다. 단식은 대사질환을 막을 뿐 아니라 대장 줄기세포도 젊게 만든다. 대장 상피세포는 각종 음식, 장내 미생물과 접촉해서 쉽게 상처를 입는다. 줄기세포가 이를 보충한다. 굶을 경우 이런 대장재생능력이 더 높아진다(2018, 셀스템셀). 고대부터 단식하면 장수한다고 했다. 현대과학이 이를 증명한 셈이다. 단식은 건강에 좋다. 그건 맞다. 하지만 ‘사흘 굶어 담장 안 넘는 놈 없다’고 했다. 더구나 굶다가 먹으면 폭식하기 십상이다. 보통사람들이 쉽게 할 수 있는 일상적 단식방법은 없을까? 간디는 저항의 표시로 21일간 단식을 했다. 단식이 시작되면 몸은 초비상이다. 혈중 포도당은 금방 떨어지고 간·근육에 쌓아둔 단기비상식량인 글리코겐이 소비되고 장기비상식량인 지방이 분해되어 포도당으로 변환되는 ‘케토(Keto)’대사가 시작된다. 이렇게 완벽한 단식효과를 보려면 3~4일 굶어야 한다. 독해져야 한다. 독종 아닌 보통사람이 일상에서 청소효과를 볼 수 있는 다이어트방법이 필요하다. 다이어트는 식사종류와 함께 식사방법도 중요하다. ‘아침은 왕처럼, 점심은 평민처럼, 저녁은 거지처럼’이란 말이 사실일까. 미국 성인 5만660명을 7년간 추적 조사했다. 사람들 식사습관(식사횟수·시간·식사량·간식)에 따라 비만도(BMI)가 달랐다. 아침-왕, 점심-평민, 저녁-거지 속설이 사실이었다. 하루 1, 2회 식사를 하고, 아침은 잘 먹고, 저녁-아침 공복시간이 18시간인 그룹들이 비만도가 가장 낮았다(2017, 미영양학회지). 다른 연구에서도 12시간 공복(저녁-아침 사이 공복)그룹보다 16시간 공복그룹이 BMI가 낮았다. 저녁을 7시보다 4시에 먹으면, 체중감소는 비슷해도, 인슐린이 월등 낮았다. 요약해 보자. 저녁-아침 공복이 길수록 감량이 잘되고 리사이클로 건강증진 효과가 높다. 그럼 세끼 소식(小食)은? 소식은 장수촌 공통사항이다. 적게 먹으면 세포 내 보일러인 미토콘드리아가 최적 효율로 연소하면서 유해물질인 활성산소(ROS)가 덜 생긴다. 리사이클도 생긴다. 하지만 중간에 간식을 하면 ‘도루묵’이다. 세포 내에 조금이라도 에너지가 들어오면 ‘굶는 신호’가 사라진다. 인슐린이 다시 높아진다. 무엇보다 리사이클이 중단된다. 리사이클은 굶은 상태 ‘유지’가 핵심이다. 병에 걸려 아픈 개도 끼니를 굶음으로 몸을 고칠 줄 안다. 리사이클, 즉 자가소화(autophagy)가 모든 생물 기본 생존전략이란 의미다. 식사는 평생 습관이다. 본인에 맞는 리사이클 방법을 찾자. 그래서 청춘으로 돌아가자. 단식 습관 안 되면 요요 올 수도 ‘24시간 단식’은 주 1~3일 완전 금식한다. 폭식으로 이어질 수도 있다. ‘16:8 단식’은 저녁식사 후 16시간을 먹지 않는다. 조금 쉬운 방식이다. ‘5:2’단식은 2일간 반 정도 식사를 한다. 다이어트는 어떤 형태든 주의해야 한다. 평생 습관이 안 되면 도루묵이고 오히려 요요·폭식이 생긴다. 필수 영양소가 공급되어야 한다. 당뇨 등 기존 질병이 있는 경우 식습관을 변경하려면 반드시 전문의와 상의해야 한다. 김은기 인하대 교수 ekkim@inha.ac.kr 서울대 졸업. 미국 조지아공대 공학박사. 한국생물공학회장, 피부소재 국가연구실장(NRL), 창의재단 바이오 문화사업단장 역임. 인하대 바이오융합연구소(www.biocnc.com)를 통해 바이오테크놀로지(BT)를 대중에게 알리고 있다. ▶중앙SUNDAY ⓒ중앙SUNDAY and 중앙일보 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>"아이돌한텐 안 묻는데…왜 유튜버만 얼마 버냐가 관심이죠?"</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>스타 크리에이터 도티 "이젠 유튜브도 프리미엄 콘텐츠" 유튜브 크리에이터 '도티'가 23일 오후 서울 강남구 코엑스 그랜드볼룸에서 열린 '국제방송영상마켓(BCWW) 2019'에서 강연하고 있다. © News1 (서울=뉴스1) 박병진 기자 = "사람들은 잘나가는 배우나 아이돌에게는 '얼마 버냐'고 물어보지 않으면서 유튜버한테는 쉽게 물어봅니다. 유튜버의 수익보다는 콘텐츠에 관심을 가져줬으면 하는 바람입니다." 유튜브의 보급 속도만큼 콘텐츠를 만드는 유튜버에 대한 사회적 인식도 개선될 필요가 있다는 유명 크리에이터의 주장이 나왔다. 23일 서울 강남구 코엑스에서 열린 '국제방송영상마켓(BCWW) 2019'에서 구독자 252만명을 거느린 스타 유튜버 도티(본명 나희선)는 "지난해 삼성전자와 같이 스마트폰 '갤럭시A7'을 브랜디드 콘텐츠로 제작한 적이 있다"며 "메이저 브랜드는 어느 모델을 기용하느냐가 굉장히 중요한 일인데 삼성전자가 협업했다는 건 유튜버가 그만큼 가치를 인정받고 존중받는 시대가 된 것"이라고 말했다. 지금 대한민국은 바야흐로 유튜브 전성시대다. 애플리케이션(앱) 분석업체 와이즈앱에 따르면 지난 4월 유튜브의 국내 월간활성사용자(MAU) 수는 3271만명에 달했다. 10대부터 50대 이상까지, 모든 세대가 가장 오래 사용한 앱으로 유튜브가 꼽혔다. 그러나 콘텐츠를 만드는 유튜버의 사회적 인식은 유튜브 사용 빈도와 별개라는 지적이다. 실제로 지난해 10월부터 11월까지 한국노동연구원이 1인 미디어 콘텐츠 크리에이터 250명을 대상으로 설문조사를 실시한 결과 유튜버와 지위가 동일한 직업으로 단순노무자(18.5%)를 꼽은 사람이 가장 많았다. 이날 도티는 소위 '프리미엄 콘텐츠'를 정하는 기준이 바뀌어야 한다고 주장했다. 그는 "유튜브를 보는 '디지털 네이티브' 세대는 거실 TV 채널 선택권이 없기 때문에 유튜브를 보는 게 아니다"라고 지적했다. TV나 영화 같은 기존 프리미엄 콘텐츠 대신이 아니라 그냥 제일 재미있어서 유튜브를 본다는 것이다. 그는 이어 "누군가에게는 블록버스터 영화보다 도티TV의 20분 영상이 더 재미있을 수 있다"며 "프리미엄 콘텐츠는 제작비, 셀럽 출연 여부가 아니라 사용자 효용을 근거로 판단해야 한다"고 말했다. 유튜버도 기존 방송국, 엔터테인먼트사, 프로덕션처럼 프리미엄 콘텐츠를 만드는 사람이라는 논리다. 그는 또 "최근 유튜브를 쉬고 방송을 많이 하고 있는데, 유튜브 콘텐츠도 레거시 미디어 콘텐츠 못지않다는 인식을 높이기 위해 콜라보레이션을 열심히 하고 있다"며 "연예인 되고 싶어서가 아니라 레거시 미디어 방식의 좋은 점을 배우려는 것"이라고 밝혔다. 그는 지난 2월 이후로 유튜브 채널에 동영상을 거의 업로드하지 않는 대신 MBC 예능 프로그램 '라디오스타', '마이 리틀 텔레비전 V2' 등에 출연했다. 아울러 도티는 유튜브 전성시대가 이제 시작 단계며, 앞으로 더 성장할 것으로 내다봤다. 4차 산업혁명으로 기술이 고도화되면 사람들이 그로 인해 편해진 일상을 콘텐츠로 채우리란 것. 그는 "예를 들어 자율주행이 보급된다면 차 안에서 유튜브를 보는 사람이 많아지지 않겠느냐"며 "콘텐츠 산업은 미래가 확실히 보장된 일"이라고 내다봤다. 최근 화제인 유튜브 광고수입에 대해서는 '조회수 장사꾼'을 자처하면 안 된다고 선을 그었다. 도티는 "썸네일, 주제, 제목을 자극적으로 만들면 조회수가 잘 나올 때도 있지만, 매일 자극적인 콘텐츠를 만들다 보면 돌이킬 수 없는 상황에 빠지고 만다"며 "돈만 보고 유튜브를 시작하는 사람은 금방 지치고 콘텐츠의 한계가 금방 드러나게 된다"고 말했다. 그는 유튜버를 희망하는 사람들에게는 "짧게는 1~3년에서 길게는 평생까지 관심을 가지고 재밌게 할 수 있는 주제, 건강하고 지속가능한 콘텐츠에 대한 고민을 먼저 해야 한다"며 "대박을 치기보다는 꾸준히 콘텐츠를 업로드하고 사용자와 소통하며 소박을 차근차근 쌓아가는 게 1인 크리에이터로서의 성공 전략"이라고 조언했다. pbj@news1.kr [© 뉴스1코리아(), 무단 전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>“공인인증서가 필요할 땐 가까운 KT 직영매장으로”</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>[이데일리 김현아 기자] KT그룹의 전자금융 전문 계열사 이니텍(대표 강석모)이 공인인증서 대면 접수처를 전국의 250여개 KT 직영매장(KT M&amp;amp;S)으로 확대했다. 이니텍은 KT, KT M&amp;amp;S와 공인인증서 등록대행 기관 계약을 체결하고 지난 6월부터 주요 KT 직영매장 10곳에서 공인인증서 발급 서비스를 제공해왔다. 고객들은 통신사나 인터넷뱅킹 가입 유무와 관계 없이 이니패스 홈페이지에서 간단한 신청서를 작성하고 가까운 KT 직영매장을 방문하면 5분 만에 범용 공인인증서를 발급받을 수 있다. 이니텍이 발급하는 공인인증서는 사설 인증서와는 달리 인터넷 뱅킹, 온라인 주식거래, 전자민원 서비스 등 공인인증서가 필요한 모든 업무에 범용적으로 사용이 가능하다. 범용 공인인증서는 국가에서 지정한 공인인증기관을 통해서만 발급 받을 수 있으며, 이니텍은 지난해 6월 공인인증기관 지위를 획득했다. KT 직영매장은 금융기관의 영업점 이용 시간 이후인 평일 저녁이나 토요일과 공휴일(일요일과 명절 당일 제외)에도 운영해 평일 일과시간 중에 금융기관을 방문해 공인인증서를 발급 받기 어려운 직장인들이나 학생들이 편리하게 이용할 수 있다. 이니텍은 올 연말까지 개인 범용 공인 인증서(1년)는 무료로, 사업자 범용 공인인증서(1년)는 50% 할인된 5만 5천원에 발급받을 수 있는 프로모션을 진행한다. 9월 말까지 개인 범용 공인인증서를 신규 발급한 고객들은 LG전자 그램 노트북을 비롯해 아이패드, 금 1돈 등 총 2천만원 상당의 푸짐한 경품을 제공하는 ‘이니패스 빅 페스티벌’ 이벤트에 응모할 수 있다. 이벤트 결과는 오는 10월 14일 홈페이지를 통해 발표될 예정이며, 이외에도 주요 KT 직영매장과 이니패스 공식 SNS에서 다양한 프로모션과 게릴라 이벤트가 진행된다. 강석모 이니텍 대표는 “고객들이 보다 편리하게 공인인증서를 발급받아 사용할 수 있도록 대면 접수처를 계속해서 확대할 예정”이라며, “공인인증서 외에도 전자서명 및 다양한 생체 정보 인증과 비대면 실명확인 등 혁신적인 인증 서비스를 제공하는 차세대 통합 인증 플랫폼 이니패스 서비스를 선보이겠다” 고 밝혔다. 김현아 (chaos@edaily.co.kr) 네이버 홈에서 ‘이데일리’ 뉴스 꿀잼가득 , 청춘뉘우스~ ＜ⓒ종합 경제정보 미디어 이데일리 - 무단전재 &amp;amp; 재배포 금지＞</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>"갤노트10 플러스 아우라글로우·블루는 없어서 못 판다"</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>공식출시 첫날 휴대폰 집단상가 가보니 “지원금 더해 40만원대 가능”…갤노트+ 256GB 아우라 글로 ‘인기’ 특정 색상 품귀현상 빚지만 전체 성적표는 지켜봐야 [이데일리 장영은 기자]“갤럭시노트10 이요? 큰 거(플러스 모델) 보시면 지금 아우라 글로우랑 블루는 좀 힘든데” 갤럭시노트(갤노트)10의 공식 판매가 시작된 23일 오후 서울 강변 테크노마트 내 휴대폰 판매점을 방문해 보니 가장 인기 있는 모델은 갤노트10 플러스(+) 256GB ‘아우라 글로우’ 색상이었다. 지난 9일부터 19일까지 진행된 사전예약 결과와도 같다. 갤럭시노트10과 갤럭시노트10 플러스 아우라 글로우 색상 ◇ 공시지원금 28만~45만원…통신사 ‘리베이트’ 50만~60만원 평일 오후라 전반적으로 한산한 모습이었지만 곳곳에서 휴대폰 가격을 상담하거나 계약을 진행하는 모습이 눈에 띠었다. 단일 상품으로는 갤노트10이 단연 인기라는 게 판매점들의 공통된 목소리. 방문 고객 중 열에 일곱은 갤노트10을 찾는다는 설명이다. 이같은 인기는 물량부족 현상으로 나타났다. 현장에서 계약을 하고 돈을 내도 특정 색상의 경우 바로 개통을 하지 못한다는 것이다. 판매점마다 가지고 있는 물량에 차이가 있기는 했으나 갤노트10의 대표 색상인 아우라 글로우와 아우라 블루(SKT 전용)는 최소 일주일 이상은 기다려야 한다는 곳이 많았다. A 판매점 사장은 “아무래도 노트 고객들은 더 큰 화면의 플러스 모델을 선호해 기본 모델(갤노트10)은 전 색상이 다 가능한데 플러스 모델 같은 경우 아우라 글로우는 512GB만 가능하다”며 “블루도 물량이 좀 부족하고 블랙이나 화이트는 당장 개통할 수 있다”고 말했다. 가격은 5G 8만원대 요금제(SKT는 8만9000원, KT는 8만원)를 선택하는 걸 기준으로 공시지원금과 통신사 판매장려금(리베이트)을 통한 할인까지 받으면 갤노트10 플러스(256GB)가 40만원 중후반대에 형성돼 있었다. 해당 모델의 출고 가격이 139만7000원이고, 공시 지원금이 40만원 정도인 것을 감안하면 판매점에서 유통점 리베이트를 받아 50만원 이상 추가 할인을 해주는 셈이다. [이데일리 이동훈 기자]갤럭시노트10과 플러스모델 사양 비교 ◇“사전예약하고 못 받은 사람 수두룩”…가격전망은 엇갈려 B 판매점 직원은 “통신사에서 뿌리는 지원금이 하루에도 바뀌어서 가격을 정확히 말하기 어렵다”면서도 “인터넷 상에서 나오는 것 처럼 10만원대 가격은 현실적으로 힘들고 앞으로도 안 될 것”이라고 설명했다. 10만원이 넘는 가장 높은 요금제를 유지하고, 카드를 새로 만들어 할인을 받는 방법을 동원하면 가능할 수 있지만 그렇게까지 해서 싸게 구매하려는 고객들은 많지 않다고 덧붙였다. 다른 판매점 직원도 “저렴한 가격에 사전 예약한 고객들 중에서도 그 가격으로는 언제 받을지 기약이 없어서 지금 가격으로 돈 더 내고 사은품 받아서 챙겨가시는 분들이 많다”며 “오늘 오전에도 10명도 넘게 그렇게 (제품을) 가져갔다. 더 지나서 9월이 되면 어차피 사전예약 사은품도 못 받는다”고 전했다. 자급제 폰을 판매하는 삼성닷컴의 경우도 사전 예약기간 동안 준비한 물량이 모두 소진돼 지난 19일 이후로는 판매가 중단된 상태다. 삼성전자측은 “지금은 사이트를 통해 주문을 받아도 바로 물건을 받아볼 수 없는 경우가 생겨 삼성닷컴을 통한 갤노트10 판매를 준비 중인 상황”이라고 밝혔다. 삼성전자와 통신사, 판매점 현장 상황을 종합해 볼 때 갤노트10에 대한 초기 반응은 예상치를 웃돌며 호조를 보이고 있는 것으로 판단된다. 다만 최종 성적표는 지켜봐야 할 것으로 보인다. 현재 품귀 현상을 빚고 있는 것이 특정 색상에 한정돼 있고 역대 최대 수준으로 예상됐던 공시지원금이 28만~45만원선으로 ‘실망스러운’ 수준에 머물렀기 때문이다. 사전 예약기간이 끝나면서 오히려 통신사에서 지급하는 리베이트도 다소 줄었다는 게 대다수 판매점측 얘기다. ‘기다리면 더 가격이 떨어지지 않겠느냐’라며 구매 시점을 묻자, 이제는 점점 더 오를 가능성이 높다는 예상과 지금보다 휴대폰 가격이 더 오르진 않을 것 같다는 의견이 반반이었다. 장영은 (bluerain@edaily.co.kr) 네이버 홈에서 ‘이데일리’ 뉴스 꿀잼가득 , 청춘뉘우스~ ＜ⓒ종합 경제정보 미디어 이데일리 - 무단전재 &amp;amp; 재배포 금지＞</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>[노정동의 3분IT] 폴더블폰 나오면 갤럭시노트·갤럭시S 둘 중 하나는 단종?</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>노트10 개발前 S시리즈와 모델통합 논의 S시리즈 화면 커지며 "차별성 부족" 지적 "5G 시대 폴더블폰 나오면 주도권 넘어가" 플래그십 모델 판매량도 점차 하향세 영향 &amp;lt;자료=유진투자증권&amp;gt; 삼성전자의 프리미엄 스마트폰 '갤럭시S'와 '갤럭시노트' 시리즈의 모델 통합설(說)이 흘러나온다. 다음달 5세대 이동통신(5G) 시대의 새로운 폼팩터(특정 기기 형태)로 꼽히는 폴더블폰이 출시되면 효율적 운영을 위해 프리미엄급 두 모델 중 하나는 단종 가능성이 있다는 얘기다. 23일 정보기술(IT) 업계에 따르면 삼성전자 무선사업부(IM)는 이번 갤럭시노트10을 준비하는 과정에서 S시리즈와 모델 통합 가능성을 염두에 두고 제품 개발에 돌입했던 것으로 알려졌다. 갤럭시S와 갤럭시노트의 차별성이 점차 사라지고 있다는 지적이 시장에서 제기되고 있어서다. 실제로 두 모델 간 차별화 포인트 중 하나였던 화면 크기 차이는 이미 사라졌다. 갤럭시S9의 플러스 모델은 6.2인치로 갤럭시노트8(6.3인치)과 유사한 크기였고, 갤럭시S10 플러스 모델(6.4인치)은 심지어 갤럭시노트10(6.3인치)보다 크다. S시리즈 최신작인 '갤럭시S10 5G' 모델도 화면 크기가 6.7인치로 종전에 나온 모든 갤럭시노트 시리즈 디스플레이보다 크다. 이날 공식 출시되는 갤럭시노트10 플러스(6.8인치)만이 갤럭시S10 5G보다 큰 유일한 플래그십 모델이다. 갤럭시S 모델 화면 크기가 점차 커지면서 한 손에 잡히는 그립감을 선호하면 갤럭시S, 대화면 스크린을 선호하면 갤럭시노트 시리즈를 선택했던 종전과는 달라졌다. 삼성전자 내부에서 "둘 중 하나는 정리해야 하는 것 아니냐"는 분위기를 형성하는 더 큰 요인은 스마트폰 사업 수익성 악화다. 삼성전자는 지난 2분기 스마트폰을 담당하는 IM 부문에서 매출 25조8600억원, 영업이익 1조5600억원을 거뒀다. IM 부문 영업익이 2010년 이후 2분기 기준 최저치로 떨어진 것이다. 영업이익률도 6%에 그쳤다. 삼성전자가 스마트폰 사업을 시작한 이래 최악 국면이라 할 만하다. 글로벌 스마트폰 시장이 하락세로 접어든 상황에서 중국 업체들과 경쟁하기 위해 마케팅비 지출을 늘리는 점, 스펙 경쟁으로 생산 원가가 이전보다 크게 뛰는 점이 스마트폰 사업 수익성을 떨어뜨리는 주요인으로 지적된다. 삼성전자는 지난해 스마트폰 연간 판매량이 2013년 이후 처음으로 3억대 밑(2억9130만대)으로 내려섰다. 수익성이 다소 떨어져도 규모의 경제로 버텨온 그간의 스마트폰 사업 전략에 변화가 필요하다는 신호가 내부에서도 나오는 이유다. 삼성전자 관계자는 "중저가 스마트폰 판매량은 호조를 보였지만 프리미엄 제품군 수요가 줄었기 때문"이라고 설명했다. 때문에 삼성전자는 내년부터 스마트폰 출하량의 3분의 1(1억대) 가량을 ODM(제조자개발생산) 방식으로 돌려 효율화하는 방안을 검토하고 있다. 갤럭시J 시리즈 등 저가 제품 라인을 제조업자에 맡기고 프리미엄급 스마트폰만 삼성이 자체 생산하는 게 골자다. ODM으로 가격경쟁력을 확보해 신(新)시장으로 꼽히는 인도·중국 등에서 화웨이, 오포 등 중국 업체들과 맞붙겠다는 심산. 특히 최근 삼성전자가 공을 들이고 있는 인도는 주로 저가 제품 이주 시장으로, 출고가가 100만원 안팎에 달하는 갤럭시S와 노트 시리즈의 주력 시장은 아니다. 여기에 5G가 범용화되면 프리미엄급 제품에선 주도권이 폴더블폰으로 넘어갈 가능성도 제기된다. 삼성전자는 다음달 전세계에서 처음으로 접이식 '갤럭시폴드'를 출시한다. 업계에선 LTE에서 5G로의 이동이 단순히 속도만 높아지는 것이 아니라 그동안 무선에선 쉽게 구현할 수 없었던 증강현실(AR)·가상현실(VR)·인공지능(AI)·클라우드 게이밍 콘텐츠가 개인 스마트폰에서 접할 수 있다고 본다. 소화면과 대화면을 한 번에 쓸 수 있는 폴더블폰 활용도가 극대화될 것이란 설명이다. 고동진 삼성전자 스마트폰 총괄사장은 지난 8일 미국 뉴욕에서 갤럭시노트10 언팩 행사 후 취재진과 만나 "5G 시대에 접는 폰에 대한 수요는 반드시 있을 것이다. (현재 200만원대인) 가격도 낮아질 수 있다"고 언급했다. "5G는 삼성전자 무선사업부의 차세대 먹거리", "폴더블폰만의 역할이 있을 것"이라고도 했다. 문제는 판매량이다. 현재 플래그십 라인에서만 수익을 내고 있는 삼성전자로선 갤럭시S와 갤럭시노트 시리즈 판매량이 특히 중요하다. 기존 프리미엄 라인을 정리·통합한다고 할 때 결국 두 모델 가운데 어느 모델이 소비자 선택에서 멀어질지가 관건이 될 것으로 보인다. 시장조사업체 스트래티지 애널리틱스(SA)와 증권업계에 따르면 역대 갤럭시S 시리즈는 △S1 2500만대 △S2 4000만대 △S3 6500만대 △S4 7000만대 △S5 4500만대 △S6 4500만대(엣지 포함) △S7 4900만대 △S8 4000만대 △S9 4300만대 수준이다. 노트 시리즈도 △노트1 1000만대 △노트2 850만대 △노트3 1200만대 △노트4 800만대 △노트5 850만대 △노트8 1100만대 △노트9 960만대다. 노트6는 출시되지 않았고 노트7은 배터리 발화 사태 이후 FE 모델로 재출시돼 40만대만 한정 판매됐다. 판매량만 놓고 보면 90만원대인 갤럭시S 시리즈가 120만원대 갤럭시노트 시리즈보다 많지만 삼성전자는 가격대와 'S펜' 충성고객 등을 고려했을 때 노트 1000만대 판매면 나쁘지 않은 성적으로 보고 있다. 다만 이번 갤럭시노트10 성적이 좋지 않을 경우 마지막 노트 제품이 될 가능성도 배제할 수 없다. 과거 갤럭시노트7 배터리 발화 사태 이후 삼성전자 내부에서 노트 시리즈 존폐 여부를 놓고 논의를 거쳤을 때도 가장 먼저 고려한 건 향후 소비자 수요였다. 노트8 판매량이 유독 높았던 건 노트5 이후 교체 수요가 몰렸기 때문이다. 고동진 사장은 "다음달 갤럭시폴드가 출시됨에도 불구하고 스마트폰 포트폴리오 측면에선 아직 노트 시리즈를 최상위급으로 보고 있다"면서 "폴더블폰은 이제 시작하는 사업이고 이들(갤럭시S, 갤럭시노트)과는 완전히 다른 폼팩터로 판단하고 있다"며 조심스러운 입장을 나타냈다. 한 업계 관계자는 "S펜에 대한 충성고객을 놓치기 싫다면 노트 시리즈를 포기한 뒤 애플처럼 S펜을 별도 판매하는 방식을 채택할 수 있다"며 "갤럭시노트10이 어느 정도 의미 있는 판매량을 보일지가 향후 노트 시리즈의 향방을 결정할 수 있다"고 덧붙였다. 노정동 한경닷컴 기자 dong2@hankyung.com ▶ ▶ ▶ ⓒ 한국경제 &amp;amp; , 무단전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>신형 아이폰 초광각·역충전 도입…"갤럭시 쏙 빼닮았네?"</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>블룸버그 "9월 신형 아이폰 3종 공개…2종에 '프로' 명칭" 핵심은 카메라…초광각, 동영상 촬영에 방점 에어팟 충전 위한 무선 배터리 공유 기능도 탑재 [이미지출처=연합뉴스] [아시아경제 임온유 기자] 9월 공개되는 신형 아이폰의 핵심은 카메라다. 특히 '넓게 찍는 초광각'과 '전문가 수준의 동영상' 촬영이 새로이 도입될 것으로 예상된다. 블루투스 이어폰 에어팟을 충전할 수 있는 '무선 배터리 공유' 기능 역시 히든 카드 중 하나다. 모두 애플이 아이폰에 처음 시도하는 것들이다. 하지만 소비자를 놀라게 할 '와우 포인트'는 부족하다. 이 모든 기능들은 삼성전자가 3월 출시한 '갤럭시S10'에 이미 탑재된 바 있기 때문이다. 22일(현지시간) 미국 블룸버그에 따르면 애플은 내달 신형 아이폰 3종을 공개한다. 3종은 각각 아이폰XS·XS맥스·XR의 후속작으로 상위 2종에는 '프로'라는 명칭이 붙을 것으로 예상된다. 블룸버그는 프로 2종의 핵심은 업그레이드된 후면 카메라 시스템이라고 지목했다. 이들은 트리플 카메라를 장착하는데 특히 광각을 넘어서는 초광각 촬영에 특화될 전망이다. 동영상 촬영 기능도 대폭 업그레이드된다. 블룸버그는 "신형 아이폰의 카메라는 전문 비디오 카메라에 더 가까이 다가갈 것"이라고 했다. 사용자가 촬영하며 실시간으로 수정, 효과 적용, 색상 변경, 프레임 변경, 자르기를 할 수 있다는 설명이다. 이외에도 어두운 곳에서의 촬영 기능이 향상되고 세 개의 이미지를 한꺼번에 촬영한 뒤 인공지능(AI) 소프트웨어로 이를 합성해 최적의 결과물을 얻을 수 있게 한다고 블룸버그는 전했다. 모두 아이폰에 처음 도입되는 기능이지만 혁신의 측면에서는 아쉽다. 삼성전자를 비롯한 안드로이드폰에서 대부분 시도된 사항들이기 때문이다. 특히 출시된 지 5개월이 지난 갤럭시S10과의 유사성이 크다. 삼성전자는 지난 2월 갤럭시S10을 공개할 당시 초광각 트리플 카메라를 장착하고 전문가 수준의 동영상 촬영이 탁월하다고 강조한 바 있다. 지난 20일 출시된 '갤럭시노트10'의 경우 신형 아이폰처럼 고도화된 동영상 편집 툴을 자체 탑재했다. 스티브 잡스가 집권하던 시절 애플은 '혁신의 아이콘'으로 불렸다. 그러나 최근 팀 쿡 체제 애플의 행보는 혁신보다는 안정에 방점이 찍혔다. 새로운 시도를 하기 보다는 이미 시도된 것을 향상시키는 데 보다 집중하는 것이다. 프리미엄 스마트폰 시장이 마이너스 성장을 거듭하고 있는 상황에서 혁신과 안정 중 정답이 무엇인지는 알 수 없다. 그러나 애플의 선택은 스마트폰 시장의 침체를 인식하고 서비스·소프트웨어 시장에 역량을 분산하는 것과 무관하지 않다고 분석된다. 애플은 최근 애플뮤직, 앱스토어 등 서비스 흥행에 힘입어 역대 최고 2분기 매출 538억 달러(약 65조 980억 원)를 기록했다. 반면 아이폰 매출은 259억9000달러(약 31조3390억원)로 7년 만에 처음으로 전체 매출의 절반에 미치지 못했다. 임온유 기자 ioy@asiae.co.kr &amp;lt;ⓒ경제를 보는 눈, 세계를 보는 창 아시아경제 무단전재 배포금지&amp;gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>[+다큐] 알파고 충격 후 3년‧‧‧그간 바둑은 어떻게 변했을까?</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>동영상 뉴스 	 	구글의 바둑 인공지능, 알파고의 등장으로 바둑계의 판도가 바뀌었습니다. 알파고가 바둑계 판도 변화의 신호탄을 던졌다면 페이스북의 바둑 인공지능 엘프고는 실제적인 판도 변화를 이끌어냈습니다. 바둑을 공부하는 방법이 바뀌었고, 포석 전략이 단순화되었고, 바둑 기사들의 실력도 전반적으로 늘었습니다. 이제는 만만하게 볼 프로기사가 거의 없다고 합니다. 실력이 상향 평준화됐다는 이야기입니다. 그러나 바둑 고유의 인간미는 점점 사라져가는 것 아니냐는 질문도 제기됩니다. 알파고 이후, 바둑 인공지능이 바둑계에 미친 영향과 미칠 영향을 취재했습니다. 기획 : 김동민(kdongmin@ytn.co.kr) 연출 : 서정호(hoseo@ytn.co.kr) 편집 : 강재연, 서정호 촬영 : 함초롱, 안용준 [저작권자(c) YTN &amp;amp; YTN PLUS 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>"실험 적극 참여했다는데"…조국 딸 1저자 논란 입증할 '연구노트' 있을까</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2007년 연구노트 지침 제정…2010년 8월 연구노트 의무화 조양 2007년 실험 참여…"황우석 사태로 당시 연구노트 중요성 높을 시기" 조국 법무부 장관 후보자가 23일 오전 인사청문회 준비를 위해 서울 종로구 현대적선빌딩에 마련된 사무실로 출근하며 취재진의 질문에 답하고 있다. 2019.8.23/뉴스1 © News1 이재명 기자 (서울=뉴스1) 최소망 기자 = 조국 법무부 장관 후보자 딸의 의학논문 제1저자 등재 논란이 일파만파로 확산되면서 국내 규정상 의무화된 '연구노트' 유무에 관심이 쏠리고 있다. 연구노트는 조국 후보자의 주장대로 딸이 직접 연구에 참여했다는 주장을 입증할 결정적 근거로 될 수 있기 때문이다. 반면 이를 작성하지 않았을 경우 '연구부정'에 무게가 실린다. 23일 과학기술계에 따르면 지난 2007년 12월 교육과학기술부 훈령 '국가연구개발사업 연구노트관리지침'이 제정됐다. 이후 2008년 1월 지침이 시행됐으며 2010년 8월 대통령령 '국가연구개발사업의 관리 등에 관한 규정'이 개정돼 모든 국가 연구개발(R&amp;amp;D)에 참여하는 연구자는 연구노트를 작성하는 게 의무화됐다. 연구노트는 연구자가 수행하는 연구와 실험 등 모든 과정을 기록하는 것으로 실험을 위한 환경, 조건, 과정, 현상, 결과 등을 구체적으로 작성해야 한다. 이같은 기록은 연구윤리 측면에서 중요한 역할을 한다. 연구자가 발표한 결과를 과장, 허위, 표절없이 직접 수행했는지 증명할 수 있는 기록물이기 때문이다. 조국 후보자 딸 조 양은 지난 2009년 대한병리학회지(The Korean Journal of Pathology)에 제 1저자로 '출산전후(주산기) 허혈성 저산소뇌병증(HIE)에서 혈관내피산화질소 합성효소 유전자의 다형성'(eNOS Gene Polymorphisms in Perinatal Hypoxic-Ischemic Encephalopathy)이란 영어 논문을 출판했다. 앞서 조 양은 2007년 7월23일부터 8월3일간 약 2주간의 인턴 기간을 통해 실험을 진행했고 이후 2008년 12월 논문을 투고했다. 조 후보는 조 양이 직접 실험에 참가했다는 점을 피력한다. 조 후보자 측은 지난 20일 "후보자의 딸은 멀리까지 매일 오가며 프로젝트의 실험에 적극 참여해 경험한 실험과정 등을 영어로 완성하는데 기여하는 등 노력한 끝에 다른 참여자들과 함께 6~7페이지 짜리 영어논문을 완성해 해당 교수로부터 좋은 평가를 받았다"고 해명한 바 있다. 조 후보자 말에 따르면 조 양은 적극적으로 실험에 참가했고 이러한 부분이 연구노트에 남아 있을 확률이 있다는 것. 따라서 조 모양의 연구에 대한 기여도 등을 면밀하게 파악하기 위해서는 단국대 인턴으로 참가했을 시기의 연구노트를 공개하고 이를 투명하게 검증하는 게 중요한 사안으로 떠올랐다. 익명을 요구한 한 과학기술인은 "모든 과학기술연구는 연구노트를 작성할 의무가 있고 이를 작성하지 않거나 부실, 변경, 거짓 기재하면 연구부정행위"라면서 "단국대·공주대 연구진들은 조 양과 관련한 연구노트를 영구하게 보유하고 있어야 한다"고 말했다. 이어 "그렇지 않다면 이는 연구부정 행위"라며 "연구노트를 공개하고 투명하게 검증해야 할 필요가 있다"고 주장했다. 문제는 조 양이 실험하던 시기가 연구노트가 의무화된 시기는 아니라는 점이다. 조 양이 실험에 참가한 때는 2007년이다. 연구노트 의무화가 이뤄진 시기는 2010년이기 때문이다. 그럼에도 당시에는 2005년 황우석 사태 이후 '연구노트'에 대한 중요성이 높아진 시기라 윤리적으로나 도의적으로 연구노트가 작성됐어야 한다는 목소리가 나온다. 연구노트는 이른바 '황우석 사태'가 촉발한 제도로 꼽힌다. 정부 집계에 따르면 2008년부터 2009년까지 연구노트가 제작 보급된 수는 약 1만1000개에 달했다. 당시 국내 다수 과학자들은 해외 논문 투고 시 연구노트를 공개하라는 요구를 받기도 한 시기다. 대한의학회도 지난 22일 긴급 이사회 후 기자들과 만나 "연구노트 등 당시 기록이 없으면 당사자들의 진술이 유일한 증거가 된다"면서 연구노트의 중요성을 강조한 바 있다. somangchoi@news1.kr [© 뉴스1코리아(), 무단 전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>'병원비 걱정없는 나라' 만든다더니···국고 대신 '건보료 청구서' 꺼내</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>■국민에 부담 떠 넘긴 '文케어'···내년 건보료 3.2% 인상 국민 57% "추가부담 반대"에도 보장률 강화 정책에 매년 올려 가입자단체에도 갈수록 '큰 짐' 경총 "재정수지 적자 해결하라" 정부는 "건보 건전성 문제없다" [서울경제] ‘문재인케어’로 불리는 건강보험 보장성 강화정책으로 내년 건강보험료가 3.2% 인상된다. 지난해 건강보험 재정수지가 적자로 돌아선 가운데 3년 연속 건보료가 인상되자 정부에서 재정부담을 국민에게 전가하고 있다는 우려의 목소리가 잇따르고 있다. ’문재인 케어’의 핵심인 ‘병원비 걱정 없는 국가’ 를 건보료를 올려 만들고 있다는 자조 섞인 목소리까지 나온다. 보건복지부는 지난 22일 건강보험정책 최고의결기구인 건강보험정책심의위원회를 열어 오는 2020년 건강보험료율을 3.2% 올린다고 밝혔다. 이에 따라 직장가입자의 보험료율은 현행 6.46%에서 6.67%로, 지역가입자의 부과점수당 금액은 현행 189원70전에서 195원80전으로 인상된다. 월평균 보험료를 보면 올 3월 기준 직장가입자는 11만2,365원에서 3,653원 오른 11만6,018원을 내야 한다. 지역가입자는 8만7,067에서 2,800원 인상된 8만8,867원을 내년부터 추가로 부담해야 한다. 김재헌 무상의료운동본부 사무국장은 “국고지원금 없이 국민을 볼모로 건강보험료를 올리는 문재인케어가 계속 시행되면 예상보다 빨리 적립금이 고갈되는 최악의 상황에 직면할 수 있다”고 말했다. 국민 57% “추가부담 반대”에도 보장률 강화 정책에 매년 올려 가입자단체에도 갈수록 ‘큰 짐’ 경총 “재정수지 적자 해결하라” 정부는 “건보 건전성 문제없다” 건강보험료율은 최근 10년 동안 2009년과 2017년을 빼고 매년 올랐다. 2007년(6.5%)과 2008년(6.4%), 2010년(4.9%), 2011년(5.9%)에는 4∼6%대 인상률을 기록했고 2012년(2.8%), 2013년(1.6%), 2014년(1.7%), 2015년(1.35%), 2016년(0.9%)에는 1% 안팎에 그쳤다. 문재인 정부 출범 이후 건강보험 보장성 강화정책을 본격적으로 시행한 지난해와 올해 인상률은 각각 2.04%와 3.49%였다. 건보료 인상을 둘러싼 국민 여론은 싸늘하기만 하다. 한국보건사회연구원이 지난해 성인 2,000명을 대상으로 건강보험 보장률과 건강보험료 인상률을 조사한 보고서를 보면 응답자의 57.1%는 ‘건강보험 보장성 확대는 찬성하지만 보험료 추가 부담은 반대한다’고 답했다. 건강보험정책심의위원회 가입자단체도 정부의 일방적인 건보료 인상에 일제히 우려를 나타내고 있다. 한국경영자총연합회 관계자는“엄중한 대내외 경제 현실을 고려해 건보료 인상에 대해 거듭 우려를 밝혔지만 정부가 인상을 강행한 것에 깊은 유감을 표명한다”며 “국민과 기업에 건보료 부담을 전가시킬 것이 아니라 지금이라도 국고지원금으로 건강보험 재정수지 적자를 해결해야 한다”라고 말했다. 국고 지원을 늘이고 건보료 인상률은 대폭 낮춰야 한다는 게 가입자단체들의 지적이다. 건강보험법과 건강증진법과 따르면 정부는 매년 건보료 예상수입액의 20%를 국고로 지원해야 한다. 하지만 지난 2007년 법률 개정 이후 정부는 이를 제대로 지킨 적이 한 차례도 없다. 올해까지 연평균 건보료 국고지원율은 15.3%에 그쳤고 미납액은 24조5,374억원에 달한다. 보건복지부는 내년부터 국고지원금을 최소 14% 이상 확보하겠다고 밝혔지만 예산집행 권한을 가진 기획재정부가 회의적이어서 이마저도 불투명하다. 한편 정부는 건강보험 재정에 경고등이 켜졌음에도 누적 적립금이 20조5,955억원에 달해 문제가 없다는 입장이다. 문재인 케어가 완료되는 오는 2022년까지 최소 30조원의 재원이 필요한데 10조원은 누적 적립금으로 채우고 20조원을 건보료 인상으로 충당하면 여전히 10조원의 누적 적립금을 예비비로 확보할 수 있다는 설명이다. 하지만 국회예산정책처의 보고서에 따르면 문재인 정부의 임기가 끝나는 2022년까지 총 13조5,000억원의 건강보험 수지 적자가 이어질 전망이다. 차기 정부에도 문재인 케어가 계속 시행된다고 가정하면 2023년부터 2027년에는 총 12조1,000억원의 적자가 추가로 발생해 적립금마저 완전히 고갈되는 것으로 나타났다. 김우현 한국조세재정연구원 연구위원은 “문재인 케어로 국민의 평균 의료비가 줄어드는 효과는 있겠지만 고령화로 급격히 증가하는 건강보험 재정지출을 감당하는 것은 사실상 불가능하다”며 “건강보험 재원을 마련하는 것 못지않게 불필요한 지출을 줄여 건강보험 재정 효율화를 달성하는 노력이 절실하다”고 말했다. /이지성기자 engine@sedaily.com | 저작권자 ⓒ 서울경제, 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>길어지는 스마트폰 교체주기…"美소비자, 평균 33개월 쓴다"</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>미국인들의 스마트폰 교체주기가 평균 33개월에 달하는 것으로 나타났다. 애플 아이폰과 삼성 갤럭시의 평균 교체주기는 각각 35.4개월, 32.7개월이었으며 스마트폰 교체 원인으로는 디스플레이 파손, 배터리 소모가 가장 많았다. 24일 시장조사업체 스트래티지 애널리틱스(SA)가 18~64세 스마트폰을 사용하는 미국인 2513명을 조사한 결과 이들이 사용중인 스마트폰 평균 보유기간은 17개월로 집계됐다. 애플 아이폰이 18.3개월로 가장 길었고 모토로라가 14.3개월로 가장 짧았다. 삼성전자와 LG전자는 각각 16.5개월, 15.7개월로 조사됐다. 다음 스마트폰 교체 시점을 묻는 질문에는 응답자 90% 이상이 16개월 뒤에 교체하겠다고 답했다. 브랜드별로는 애플 17.1개월, 삼성 16.1개월, LG전자 14.2개월 순이었다. SA는 이를 근거로 예상 스마트폰 교체주기를 평균 33개월로 추산했다. 현재 보유기간에 예상 보유기간을 더한 수치다. 이에 따라 교체주기는 애플 아이폰 36개월, 삼성 갤럭시 33개월, LG전자 29.9개월로 환산됐다. 구글 넥서스가 35.9개월로 교체주기가 가장 길었다. 미국 스마트폰 교체주기는 길어지고 있다. 2016년 26개월을 넘어선 후 지난해 31개월로 늘었다. 참고로 우리나라는 지난해 기준 31개월로 집계됐다. 응답자 79%는 디스플레이가 파손됐을 때 스마트폰을 교체하겠다(복수응답 기준)고 답했다. 배터리 소모가 너무 빠르거나 스마트폰 속도가 현저히 저하됐을 때 교체하겠는 답변도 78%, 73%에 달했다. 신제품 교체를 이유로 든 응답자는 30%에 그쳤다. 스마트폰 구매를 결정하는 요소로는 '배터리 성능'과 '기기에 대한 신뢰'가 가장 앞섰다. 응답자의 70%가 배터리 성능을 1순위로 꼽았으며 기기에 대한 신뢰 54%, 카메라 성능 52%로 뒤를 이었다. 한편 올 상반기 미국 스마트폰 출하량은 6570만대로 글로벌 전체 출하량(6억7180만대)의 9.7%를 차지했다. 애플 아이폰이 출하량 3300만대로 미국 내 점유율 1위(50.2%)를 기록했고 삼성 갤럭시는 1790만대(27.2%)로 2위에 올랐다. LG전자(880만대), TCL-알카텔(460만대), 레노버-모터로라(450만대)가 3~5위에 이름을 올렸다. 윤진우 한경닷컴 기자 jiinwoo@hankyung.com ▶ ▶ ▶ ⓒ 한국경제 &amp;amp; , 무단전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>"5G 가입자, 벌써 250만명"…'빠름빠름' LTE보다 2배 빨라</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SKT100만·KT 75만·LGU+ 67만 순…커버리지 확대 총력 SK텔레콤이 지난 21일 단일 통신사 기준 5G 가입자 100만 명을 돌파했다고 22일 전했다. 지난 4월 3일 세계 첫 5G 스마트폰을 출시한 이후 140여일 만이다. 사진은 SK텔레콤 모델들이 서울 명동에 위치한 대리점에서 ‘갤럭시 노트10’로 5G 서비스를 사용하고 있는 모습. (SK텔레콤 제공) 2019.8.22/뉴스1 (서울=뉴스1) 강은성 기자 = 지난 4월 한국이 세계 최초로 상용화한 5세대(5G) 이동통신 가입자가 상용화 142일 만에 250만명에 육박하는 것으로 나타났다. 4G 롱텀에볼루션(LTE) 가입자 증가보다 2배 가까이 빠른 속도다. 24일 업계에 따르면 국내 5G 가입자가 250만명 돌파 초읽기에 돌입했다. 이미 지난 21일 기준으로 SK텔레콤은 5G 가입자 100만명을 넘어섰고 KT는 75만명, LG유플러스는 67만명의 가입자를 각각 확보해 국내 5G 가입자는 총 242만명에 달했다. 이후 갤럭시노트10 5G 모델 사전개통과 이날 공식 출시까지 맞물리면서 이틀간 5G 가입자가 빠르게 증가해 250만명에 육박하는 것으로 나타났다. 이통사 관계자는 "이런 추세라면 주말쯤 3사 통합 250만명 돌파는 무난할 것으로 예상된다"고 설명했다. 이는 지난 2011년 7월 처음으로 상용화한 4G LTE에 비해 2배 가까이 빠른 수치다. 당시 LTE는 200만 가입자를 돌파하는데 이미 7개월, 215일이 소요됐었다. 그러나 5G의 경우 상용화 120일여만인 이달 초에 200만 가입자를 넘어서면서 LTE보다 급격히 빠른 속도로 가입자를 불리고 있다. 통신업계 전문가는 "4G LTE의 경우 2011년 7월 상용화는 시작했지만 LTE 스마트폰이 출시된 것은 10월이 넘어서였다"면서 "게다가 4G LTE 주파수 확보에 실패한 KT가 2012년 1월이나 되어서야 비로소 LTE 스마트폰을 출시하고 가입자를 모집했기 때문에 LTE 200만 가입자 돌파 시점에서는 SK텔레콤과 LG유플러스 가입자로 한정되는 부분이 있었다"고 설명했다. 이 전문가는 이어 "반면 5G는 정부 주도로 상용화 관련 정책을 마련하고 대통령까지 상용화 행사에 나서는 등 국민적 관심이 컸고, 상용화와 함께 삼성전자, LG전자의 스마트폰도 적시에 출시되면서 가입증가 속도가 빨라지는 것으로 보인다"고 분석했다. 여기에 이통3사가 5G 초기 시장에서 승기를 잡기 위해 공격적으로 마케팅 경쟁을 벌이며 '역대급' 공시지원금을 지급한 것도 가입자를 유인한 요인으로 작용했다. 다만 아직 전국망과 실내망이 제대로 갖춰지지 않은 상황에서 마케팅 경쟁을 통해 가입자만 늘리다보니 초기 가입자들이 5G 품질에 대해 적지 않은 불만을 제기하는 것은 심각한 문제로 지적되고 있다. 이에 이동통신3사는 연말까지 전국 옥외 커버리지를 인구대비 90% 대로 끌어올리고 실내 커버리지 확대에도 총력을 기울이기로 했다. 주요 공항 및 KTX 역사, 대형 쇼핑센터 및 전시장 등 전국 120여개 인구밀집 건물 내에서는 이미 실내 5G 서비스를 시작했으며 연말까지 전국 350여개 영화관·체육경기장·대형마트 등을 추가 선정해 이통3사가 실내 5G 망을 공동구축하기로 했다. 서울을 비롯한 전국 지하철에도 5G 망을 공동구축한다. 과기정통부는 "5G 가입자가 200만명에 달하는 만큼 내실 있는 5G 서비스를 이용할 수 있도록 이동통신사와 제조사에 지속적인 품질 개선 노력과 적극적인 서비스 다변화를 요청했다"며 "앞으로도 민관과의 긴밀한 협력을 통해 국민에게 최고 품질의 5G 서비스를 제공하기 위하여 최선의 노력을 다할 계획"이라고 밝혔다. esther@news1.kr [© 뉴스1코리아(), 무단 전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>만능폰 '갤노트10'…꼭 써봐야할 숨겨진 기능 5選</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>[머니투데이 박효주 기자] [편집자주] 박푸로의 IT썰은 특정 분야의 전문가인 '프로'에는 못미치지만, 그에 준하는 시각에서 IT 관련 이슈를 다뤄보고자 만든 코너입니다. 스마트폰, 모바일 서비스, 카메라 등등 제품 및 서비스에 관한 내용을 쉽게 풀어내겠습니다. [[박푸로 IT썰]덱스·향상된카메라·동영상편집·게임스트리밍·AR두들] 맥북에서 덱스를 구동하면서 갤럭시 노트10에서는 넷플릭스를 실행하는 모습. 스마트폰 성능은 나날이 진화하고 있지만, 모든 기능을 일일이 찾아 100% 활용하기란 쉽지 않다. 갤럭시노트10(이하 갤노트10)도 삼성 모바일 기기의 혁신 집대성이라 불릴 만큼 다양한 기능을 품고 있다. 갤럭시S10에서 적용됐던 무선 배터리 공유, 초음파식 지문 스캐너, 초광각 카메라 등 대표적인 기능 외에도 새롭게 들어간 기능이 많다. 노트 시리즈인 만큼 S펜에 가려진 기능 중에서 꼭 써봐야 할 5가지를 꼽아봤다. ◇더 쉽고 편해진 '덱스'…연결만 하면 끝= 스마트폰에서 마치 PC와 같은 사용 경험을 제공하는 삼성 덱스가 갤노트10에서 한 단계 발전했다. 이제 별도의 액세서리 없이 USB 케이블로 PC와 연결만 하면 PC의 큰 화면과 키보드·마우스를 활용해 더욱 편하게 갤노트10을 사용할 수 있다. 이번 덱스의 변화에서 눈여겨볼 부분은 윈도뿐만 아니라 맥도 지원한다는 점이다. 윈도나 맥에 덱스 전용 프로그램을 설치하고 갤노트10을 연결하면 다른 조작 없이 바로 덱스 화면이 나타난다. PC 안에 PC가 구현된 느낌이다. PC파일을 끌어다 덱스에 놓으면 갤노트10으로 파일이 바로 전송되며, 반대도 가능하다. 드래그앤드롭으로 갤노트10의 사진을 PC로 보내는 모습. 덱스를 사용하면서 갤노트10도 동시에 사용할 수 있다는 점도 꽤 유용하다. 덱스를 통해 게임을 구동하고, 갤러리 사진을 보면서 갤노트10에서는 전화나 문자를 하거나 은행 업무를 동시에 처리할 수 있다. ◇소리도 확대한다?…'줌인 마이크'= 갤노트10은 동영상 촬영 중 특정 부분을 확대하면 해당 부분의 피사체의 소리를 키워서 녹음해주고, 주변 소음은 줄여주는 '줌 인 마이크' 기능을 지원한다. 예컨대 야외에서 뛰어노는 아이를 중앙에 맞혀 확대하면 아이의 목소리를 주변 소리보다 더 또렷하게 녹음할 수 있다. 줌인마이크가 활성화 되어 있을 때 영상 촬영 중 소리가 나는 쪽으로 확대하면 마이크 아이콘이 표시된다. 카메라 기능에는 줌인 마이크 외에 흔들림 없는 영상 촬영을 가능하게 해주는 향상된 '슈퍼 스테디'가 적용됐다. 샘플 레이트를 500MHz에서 833MHz로 향상해 미세한 흔들림까지 감지한다. 특히 하이퍼랩스 촬영 시에도 지원해 더욱 다양한 콘텐츠를 흔들림 없이 제작할 수 있다. ◇동영상 편집, 갤노트에서 바로= 아이폰에서 대표적으로 사용할 수 있는 동영상 편집 앱 '아이무비'와 같은 가볍고 강력한 영상 편집 기능이 갤노트10에 들어갔다. 별도의 앱 설치 없이 바로 손쉽게 편집과 공유가 가능하다. 갤러리에서 영상을 선택하고 연필 모양을 누르면 바로 편집 메뉴가 등장한다. 여기서는 영상 길이를 조정하거나 영상과 영상 사이에 특수효과를 넣을 수 있다. S펜을 이용한 영상 내 메시지를 추가할 수 있으며 재생속도 변경과 다른 영상과 합치는 등의 기능을 제공한다. S펜을 활용하면 더욱더 세밀한 영상 편집이 가능하다. 기본 탑재된 영상 편집 도구 ◇깨알 재미 'AR(증강현실) 두들'= 갤노트10은 정교한 모바일 AR 기술이 접목된 'AR 두들' 기능을 지원해 즐거우면서도 창의적인 콘텐츠를 만들 수 있게 했다. AR 두들은 S펜 메뉴에서 선택할 수 있다. 이 기능은 사진이나 영상 촬영 시 공간을 인식하는 알고리즘을 사용해 사람이나 공간을 추적해 사용자가 S펜으로 그린 그림과 움직이는 피사체가 함께 조화롭게 보인다. 갤노트10+(플러스)는 후면에 뎁스비전 카메라를 추가로 탑재해 피사체를 스캔해 3D 이미지를 만들 수 있다. 이렇게 제작된 3D 이미지가 피사체를 따라 움직이는 영상도 제작이 가능하다. 사물까지의 거리와 사물의 길이나 크기를 측정하는 '간편 측정' 기능도 전작에 이어 탑재됐다. 3D 스캐너 앱으로 사물을 갤노트10에 3D로 구현할 수 있다. ◇어디서나 고성능 게임 즐긴다= 집에서 PC로만 즐기던 고성능 게임을 갤노트10으로 언제 어디서나 그대로 즐길 수 있는 '플레이갤럭시 링크' 기능을 갤노트10에 처음으로 탑재했다. 이 기능은 사용자가 PC로 게임을 하다가 잠시 PC 앞을 떠날 때 하고 있던 게임을 그대로 갤노트10에서 이어 할 수 있다. P2P 스트리밍으로 PC 화면을 전송하기 때문에 갤노트10에 게임 별도 설치할 필요가 없으며, 높은 사양을 요구하는 게임도 문제없다. 사용자가 갤노트10을 직접 터치하거나 전용 게임패드를 통해 게임을 조작하면 연결된 PC로 게임 명령이 전달된다. 플레이갤럭시 링크로 PC게임을 갤노트10으로 스트리밍 하는 모습. /사진=슬래시기어 박효주 기자 app@ &amp;lt;저작권자 ⓒ '돈이 보이는 리얼타임 뉴스' 머니투데이, 무단전재 및 재배포 금지&amp;gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>지구보다 나은 생명체 서식 조건 갖춘 외계행성 가능</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>美연구팀, 대양 조건 분석 결과 "최적화된 곳 아닐 수도" '트라피스트(TRAPPIST)-1' 행성계 상상도 지구에서 가장 가까운 별인 트라피스트-1 행성계는 모두 7개의 행성을 거느리고 있으며 이 중 3개가 액체상태의 물이 존재할 수 있는 서식가능지역 안에 있다. [NASA/JPL-Caltech 제공] (서울=연합뉴스) 엄남석 기자 = 지구를 닮은 행성을 찾는 노력이 무위로 그치고 있지만 외계행성 중에는 지구보다 생명체가 살기에 더 좋은 조건을 갖춘 곳이 있을 수 있다는 연구결과가 나왔다. 국제 지구과학 학술대회인 '골드슈미트 콘퍼런스(Goldschmidt Conference)'와 외신 등에 따르면 미국 시카고대학의 스테파니 올슨 박사가 이끄는 연구팀은 바르셀로나에서 진행 중인 이 학술대회 기조연설을 통해 생명체가 서식할 수 있는 외계행성 대양(大洋)의 조건에 초점을 맞춰 진행한 연구결과를 발표했다. 연구팀은 미국항공우주국(NASA) 고다드우주연구소(GISS)가 개발한 암석형 행성 3D 시뮬레이션 프로그램인 'ROCKE-3D'를 이용해 다양한 조건을 부여하며 생명체가 서식하는데 가장 적합한 대양 환경을 분석했다. 지구 대양의 경우 생명체는 심해의 영양분을 광합성 생물이 서식하는 햇빛 수역으로 올려놓는 '용승(湧昇)' 작용에 의존하는데, 이런 용승작용이 강할수록 영양분 공급도 늘어나 생물학적 활동도 늘어나게 된다. 연구팀은 "이것이 바로 외계행성에서 들여다봐야 할 조건"이라고 강조했다. 연구팀은 해양순환 모델까지 이용해 어떤 행성이 가장 효율적인 용승작용이 일어나 생명체에 특별히 더 적합한 대양 환경을 제공하는지를 분석했으며, 그 결과 대기 밀도가 높고 자전율이 느리며 대륙이 존재하는 곳에서 더 효율적인 용승작용이 일어난다는 점을 확인했다. 연구팀은 이런 결과는 지구가 생명체 서식에 최적화된 곳이 아닐 수도 있다는 점을 시사하는 것으로 다른 행성의 생명체가 지구보다 더 나은 환경을 누리고 있을 수 있다는 의미라고 설명했다. 트라피스트-1f 대양 상상도 트라피스트-1 행성계의 다섯번째 행성인 트라피스트-1f는 조석고정으로 늘 햇빛을 받는 쪽은 대양이 존재하고 그 반대 쪽은 얼음세계인 것으로 추정되고 있다. [NASA/JPL-Caltech 제공] 올슨 박사는 "(생명체에) 유리한 해양순환 패턴을 가진 일부 외계행성의 조건이 지구 생명체보다 더 많고 활발한 생명체를 지탱하는데 적합할 수 있다는 것을 보여준 것은 놀라운 결론"이라고 강조했다. 이번 연구결과는 외계 생명체 탐색과 망원경을 비롯한 탐색 장비 개발에서 추가로 고려해야 할 기준을 제시하는 것으로 받아들여지고 있다. 지금까지는 외계행성이 생명체 '서식가능지역(habitable zone)' 안에 있는지만을 기준으로 삼아왔다. 별에 너무 가까이 붙어 있어 표면의 물이 증발하거나 너무 멀리 떨어져 있어 물이 얼면 생명체가 존재할 가능성이 희박해지기 때문에 표면의 물이 액체 상태를 유지할 수 있는 곳의 행성을 찾아왔다. 그러나 대양이 존재한다고 해서 생명체 서식 조건이 모두 같은 것은 아니라는 점이 이번 연구를 통해 구체적으로 확인된 만큼 서식가능지역 기준을 넘어 대양 환경도 확인하는 작업이 필요하다는 것이다. 조지아 공대의 크리스 레인하드 교수는 논평을 통해 대양은 생명체 지표로서 중요하지만 "태양계 밖 외계행성의 대양에 대한 이해는 매우 초보적인 상태"라면서 "이번 연구 결과는 외계행성의 대양에 관한 이해를 넓히는 중요하고 흥미로운 진전을 나타내는 것"이라고 평가했다. eomns@yna.co.kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>갤노트10 ‘LTE’가 쉽지 않은 이유는 ‘단통법’ 때문</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>ⓛ자급제 단말기 나와도 힘 못 써..이통사 유통점 구매 안 돼 ②이통사 약관 변경 해도 지원금 차별 금지 조항에 발목 ③삼성과 이통사 책임공방..단말기유통과 통신 가입 분리하면 해결 [이데일리 김현아 기자] 23일 삼성전자의 플래그십 스마트폰인 ‘갤럭시 노트10’이 공식 출시됐지만 5G 버전만 출시돼 이용자들의 불만이 커지고 있다. LTE 가입자들 중에서도 ‘갤노트10’을 쓰고 싶은 사람이 있는데, 굳이 비싼 5G에 가입해야 쓸 수 있다니. 올해 출시된 갤럭시S10은 LTE 버전과 5G 버전이 모두 출시됐는데, 노트10만 안 되는 것도 이해하기 어렵다는 반응이다. 갤노트 10을 LTE로 가입해 쓰기 어려운 이유 중 하나는 ‘단말기유통구조개선법’때문이라는 평가가 나온다. 단통법은 기본적으로 통신사유통점의 단말기 판매를 전제로 한 법률인데 이 때문에 ⓛ갤노트10은 주로 이통사 대리점·판매점에서 유통된다(삼성이 자급제향으로 5G칩과 LTE칩이 모두 들어간 갤노트10을 출시해도 이통사 유통점에서는 만날 수 없다는 점). 또 ②이통사에서 약관 변경을 통해 5G칩과 LTE칩이 모두 들어간 단말기(같은 모델)를 5G와 LTE로 나눠 가입시키는 것도 쉽지 않다(단통법상 지원금 차별 금지). 여기에 ③삼성과 이통3사 사이에서 갤노트 10 LTE 버전 출시 책임 공방이 일고 있다는 점(단말기와 통신이 분리되면 이런 논란이 사라짐)도 단통법의 부정적인 효과다. 삼성 갤럭시노트 10 ◇LTE 유심 가입 가능한 자급제 ‘갤노트10’ 조만간 출시 과학기술정보통신부에 따르면 삼성은 ‘갤노트10’ LTE 버전을 따로 내기는 쉽지 않지만, 자급제폰으로는 내놓겠다고 밝혔다. 만약 소비자가 온라인 마켓이나 전자제품 양판점 등에서 ‘갤노트10 5G버전’ 자급제폰을 산다면 LTE로 쓸 수 있다. 집에서 쓰던 단말기의 유심(USIM·가입자식별모드)칩을 꺼내 자급제로 산 갤노트10에 끼워 넣으면 된다. 이런 일이 가능한 것은 국내에서 출시되는 갤노트10 5G버전에는 5G칩과 LTE칩이 들어가 있는데, 국내 통신3사의 5G 통신망은 LTE연동형(NonStandAlone)이기 때문이다. 즉, 5G의 빠른 속도보다는 저렴한 요금제를 원한다면 자급제폰을 사서 LTE 유심을 끼워쓰면 된다. ◇자급제 갤노트10, 이통사 유통점에서는 불가능 하지만 자급제향으로 출시된, LTE 유심 가입이 가능한 ‘갤노트10’은 이동통신3사 유통점에서는 만날 수 없다. 자급제폰(언락폰)이란 이동통신사 대리점 방문 없이 기존에 사용하던 유심을 꽂아서 바로 사용 가능한 단말기이기 때문이다. 그러나 우리나라에서 소비자가 스마트폰을 사는 대부분의 장소는 이통사 대리점이나 판매점이다. 이처럼 단말기 판매와 통신서비스 가입이 결합돼 이용자의 선택권을 저해한다는 비판이 제기되자 국회에서는 단통법 폐지와 완전자급제 도입을 위한 입법 논의가 있었지만, 이동통신 유통업계의 반발로 좌절됐다. 완전자급제법은 통신사의 단말기 판매를 금지한 법으로, 김성태·박홍근·김성수 의원 등이 발의했다. ◇이통3사가 약관 변경해도 지원금은 똑같이 줘야 하는 문제 삼성은 이통사에 기술적으로는 가능하니 과기정통부에 약관 변경을 신청해 칩이 두 개인 ‘갤노트 10’을 5G 요금제와 LTE 요금제로 가입시키라고 제안하고 있다. 하지만 이통사들은 약관 변경을 신청한다고 해도 한 가지 모델에 대해 요금제 외에 다른 이유로 차별적인 지원금을 줄 수 없는 단통법때문에 어렵다는 입장이다. 단통법에는 이동통신 요금제에 따른 지원금 차이외에 5G냐 LTE냐에 따라 동일 단말기에 대해 지원금을 다르게 줄 수 있는 근거가 없다. 단통법을 개정해야 하는 것이다. 이통사들이 약관을 바꿔 5G와 LTE가 모두 되는 ‘갤노트 10’에 같은 공시 지원금을 준다해도 혼란이 불가피하다. 이통사들이 고가 요금제를 쓰는 5G 고객과 상대적으로 저렴한 요금제에 가입하는 LTE 고객에게 같은 지원금을 주는 걸 꺼리는 것은 물론, 공시 지원금은 같게 하고 유통점 장려금(리베이트)로 조절할 경우 단통법상 처벌받는 이용자 차별 행위(지역별 유통점별 단말기 가격의 현저한 차이)가 발생할 가능성이 높기 때문이다. ◇통신사 삼성 네탓 공방의 원인도 단통법 이런 이유로 이동통신3사는 삼성에 ‘갤노트10’ LTE 버전 출시를 요구하고 있다. 유럽이나 중국, 미국에 파는 LTE 전용 모델 같은 걸 국내향도 만들어 달라는 것이다. 미국과 중국에서는 5G 버전과 LTE 버전이 모두 출시된다. 그러나 삼성은 이통사에 유럽에서 파는 LTE 모델(899유로, 약120만8100원)과 한국에서 출시된 5G 모델(124만8500원)간 가격 차이가 크지 않고 생산라인 문제도 있다며 난색이다. 5G 모델은 5G칩과 LTE칩이 두 개 들어가 있어 원가를 보면 LTE 모델에 비해 비싸다. 즉 한국에서 노트10 LTE를 출시할 경우 유럽 판매 제품보다 저렴해야 하는데, 이 가격 차이가 클 경우 유럽 소비자들이 반발할 것이라는 게 삼성 주장이다. 이런 갈등도 단통법을 없애고 완전자급제가 실현되면 사라진다. 각자 자기 상품을 자기 계획에 맞춰 내고 소비자 반응을 책임지면 되기 때문이다. 통신 가입과 단말기 유통 분리가 소비자에게 이익이 된다는 사실이 이번 노트10 LTE 버전 출시 갈등에서도 증명됐다는 평가다. 김현아 (chaos@edaily.co.kr) 네이버 홈에서 ‘이데일리’ 뉴스 꿀잼가득 , 청춘뉘우스~ ＜ⓒ종합 경제정보 미디어 이데일리 - 무단전재 &amp;amp; 재배포 금지＞</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>[르포] `갤노트10` 공짜폰은 없었지만 `낚시성 마케팅`은 극성</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>신도림 집단상가 현장 탐방 갤럭시노트10 정식 개통 첫날인 23일 신도림 테크노마트 내 휴대폰 집단상가 모습. 김은지 기자 '갤럭시노트10' 예약판매 시 100만원 넘는 지원금이 난무했지만, 정식 출시 첫날인 23일 공짜폰은 찾아볼 수 없었다. 하지만 '공짜폰 코스프레'는 만연했다. 지원금 내역을 따져보면 공짜폰이 아님에도 고객 유치를 위해 '공짜폰' 마케팅을 하는 사례를 심심치 않게 찾을 수 있었다. 일종의 '낚시성 마케팅'인 셈이다. 할인 내역에 대한 안내가 미진하거나 실질적으로 연 360만원의 신용카드 사용 금액(카드 제휴·결합 할인)을 감수해야 하는 상황에서 '기기값 0원'이라는 단어를 어렵지 않게 만날 수 있었다. 삼성전자의 전략 스마트폰인 갤럭시노트10이 23일 정식 출시됐다. 사전 예약 물량만 이미 역대 최고치인 130만대를 넘어서면서 서울 신도림 테크노마트 내 휴대폰 집단상가는 예상보다는 한산했다. 이날 취재는 대표적인 스마트폰 성지에서 '갤럭시노트10을 얼마나 초단가로 살 수 있는지' 궁금증을 해소하기 위해 진행됐다. 우선, 방문객이 많이 없다 보니 등장부터 많은 호객행위에 노출이 됐다. 상가에 들어서자마자 "고객님 알아보셨어요?", "어떤 것을 찾으세요?"라는 물음이 끊임없이 이어졌다. 집단상가 등 일부 유통점은 차별적 리베이트 지급에 대한 방송통신위원회의 단속이 집중될 수 있는 곳이다. 방통위 단속을 의식해 "얼마에 알아보고 왔다", "XX만원에 정말 살 수 있냐"라고 말하는 것은 금기어. "무조건 가장 싸게 사려 하면 어떻게 하냐?"라고 물으면 말없이 계산기에 숫자를 쳐서 보여주는 방식으로 상담이 진행됐다. 다만 기대와 달리, 불법 보조금으로 문제가 됐던 10만원 미만 갤럭시노트10 폰을 찾는 것은 쉽지 않았다. 아예 고객이 없는 상점도 절반 정도. 그나마 1~2명씩의 사람이 방문한 상점은 '갤럭시노트10 0원' 혹은 '갤럭시노트10 사전예약 현금 완납' 등의 홍보 문구를 붙여놓은 곳이었다. 초단가에 스마트폰을 구매하려면 이 같은 문구를 붙여놓은 상점을 최대한 돌아다니고 시세를 비교해야 했다. 많은 곳을 돌아다닐수록 싼 값을 제시받는 데 요령이 생겼다. "옆집에 갔는데 생각보다 비싸게 부른다. 무조건 싸게 갤럭시노트10을 사고 싶다"는 말에 기기가 "공짜"라는 말은 빈번하게 돌아왔다. 여러 상점들이 제시한 초단가 조건은 SK텔레콤 고객인 기자가 번호이동(LG유플러스)에 특정 신용카드 사용할 시 기기값은 0원, 7만5000원(스탠다드,150GB 제공) 가량의 요금만 내도록 맞춰준다는 것이었다. 다른 부가 조건들은 설명하지 않았지만, 월 20~30만원 상당의 특정 신용카드 사용금액을 지켜줘야 한다는 설명도 덧붙였다. 가전을 할부로 구매하거나 공과금 자동이체를 걸어놓거나 하는 방식으로 카드를 이용하면 된다는 것이다. 이 조건의 약정은 24개월이고 갤럭시노트10과 마찬가지로 신용카드 또한 24개월 동안 사용을 유지해야 한다. 보조금이나 공시지원금에 대한 언급은 없었다. 일단 '기기값 0원'을 내세워 실적을 올리는 데만 집중하는 모습이었다. 신용카드사의 마케팅인지 스마트폰 마케팅인지, 초단가에 구매를 할 수 있다는 점은 흥미로웠지만 의아함은 가시지 않았다. 결국 배보다 배꼽(늘어나는 신용카드 사용금액)이 클 수 있구나 하는 생각이 머리를 스쳐갔다. 연 360만원의 신용카드 지출은 갤럭시노트10 일반형 256기가바이트(GB) 출고가 124만8500원의 배가 넘는 금액이다. 갤럭시노트10 아우라 글로우 신용카드와 결합된 방식 외에 '휴대폰 반납을 통한 기기값 0원' 마케팅도 만날 수 있었다. 5GX클럽 노트10 혜택을 활용하는 등의 방식인데, 이를 통해 갤럭시노트10 가격을 할인 받을 수 있었다. SK텔레콤 '5GX클럽_노트10'은 고객이 단말 구매 12개월 뒤 사용하던 제품을 반납 후, 다음 갤럭시 시리즈를 구매할 때 출고가의 최대 50%를 면제받을 수 있는 프로그램이다. 상담 고객이 구체적으로 묻기 전에는 이 같은 프로그램명을 제대로 설명하지는 않았다. 안내 미진으로 인한 '호구 고객(호갱)'을 만들 수 있는 요소였다. 실제 스마트폰 구매가 아닌 '렌탈'이 아니냐며 불만을 토로하는 이도 있었다. 또 이날 초단가를 제시하는 상점을 찾을수록 "지금 기기 개통을 할 것인지"를 묻는 횟수가 늘어났다. 현재 사용 중인 스마트폰의 약정이 남아있고 위약금액이 30~40만원 가량인 덕에 당장 개통은 피할 수 있었다. 한 상인은 위약금에도 불구하고 개통을 한다면 갤럭시노트10 '핑크' 색상을 사용할 것을 권했다. 시그니처 색상인 '아우라글로우'를 쓰고 싶다 말했지만, 품귀현상 때문에 물량 확보가 쉽지 않다는 설명이다. 아우라 화이트도 당일 구하기 어려울 수 있다는 답이 돌아왔다. 이동통신사별 특화 색상인 SK텔레콤 갤럭시노트10 블루, KT 갤럭시노트10 레드도 사전 예약 고객들을 위해 물량이 묶여 있었다. 한편 이날 갤럭시노트10 정식 개통 시작과 아울러, 갤럭시S10 5G를 찾고 상담하는 사람들의 모습도 많이 볼 수 있었다. 또 다른 상인은 "갤럭시S10 5G의 조건이 나쁘지 않아 오히려 지금이 갤럭시S10 5G 구매 적기"라면서 "노트 시리즈와 S시리즈의 팬층이 극명히 나뉘기 때문에 S시리즈를 찾는 사람들의 발걸음도 여전하다"고 설명했다. 김은지기자 kej@dt.co.kr /</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>대란 없는 갤노트10…일반 판매 첫날 ‘잠잠'</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>집단상가, 실구매가 40만원대…이달 말까지 안정화 추세 예상 (지디넷코리아=선민규 기자)대란은 없었다. 갤럭시노트10 공식 출시 첫 날 시장은 잠잠한 분위기를 이어가고 있다. 갤럭시노트10이 사전 개통을 마치고 일반 판매를 시작한 23일, 이른바 ‘성지’로 알려진 집단상가는 비교적 한산한 모습이었다. 판매자들은 지나가는 방문객에게 연신 말을 걸었고, 발길을 멈춘 방문객도 가격을 듣고선 발길을 돌리기 일쑤였다. 서울시내 휴대폰 집단상가 내 판매점은 출고가 124만8천500원인 갤럭시노트10의 실구매가로 40만~50만원대를 제시했다. 이는 제품 출고가에 비해 70만원 가량 낮은 금액이지만, 올 상반기와 같은 대란을 기대했던 구매자들의 기대에는 못 미치는 수준이다. 삼성전자 갤럭시노트10과 갤럭시노트10 플러스.(사진=삼성전자) 집단상가 판매점 관계자는 “5G 스마트폰이 처음 나왔을 당시와 비교하면 방문자가 많이 없는 편”이라며 “노트10 가격에 대해 문의만 하고 돌아가는 경우가 많다”고 말했다. ■ 이통3사, 5G 가입자 보다 ‘시장 안정화’ 초점 단말기를 저렴한 가격에 구매할 수 있는 기회를 일컫는 ‘대란’은 유통점 및 대리점이 본사로부터 지급받는 리베이트에 따라 좌우된다. 리베이트 금액이 높을수록 소비자에게 더 많은 할인을 제공할 수 있기 때문이다. 이통3사는 시장 안정화로 방향을 잡았다. 시장 안정화는 일선 유통판매점에 지급하는 리베이트를 줄이는 방식으로 유도할 수 있다. 이통3사는 시장 과열을 피하고자 보조금 기준 및 영업점에 부과하는 페널티를 강화하는 등 선제적 조치에 나섰다. 이는 통신 시장 과열을 점검하는 방송통신위원회의 긴급 상황반을 의식한 움직임이다. 긴급 상황반은 신규 단말기 출시를 전후해 시장 과열을 점검하는 조직이다. 23일 서울 시내 휴대폰 집단상가의 모습. 상반기 과도한 마케팅 경쟁이 실적에 악영향을 미쳤다는 점과 5G 가입자가 안정화 추세에 접어들었다는 점 등도 이통 3사의 전략 수정 배경으로 꼽힌다. 실제로 지난 22일 박종욱 LG유플러스 PS부문 전무는 “경쟁사가 보조금(리베이트) 지급을 통한 출혈 경쟁을 시작해도 우리는 경쟁 참여를 지양할 것”이라며 “보조금 중심의 경쟁에서 서비스 중심으로 시장이 변화하는 것이 맞다고 생각한다”고 말하기도 했다. ■ 대란 없이 노트10 순항 중 대란은 없었지만 노트10 판매는 순항하고 있다. 집단상가나 온라인이 아닌 일반 소매 대리점의 단말기 판매가 늘고 있다는 점이 특징이다. 유독 저렴한 가격에 단말기를 판매하는 성지가 사라지면서, 접근성에서 강점이 있는 일반 소매 대리점의 판매량이 높아진 것으로 풀이된다. 통신업계 관계자는 “이제 일반 판매가 시작된 탓에 구체적인 판매량을 집계하긴 어렵지만, 예약 판매 성적과 시장 분위기를 봤을 때 전작에 비해 좋은 것은 사실”이라며 “올 상반기 출시된 5G 스마트폰에 비해 노트10은 소매 대리점에서 개통하는 비중이 높다”고 말했다. 종각역직영점에서 갤럭시 노트10 5G 사전예약자가 개통을 진행하는 모습.(사진=LG유플러스) 제품에 대한 호평과 상반기에 비해 개선된 5G 네트워크 품질도 판매량 증가를 이끈 것으로 풀이된다. 소매 대리점 관계자는 “노트10의 성능을 고려할 때, 가격 부담을 감당하는 것이 옳다는 공감대가 만들어지고 있는 것 같다”며 “다소 불안했던 5G 상용화 초기와 달리 현재는 커버리지와 네트워크 품질 면에서 상당히 안정화됐다는 점도 판매량 증가에 영향을 미쳤을 것”이라고 설명했다 시장 안정화 흐름은 최소 이달 말까지 유지질 것으로 예상된다. 통신업계 관계자는 “정부의 규제 상황을 생각할 때, 최소 이달 말까지는 시장 안정화 추세가 이어질 것”이라며 “다만 추석 연휴를 전후해 시장이 과열될 가능성도 배제할 수는 없다”고 말했다. 선민규 기자(sun1108@zdnet.co.kr) /</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>삼성전자, 반도체·무선사업부 성과급 절반으로 줄듯</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>가전사업부는 올해와 비슷한 수준으로 공지 반도체 시황 부진, 스마트폰 성장세 둔화 등으로 삼성전자의 영업이익이 급감하면서 내년 초 직원들에게 지급될 성과급도 올해 초 대비 절반 수준에 그칠 전망이다. 23일 업계에 따르면 삼성전자는 전날 직원들에게 내년 초 지급되는 사업부별 초과성과인센티브(OPI) 예상 지급률을 공지했다. 각 사업부의 1년 성과가 연초 사업 목표를 초과했을 경우 개인 연봉의 최대 50%를 OPI로 지급한다. 매년 1월쯤 나온다. 삼성전자 직원들이 서울 서초구 삼성전자 사옥에 들어가고 있다./연합뉴스 올해 초 최대치인 50% 내지 이에 근접한 수준의 OPI를 받았던 디바이스솔루션(DS)부문은 메모리·비메모리 사업부(시스템LSI·파운드리)를 통틀어 22~30% 수준에서 성과급이 지급될 것으로 예상됐다. 스마트폰을 담당하는 IT·모바일(IM)부문 무선사업부는 24∼28% 수준, 네트워크사업부는 이보다 높은 31∼39%가 예상됐다. IM부문의 올 초 OPI는 최대 46%였다. 소비자가전(CE)부문은 올해 초와 비슷한 수준이 될 것으로 알려졌다. 생활가전사업부는 연봉의 23∼24%, 영상디스플레이(VD)사업부는 최대 42% 수준으로 공지됐다. 지난해에도 CE 부문 성과급은 가전사업부와 VD사업부가 각각 23%, 46% 수준이었다. 삼성전자 관계자는 "각 사업부문별 OPI 예상 지급률이 공지된 것은 사실이지만 구체적인 수치를 확인해줄 수는 없다"면서 "현재 시점에서 산정한 지급률이기 때문에 하반기 실적에 따라 약간의 변경 여지는 있다"고 말했다. [장우정 기자 woo@chosunbiz.com] chosunbiz.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>조국 딸 '금수저 스펙' 뒤엔 '엄마의 서울대 동아리 네트워크' 있다?</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>조국 딸 관련 논란된 공주대 K교수..조국 부인과 서울대 81학번 동기 조국 부인 학창 시절 활동한 서울대 천문동아리 AAA가 연결고리 조국 법무부 장관 후보자가 23일 오후 서울 종로구 적선현대빌딩에서 논란이 일고 있는 사모펀드와 사학재단 웅동학원을 사회에 환원하겠다고 밝히고 있다. 2019.8.23/뉴스1 © News1 안은나 기자 (서울=뉴스1) 최소망 기자 = 조국 법무부 장관 후보자의 딸이 한영외고 재학 중 공주대에서 인턴을 하고 국제학술대회 발표초록에 제3저자로 이름을 올린 것이 특혜가 아니냐는 의혹이 제기된 가운데 공주대와 조국 가족의 연결고리로 서울대 천문 동아리인 '아마추어 천문회'(AAA)가 주목받고 있다. 23일 과학기술계에 따르면 조국 후보자 딸(28)은 2009년 공주대 생명과학과 K교수실에서 2주가량 인턴을 하고 국제학회 발표문에 제3저자로 이름을 올렸다. 당시 K교수는 조 후보자의 아내 정 씨의 대학 동기다. 정 씨와 K교수는 1981년 서울대 영어영문학과와 식물학과에 각각 입학했다. 소속과가 다른 이들은 서울대 재학시절 천문 동아리에서 같이 활동한 인연이 있는 것으로 알려졌다. 서울대에는 1980년부터 시작된 유서 깊은 아마추어 천문회(Amateur Astronomy Association·AAA) 동아리가 있다. 이름 그대로 취미로 천문활동을 하는 동아리로 해마다 천체 사진전을 열어 1년간 동아리원들이 찍은 천체사진을 엄선해 전시하는 활동을 한다. 천문회 동아리에서 맺은 어른들의 '인연'이 조국 딸의 '금수저 스펙'의 진원지 역할을 한 셈이다. 실제로 K교수는 한 언론에 "대학 동기인 조 후보자의 부인인 정 씨가 자기 딸 면접을 보는데 충남 공주까지 같이 왔다니까 놀랐다"며 동기라는 사실을 인정했다. 이를 두고 서울대생 전용 포털사이트인 스누라이프(SNULIFE)에는 "나도 AAA인데 내 자식 논문은 동아리 동기에게 맡겨야겠다", "AAA인맥이 이렇게도 활용되네요", "AAA출신인데 자괴감 느낀다" 등의 의견이 올라오기도 했다. 조국 후보자의 딸 조 씨의 단국대 논문 제1저자 논란이 일었을 때도 논란 직후에는 서울대 물리천문학과의 A교수가 조국 딸와 관련한 의혹에 대해 옹호하는 발언을 해 주목을 받기도 했다. A교수는 조국 법무부 장관 후보자 딸의 논문 논란과 관련 지난 21일 "딸도 부모도 책임이 없어 보인다"면서 "만약 문제가 된다면 결국 지도교수의 책임"이라고 밝혔다. 이어 "조국 교수가 자기 딸을 제 1저자로 넣어달라고 부탁했다면 명백한 잘못이지만 밝혀지지 않는 한 부모의 잘못을 논하기는 어렵다"고도 했다. 이외에도 조 양이 과거 한영외고 재학 시설 서울대 물리천문학부 B교수의 지도를 통해 한국물리학회에서 수여하는 물리캠프 장려상을 받은 것까지 회자된다. 조 씨는 2009년 8월 한국물리학회(KPS) 여성위원회가 숙명여대에서 개최한 '여고생 물리캠프'에 참가해 다른 학생 2명과 함께 '나비의 날개에서 발견한 광자 결정구조의 제작 및 측정'이라는 연구과제를 수행해 장려상을 받았다. 해당 캠프에서 2005년부터 현재까지 장려상을 시상한 해는 2009년이 유일해 일부러 상을 만들어준 게 아니냐는 의혹이 제기됐다. 과기계 관계자는 "조국 부인이 천문 동아리에서 활동했고 당시 동문들이 현재 서울대 물리천문학부 교수직에 포진해 있다"며 "조국 후보자의 딸과 관련해 제기되는 '금수저 스펙'에 '엄마의 서울대 AAA 네트워크'가 고스란히 담겨 있는게 아니냐"고 말했다. 이와관련 AAA는 "기사에 언급된 분들은 현재 동아리에서 보유한 연락처 목록에 기재조차 돼있지 않다"고 밝혔다. somangchoi@news1.kr [© 뉴스1코리아(), 무단 전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>바이오株 악재 속 글로벌신약 자신감··“SK바이오팜 연내 IPO”</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>뇌전증 신약인 ‘세노바메이트’ 美FDA 11월 판매허가 앞두고 SK㈜이사회, 상장 안건 가결 11월말 이후 공모 가능성 커 ‘솔리암페톨’ 등 파이프라인 다양 기업가치 5조원 안팎 달할 듯 [서울경제] 뇌전증 신약 세노바메이트의 미국 식품의약품청(FDA)의 신약판매 허가를 앞둔 SK바이오팜이 연내 기업공개(IPO)를 추진한다. 증권업계는 다양한 신약 파이프라인을 확보한 SK바이오팜의 기업가치가 5조원 안팎에 달할 것으로 추산한 바 있다. 상반기부터 계속된 제약 바이오업계 악재들로 투자 심리가 한층 위축된 가운데 올 하반기 IPO 시장 최대어로 꼽혔던 SK바이오팜이 상장에 나서면서 제약바이오업계에 분위기 반전을 몰고 올지 주목된다. 24일 업계에 따르면 SK㈜는 지난달 이사회를 열어 SK바이오팜의 상장 추진 안건을 가결해 기업공개 관련 절차를 진행했다. 이는 SK㈜가 일정 지분을 보유한 자회사의 상장을 추진할 때 이사회 의결을 거쳐야 하는 규정에 따른 것이다. 지난해 미국 나스닥 직상장을 추진했던 SK바이오팜은 올해 초 코스피로 눈을 돌려 지난 4월 기업공개 대표 주관사로 NH투자증권을, 공동주관사로 한국투자증권을 각각 선정한 바 있다. SK바이오팜은 SK㈜ 이사회 절차를 마무리한 만큼 조만간 거래소에 상장예비심사를 청구할 것으로 예상된다. 업계에서는 SK바이오팜의 상장 추진이 독자 개발한 뇌전증 신약 ‘세노바메이트’에 대한 자신감에서 비롯된 것이라고 해석하고 있다. 앞서 미 FDA는 지난 2월 세노바메이트의 허가심사를 시작했으며, 약 10개월의 검토 기간을 거쳐 오는 11월21일 허가 여부를 결정할 계획이다. 이미 S K바이오팜은 세노바메이트의 미국 마케팅을 위해서 현지에 의약품 판매법인 SK라이프사이언스를 설립해 놓은 상태다. SK㈜ 관계자는 “상장 시점은 시장 환경 등을 고려해 최적의 시점에 추진한다는 입장”이지만 공모가 등을 고려해 세노바메이트의 미국 FDA 승인 직후가 될 공산이 크다. 지난 2011년 출범한 SK바이오팜은 상대적으로 짧은 역사에도 글로벌 신약 시장에서 두각을 나타내며 우리나라를 대표하는 바이오 업체로 자리 잡았다는 평가를 받고 있다. SK바이오팜은 통상 신약을 개발해 국내에 먼저 출시한 뒤 미국·유럽 등 선진시장에 진출하는 것이 아니라 연구개발(R&amp;amp;D) 단계부터 미국 시장을 염두에 두고 신약 개발에 나서는 전략을 펴고 있다. 실제로 SK바이오팜은 지난달 8일부터 자체 개발해 기술수출한 수면장애 신약 ‘솔리암페톨’의 미국 판매를 시작했으며 글로벌 시장을 염두에 두고 소아희귀뇌전증 치료제 ‘카리스바메이트’, 희귀 신경계질환 치료제 ‘렐네노프라이드’를 개발하고 있다. 이밖에 집중력장애 치료제 SKL13865와 조현병 치료제 SKL20540 등도 개발 중이다. 증권업계 관계자는 “각종 악재로 바이오 업종에 대한 투자심리가 한층 꺾인 상황”이라며 “올 하반기 IPO 최대어로 주목받았던 SK바이오팜이 신약 허가에 대한 자신감을 등에 업고 높은 가치를 인정받을 경우 제약바이오 업계를 바라보는 투자심리에 긍정적인 영향을 미칠 수 있을 것”이라고 말했다. /박홍용기자 prodigy@sedaily.com | 저작권자 ⓒ 서울경제, 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>[우주를 보다] 인류 피조물과 첫 조우한 해왕성…30년 전 보이저 2호 포착</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>[서울신문 나우뉴스] 해왕성(왼쪽)과 트리톤의 사진. 출처=NASA/JPL-Caltech 지금으로부터 정확히 30년 전인 지난 1989년 8월 25일, 인류의 피조물이 사상 처음으로 태양계 8번째 행성의 근접 사진을 촬영했다. 촬영자는 미 항공우주국(NASA)의 태양계 탐사선 보이저 2호(Voyager 2) 그리고 대상은 이제는 태양계 끝 행성이 된 해왕성이다. 지난 22일(현지시간) NASA는 해왕성 탐사 30주년을 맞아 당시 보이저 2호가 촬영한 해왕성 사진을 홈페이지에 공개했다. 해왕성의 신비로운 모습이 인상적인 이 사진은 당시 보이저 2호가 약 700만㎞ 떨어진 지점을 지나가며 카메라에 담은 것이다. 해왕성은 태양을 기준으로 무려 45억㎞나 떨어져 있어 관측이 대단히 어렵다. 이 때문에 보이저 2호가 남긴 해왕성 사진은 천문학 역사에 길이 남을 정도의 쾌거였다. 보이저호의 상상도 이 사진과 더불어 보이저 2호는 방향을 살짝 틀어 해왕성의 가장 큰 달인 트리톤(Triton)의 모습도 생생히 잡아냈다. 해왕성의 13개 위성 중 가장 큰 트리톤(지름 2707㎞)은 자전축과 공전방향이 반대인 역행위성이다. 이 때문에 전문가들은 ‘카이퍼 벨트’(Kuiper Belt·해왕성 궤도 밖의 천체가 도넛 모양으로 밀집해 있는 지역)에 있던 트리톤이 해왕성의 힘으로 끌려 온 것으로 추측하고 있다. 이렇게 태양계 행성 탐사를 모두 마친 보이저 2호는 지난해 12월 보이저 1호에 이어 태양권 경계를 넘어 성간 우주에 도달했다. 현재 태양에서 약 180억㎞ 떨어진 심(深)우주를 비행 중으로 누구도 가보지 못한 전인미답의 경지에 오른 셈이다. 박종익 기자 pji@seoul.co.kr ★ ▶ ⓒ 서울신문(www.seoul.co.kr), 무단전재 및 재배포금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>[리뷰] '미(美)친 화질과 응답속도' LG 울트라기어 27GL850</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>게임을 즐기기 위해 준비하는 아이템에 대한 관심사가 다양해지고 있다. 과거에는 성능 위주였다면 최근에는 주변기기에도 관심을 두는 모습이다. 키보드, 마우스, 헤드셋 등 다양하지만 디스플레이에 대한 관심도 높아지는 추세다. 게이밍 환경이 고해상도와 고주사율 등 경험 위주로 발전하고 있기 때문이다. LG 울트라기어 27GL850. (출처=IT동아) 화려한 그래픽과 사운드, 조작감 등으로 다양한 짜릿함을 주는 게임. 다양한 장르가 존재하는데 국내에서 인기를 얻고 있는 주요 게임들은 민감한 조작이 필요한 것들이 많다. 리그 오브 레전드, 피파온라인, 배틀그라운드, 오버워치, 패스 오브 엑자일 등만 봐도 그렇다. 적이 어디에 있는지 빠르게 판단하고 민첩하게 키를 입력해 승리를 거머쥐어야 한다. 1초 이하의 찰나에 승패가 결정될 정도로 빠른 입력이 중요한 게임들이 최근 많아지고 있다. 이런 상황에서 방해 받는 요소는 바로 디스플레이. 게임은 입력과 출력이 실시간으로 이뤄지는 과정을 반복하게 되는데, 이 과정에서 미세하게나마 지연이 생긴다. 이를 '입력지연(Input Lag)'이라 부른다. 이를 막기 위해 많은 노력을 기울이는데, 모니터 또한 여기에 포함된다. 최근 게이밍 모니터들은 입력 지연을 줄이기 위해 화면 응답속도를 줄이고 있다. 일반적으로 3~5밀리초(ms) 정도면 빠른 것으로 분류된다. 하지만 이를 뛰어 넘는 1ms에 도달한 게이밍 모니터가 있다. 바로 LG 울트라기어 27GL850이 그것. 이 모니터는 1초에 화면이 144회 깜박이는 나노 IPS 디스플레이를 채택하면서 풍부한 색감과 고해상도(QHD – 2,560 x 1,440)를 구현했다. 엔비디아 지싱크 호환(G-SYNC Compatible)을 공식 지원하는 것도 특징이다. 게이밍 모니터 다운 완성도 돋보여 LG 울트라기어 27GL850의 디자인은 그간 LG 게이밍 모니터들과 비슷한 모습이다. 검은색과 붉은색을 적절히 조합했고, 외모를 날카롭게 다듬어 강한 인상을 준다. 이 모니터 역시 유광 재질을 최대한 배제해 묵직함을 더했다. 화려함을 강조한 효과는 없다. 흔히 고가의 게이밍 모니터는 LED 효과를 넣어 눈부시게 만들기도 하는데, 화면에 집중 가능하도록 불필요한 요소는 뺐다. LG 울트라기어 27GL850. (출처=IT동아) 모니터의 면적은 27인치(68.6cm) 정도. 화면이 휘어지지(커브드) 않은 평면이며 화면 테두리가 얇아 실제 보면 27인치보다 조금 더 작아진 듯한 인상이다. 실제 화면 테두리의 두께가 얇다. 하단을 제외하고 상단이 mm, 양쪽 측면이 mm에 불과하다. 화면이 시원하게 펼쳐져 있어 보는 맛이 좋다. 스탠드를 장착한 상태에서의 모니터 크기는 폭 614.2mm, 높이 574.8mm 정도이며, 모니터 자체의 두께는 약 56.3mm 정도다. 스탠드는 Λ 형상으로 자리만 충분하다면 모니터의 균형을 잘 잡아준다. 장착 자체도 간단하다. 모니터 하단에 있는 고정 홈에 스탠드 머리 부분을 끼워 넣기만 하면 된다. 스탠드 기능도 매력적이다. 기본적으로 높낮이 조절(Height), 모니터 각도를 앞뒤로 조절하는 틸트(Tilt), 화면을 90도 돌릴 수 있는 피벗(Pivot)을 지원한다. 모니터를 좌우로 돌리는 스위블(Swivel)은 지원하지 않는다. 모두 사용에 도움을 주는 기능들이다. 이로 인해 모니터 몸값이 상승하겠지만 사용성 측면에서 보면 이점이라 하겠다. 다양한 영상 입력 및 주변기기 확정성을 위한 단자가 제공된다. (출처=IT동아) 연결부 구성도 충실하다. HDMI 단자 2개, 디스플레이 포트 1개를 포함해 PC에 연결하기 위한 B 규격의 USB 단자(USB 2.0) 1개, 주변기기 연결을 위한 A 규격 USB 단자(USB 3.0) 2개가 배치된다. 헤드폰 연결을 지원하는 3.5mm 스테레오 단자도 포함된다. 이런 구성이면 PC와 콘솔 게임기 등 여러 출력 장치에 연결하는 것이 가능하다. 지싱크 호환 기술을 사용하려면 디스플레이 포트를 활용해야 된다. HDMI 단자는 전송 대역의 한계로 지원하지 않기 때문이다. 사용하지 않는다면 어떤 단자를 써도 무방하다. '지싱크 호환 + 1ms'로 민첩하고 부드러운 게이밍 경험 제공 LG 울트라기어 27GL850의 특징을 정리해보면 이렇다. 우선 ▲ 나노 IPS 디스플레이 적용 ▲ 1밀리초(ms) 수준의 응답속도 ▲ 엔비디아 지싱크 호환 기술 대응 ▲ 144Hz 고주사율 적용 등이다. 이 같은 구성은 게이밍은 물론, 함께 다양한 환경에서 최적의 경험을 제공하는데 도움이 된다. 흔히 게이밍 모니터는 뒤틀림 전환(TN – Twisted Nematic) 혹은 수직 전계식(VA – Vertical Alignment)을 쓴다. 반면, 이 모니터는 평면내 전환(IPS – In-Plane Switching) 구조를 적용한 것이 특징이다. LG 울트라기어 27GL850. (출처=IT동아) IPS 디스플레이는 액정이 수평으로 구동되는 원리를 이용하고 있다. 넓은 시야각과 빠른 응답속도 등이 장점으로 꼽힌다. 여기에 LG는 나노단위의 화점을 더해 색상을 더 정확하게 표현할 수 있도록 설계했다. 나노 IPS 디스플레이는 넓은 시야각을 자랑한다. 색반전 현상이 적은 편이다. (출처=IT동아) 그 덕에 모니터는 넓은 색영역을 지원한다. 디지털 영화협회(DCI)의 색역인 DCI-P3 98%, 일반 색역인 sRGB 135%에 대응한다. 색조와 명암 등을 넓게 표현할 수 있는 고관용도(HDR – High Dynamic Range)도 지원한다. 여기에 넓은 시야각이 더해지니 눈이 즐겁다. 명암비는 1,000대 1로 VA 혹은 TN 패널 기반의 모니터에 비하면 부족하지만, 밝기는 평균 350 칸델라(cd/㎡) 정도로 오히려 밝다. 색상 표현력은 HDMI 단자를 썼을 때 8비트(1,670만), 디스플레이 포트를 썼을 때 10비트(10억)까지 표현 가능하다. 시야각을 보니 만족스럽다. 제원은 178도 정도인데, 실제 좌우에서 봤을 때 색반전 현상을 거의 느끼기 어려울 정도다. 무리하게 측면에서 바라보면 색반전이 있지만 일상적인 환경이라면 문제는 없다. 개인이 쓰는 모니터지만 타인이 영상을 관전하거나 작업 내용을 확인할 때, 최대한 정확한 색상을 경험할 수 있다는 부분은 장점이라 하겠다. PC와 모니터를 디스플레이 포트에 연결한 다음, 윈도 바탕화면에서 엔비디아 제어판을 불러오면 지싱크 호환 설정이 가능하다. (출처=IT동아) LG 울트라기어 27GL850의 또 다른 특징은 가변 주사 동기화(Adaptive-Sync) 기술에 대응한다는 것. 이 제품 역시 엔비디아의 '지싱크 호환(G-SYNC Compatible)'의 인증을 받았다. 프리싱크를 지원하는 일부 중소기업 모니터가 지싱크 호환에 대응한다는 것과는 차원이 다르다. 엔비디아가 직접 모니터에 대한 품질 테스트를 진행했고, 이를 통과했기 때문에 공식 인증을 받았다. 엔비디아 홈페이지 내에도 공식 등록되어 있다. 지싱크 호환 기술을 활성화하는 방법은 이렇다. 우선 지포스 10 시리즈 이상 그래픽카드 장착 및 그래픽카드 드라이버는 최소 417.71버전 이상이어야 한다. 추가로 PC와 모니터 연결은 디스플레이 포트(DP) 케이블을 사용해야 된다. HDMI 케이블로는 대응하지 않는다. 이상 조건을 만족했다면 윈도 바탕화면 내에서 마우스 우클릭 후 '엔비디아 제어판'을 불러오자. 제어판을 보면 좌측에 'G-SYNC 설정'이 활성화 되어 있는데 이를 클릭하면 된다. 지싱크 호환 설정은 기본적으로 활성화가 활성화된 상태다. 여기에서 사용자는 전체 화면에서만 쓸지, 창 모드와 전체화면 등 대부분의 상황에서 지싱크 호환을 쓸지 여부를 확인하면 끝이다. 가변 주사 기술인 엔비디아 지싱크 호환에 대응, 게임을 즐길 때 부드러운 화면을 보여준다. (출처=IT동아) 지싱크 호환 기술이 된다면 자연스레 AMD 프리싱크 기술도 지원한다. 타 지싱크 호환 모니터와 마찬가지로 실제 라데온 그래픽카드에 모니터를 연결했더니 드라이버 내에서 프리싱크 활성화가 되어 있음을 확인할 수 있었다. 작동도 잘 된다. 전환 범위는 48에서 144Hz 사이다. 이는 곧 1초에 48매 이상 이미지가 표현되는 환경이라면 끊김 없이 부드러운 화면 전환을 지원한다는 의미다. 실제 게임을 즐겼을 때의 만족감은 높다. 초당 144회 깜박이는 모니터라는 점도 좋지만 가변 주사 동기화 기술(엔비디아 지싱크 호환)에 의한 부드러운 화면이 압권이라 해도 과언이 아니다. 기본적으로 초당 48매 이상 표시되는 환경이 유지되어야 한다는 한계는 있지만, 일정 성능 이상 나오는 게이밍 PC라면 쉽게 달성 가능한 부분이기 때문에 큰 문제라 보기 어렵다. 무엇보다 이것이 유지되면 눈에 가해지는 스트레스가 줄어든다. IT동아 내에 준비되어 있는 라이젠5 3600 프로세서와 라데온 RX 5700, 지포스 RTX 2060 슈퍼 등 그래픽카드로 구성된 게이밍 PC로 게임을 즐겨보니 그래픽 옵션을 높여도 끊김을 느낄 수 없었다. 무엇보다 반응 속도가 인상적이다. 사실, 일정 이하의 응답 속도라면 크게 느끼기 어렵지만 민감한 반응성이 필요한 게임에서는 입력 지연이 느껴질 수 밖에 없다. 1ms 정도라면 거의 바로 출력되는 수준. 이에 기자가 가끔 즐기는 리듬게임 '탭소닉 볼드'를 실행, 게임을 즐겨보니 부드러운 화면 전환도 그렇지만 입력에 따른 스트레스를 거의 느끼지 못했다. 실력의 한계로 실수가 생길 수 있어도 입력 지연에 따른 판정 실수는 거의 드물다는 이야기다. 배틀그라운드를 즐겼을 때도 동일한 인상을 받았다. 과거 즐겼던 환경에서는 입력에 따른 지연이 조금씩 느껴졌지만 LG 울트라기어 27GL850으로는 키를 입력하는 것과 거의 동시에 반응이 온다. 자연스레 입력에 대한 스트레스 없이 게임에 몰입할 수 있게 된다. 물론, 이를 가지고 치킨을 먹을 수 있느냐 없느냐는 별개의 문제다. 가격은 높지만 완성도는 기대 이상 LG 울트라기어 27GL850. 화면이 초당 144회 깜박일 정도로 높은 주사율, 1ms의 빠른 반응 속도, 광시야각 등 장점이 많다. 스탠드 활용성도 높다. 높낮이 조절은 기본이고 수직으로 세운 뒤 동일한 모니터 2~3개를 배치해 더 넓게 볼 수 있다. 지싱크 호환 기술의 대응은 게임을 더 부드럽게 즐기는데 도움이 된다. 여러모로 게이머를 위한 기능에 집중한 것이 이 모니터의 강점이라 하겠다. 영상이나 기타 작업을 할 때에도 이점이 있다. 나노 IPS 디스플레이 특유의 색표현 능력도 그렇지만, LG가 생산 단계에서 최적의 색상을 조율해 내보내기 때문에 기본 이상의 실력을 보여준다. 전문가용 모니터처럼 제품 내용물에 관련 결과표를 제공한다. 나노 IPS 디스플레이 덕에 영상 감상이 더 즐겁다. (출처=IT동아) 아쉬운 점이 있다면 가격. 여러 이점이 있다 하더라도 누구나 쉽게 접근할 수 없다면 매력이 떨어진다. 차라리 모니터 스탠드의 기능을 제한하거나 영상 입력 단자를 줄이는 식으로 가격을 조금 더 낮췄으면 좋겠다는 생각이 든다. 또한 지싱크 호환이라는 부분을 명확히 표기해 주면 소비자가 혼동을 최대한 줄일 수 있을 듯 하다. 그러나 이는 엔비디아의 문제이지 LG의 문제는 아니다. 게임을 즐기는 방법은 다양하다. 하지만 제대로 즐기기 위한 방법은 많지 않다. LG 울트라기어 27GL850은 그 해답 중 하나가 되지 않을까 예상해 본다. 1ms 반응속도와 144Hz 주사율, 지싱크 호환 등 많은 것을 한 번에 누리기 쉽지 않아서다. 동아닷컴 IT전문 강형석 기자 redbk@donga.com / ⓒ 동아일보 &amp;amp; donga.com, 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>최태원 회장 “AI 등 혁신기술 없이 미래 담보 못해”</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>SK가 디지털 트랜스포메이션(DT)과 인공지능(AI)등 혁신기술을 '딥 체인지(Deep Change)'의 핵심 동력으로 삼고, 이들 기술의 글로벌 경쟁력을 제고를 위해 그룹 역량을 결집시키기로 했다. 내년 초 그룹 인재 역량 강화를 위해 'SK 유니버시티' 설립도 검토한다. SK는 22일 막을 내린 '2019 이천포럼'에서 AI 등 '빅 트렌드'(Big Trend) 기술 전략적 중요성을 확인하고 이 같은 방침을 정했다고 밝혔다. 최태원 SK 회장은 22일 마무리 발언에서 “AI, DT 등 혁신기술을 활용해 사회적 가치를 창출하는 한편, 우리 고객 범위를 확장하고 고객 행복을 만들어 내야 한다”면서 “이를 통해 SK가 추구해 온 '딥 체인지'를 이룰 수 있다”고 밝혔다. 이번 포럼의 주요 의제로 다룬 4차 산업혁명 시대의 대표 기술이 고객 가치 창출로 연결돼야 한다는 점을 지적한 것이다. 최 회장은 특히, “거래비용을 최소화하고, 고객이 원하는 가치를 효과적으로 전달할 수 있게 하는 혁신기술을 활용하지 못하면 SK 미래를 담보할 수 없다”면서 디지털 기술 역량 강화는 '선택이 아닌 생존의 문제'임을 강조했다. 최 회장은 “이를 통해 우리의 고객이 누군지 재정의하고, 각 고객에게 맞춤형 가치를 제공해야 한다”며 '신뢰'를 기반으로 고객과 1대1 '관계'를 구축하는 데 힘을 쏟을 것을 주문했다. 내년 1월 출범을 목표로 한 그룹 차원의 교육 인프라 'SK 유니버시티' 설립을 제안한 것도 이 같은 혁신기술 역량을 내재화하고 우수 인재를 육성하기 위함이라고 최 회장은 설명했다. 이어 최 회장은 에너지·화학과 정보통신 기술을 접목한 '에너지 솔루션' 비즈니스 모델을 소개한 뒤 “앞으로 에너지 공급자 시각만으로는 에너지 산업 변화의 물결에서 생존할 수 없다”며 환경문제를 해결하면서 고객 가치를 높이는 에너지 솔루션형 비즈니스 모델 혁신에 박차를 가하겠다는 의지를 밝혔다. 끝으로 최 회장은 “나부터도 변화는 두렵고 달갑지 않은 일이지만 번지점프를 하듯이 두려움을 극복하고 자꾸 새로운 시도를 해야 '딥 체인지'를 이룰 수 있다”며 구성원들에게 “피할 수 없다면 변화를 즐기자”고 당부했다. 지난 19일부터 연 이번 포럼에는 최 회장과 조대식 SK수펙스추구협의회 의장 등 경영진과 임원 등 연인원 800여명이 참석해 국내외 석학과 전문가들의 강연을 듣고 열띤 토론을 벌였다. 또 구성원들은 전용 모바일 앱 등을 통해 이천포럼 내용을 실시간 시청하면서 강연자들과 질의·응답을 주고 받았다. 한편, 이번 포럼에서 화상강연을 한 제레미 리프킨 美 경제동향연구재단 이사장은 “SK가 새로운 개념의 에너지 솔루션 사업을 추진하는 것은 인류 전체의 지속가능한 성장을 위해서도 매우 중요하며 시의적절하다”고 평가했다. &amp;lt;노동의 종말&amp;gt;&amp;lt;엔트로피&amp;gt; 등을 저술한 세계적 석학인 리프킨 이사장은 지난 20일 강연에서 “인류가 지구온난화에 따른 파국을 피하기 위해서는 에너지 시스템을 근본적으로 혁신해 '탄소배출 제로 시대'에 진입해야 한다”며 이 같이 말했다. 이항수 SK수펙스추구협의회 PR팀장은 “DT, AI 등 첨단 기술이 SK가 추구해 온 사회적 가치와 '딥 체인지'를 구현할 수 있는 핵심 동력이라는데 구성원이 인식을 같이 한 만큼, 향후 이들 기술역량 강화에 박차를 가하게 될 것”이라고 말했다. 안호천 통신방송 전문기자 hcan@etnews.com [Copyright ⓒ 전자신문 &amp;amp; 전자신문인터넷, 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>블룸버그 "LG화학, 테슬라 中 상하이 공장에 배터리 공급"</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>중국 난징 신장경제개발구에 위치한 LG화학 전기차 배터리 1공장 전경. (사진=LG화학) LG화학이 미국 전기차 업체 테슬라의 첫 해외 생산기지인 중국 상하이 공장에 배터리를 공급할 것으로 보인다. 블룸버그통신은 23일 복수의 소식통을 인용해 “테슬라가 중국 상하이 공장에서 생산하는 전기자동차에 LG화학 배터리를 사용하기로 양사가 합의했다”고 보도했다. LG화학은 “고객사 관련 내용은 확인할 수 없다”고 공식 언급을 하지 않았으나 업계에서는 LG화학의 테슬라 공급을 기정사실로 받아들이고 있다. 보도에 따르면 LG화학이 테슬라에 공급하는 배터리는 기존 구형 배터리보다 용량이 큰 21700 셀로 난징 공장에서 생산된다. 테슬라는 상하이 공장에서 올해 말부터 본격 생산하는 '모델3'에 LG화학 배터리를 먼저 사용하고 콤팩트 크로스오버 차량인 '모델Y'가 내년 출시되면 해당 모델에도 사용할 예정이라고 통신은 전했다. 테슬라는 올 1월 초 상하이 린강산업구에 연산 50만대에 이르는 전기차 공장 '기가팩토리'를 착공했다. 배터리 업계에서는 LG화학의 테슬라 배터리 공급 가능성을 높게 봐왔다. LG화학은 테슬라 상하이 공장과 가까운 난징 신강 경제개발구에 위치한 배터리 공장 두 곳 외에 빈장 경제개발구에 전기차 배터리 2공장을 추가로 짓고 있다. 또 난징을 세계 배터리 수출 기지로 육성한다는 목표로 올해 1월 신강 배터리 공장 두 곳에 총 1조2000억원을 투자하기로 결정했다. 특히 테슬라 전기차에 탑재되는 원통형 배터리 생산량을 크게 늘리고 있다. 다만 테슬라는 LG화학 외에 다른 회사와도 배터리 구입 계약을 체결할 계획인 것으로 알려졌다. 블룸버그에 따르면 테슬라는 중국 최대 배터리 제조사 CATL과도 관련 협의를 진행 중이다. 정현정 배터리/부품 전문기자 iam@etnews.com [Copyright ⓒ 전자신문 &amp;amp; 전자신문인터넷, 무단전재 및 재배포 금지]</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>국민에 부담 떠 넘긴 '文 케어'</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>내년 건보료 3.2% 인상··· 3년 연속 ↑ [서울경제] ‘문재인케어’로 불리는 건강보험 보장성 강화정책으로 내년 건강보험료가 3.2% 인상된다. 지난해 건강보험 재정수지가 적자로 돌아선 가운데 3년 연속 건보료가 인상되자 정부에서 재정부담을 국민에게 전가하고 있다는 우려의 목소리가 잇따르고 있다. ★관련기사 5면 보건복지부는 지난 22일 건강보험정책 최고의결기구인 건강보험정책심의위원회를 열어 오는 2020년 건강보험료율을 3.2% 올린다고 밝혔다. 이에 따라 직장가입자의 보험료율은 현행 6.46%에서 6.67%로, 지역가입자의 부과점수당 금액은 현행 189원70전에서 195원80전으로 인상된다. 월평균 보험료를 보면 올 3월 기준 직장가입자는 11만2,365원에서 3,653원 오른 11만6,018원을 내야 한다. 지역가입자는 8만7,067에서 2,800원 인상된 8만8,867원을 내년부터 추가로 부담해야 한다. 정부는 건강보험 보장성 강화대책이 속도를 내면서 불가피하게 내년도 건강보험료율을 인상했다고 설명했다. 김재헌 무상의료운동본부 사무국장은 “건강보험 보장성 강화의 취지에는 동의하지만 재정확보 대책이 빠져 있다는 것이 가장 큰 문제”라며 “국고지원금 없이 국민을 볼모로 건강보험료를 올리는 문재인케어가 계속 시행되면 예상보다 빨리 적립금이 고갈되는 최악의 상황에 직면할 수 있다”고 말했다. /이지성기자 engine@sedaily.com | 저작권자 ⓒ 서울경제, 무단 전재 및 재배포 금지</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>지구급 외계행성 3개 찾았다…약 12광년밖 적색왜성 주변서 발견</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>'GJ 1061d 행성' 서식가능지역 위치 주목 스페인 우주과학연 리바스 박사, 논문초고 사이트에 공개 지구에서 약 12.08광년 떨어진 적색왜성 'GJ 1061' 주변에서 이 별을 도는 지구 크기의 외계행성 3개가 확인됐다. 이 중 가장 밖에 있는 'GJ 1061d' 행성은 표면에 액체 상태의 물이 있을 수 있는 이른바 '서식가능지역' 안에 있어 주목을 받고 있다. 과학전문 매체 phys.org 등에 따르면 스페인 우주과학연구소의 이그나시 리바스 박사가 이끄는 연구팀은 칠레 라 실라의 유럽남방천문대(ESO) 망원경을 이용해 GJ 1061 주변에서 찾아낸 외계행성 후보 관측 결과를 출간 전 논문을 모아놓는 논문 초고 사이트(arXiv.org)에 공개했다. 이 논문은 곧 영국왕립천문학회 월보(MNRAS)에 정식으로 실릴 예정이다. 연구팀은 지구 주변 작은 별을 집중적으로 관측하며 지구형 행성을 찾아온 '레드 닷(Red Dot)' 프로젝트의 일환으로 지구에서 20번째로 가까운 GJ 1061을 관측해 왔다. 연구팀은 시선속도법을 통해 별빛이 행성의 중력으로 미세하게 흔들리는 것을 포착해 행성의 존재를 찾아냈다. 이 방식은 대형 행성을 찾는 데 주로 이용돼 왔으나 최근 관측 방법이 개선되면서 소형 행성을 확인하는 데도 활용되고 있다. 관측 결과, GJ 1061 b~d 3개 행성은 지구의 1.4~1.8배 크기로 별을 3~13일 주기로 돌고 있다. 이는 태양계 수성의 공전 주기 88일과 비교할 때 별에 붙어있다시피 한 것이지만 GJ 1061이 질량이 낮은 적색왜성이어서 13일 주기의 d 행성에도 생명체가 존재할 수 있는 가능성이 있는 것으로 여겨지고 있다. GJ 1061은 태양과 비교해 질량은 10분의 1, 밝기는 1천분의 1에 불과하다. 지구에서 약 4.2광년 떨어진 가장 가까운 행성계의 별인 '프록시마 켄타우리'와 비슷하지만, 현재로선 프록시마 켄타우리보다 폭발 활동이 덜해 생명체에는 더 안전할 것으로 나타났다. 그러나 태양과 같은 별보다 수명이 훨씬 긴 적색왜성이 과거에 수백만년에 걸쳐 강한 폭발 활동을 했을 수도 있어, 가까이서 별을 도는 d행성의 대기가 생명체가 존재할 수 없을 정도로 파괴됐을 가능성도 있는 것으로 지적됐다. GJ 1061 행성계에는 b~d 행성보다 더 바깥 궤도를 가진 제4 행성으로 추정되는 천체도 발견했으나 추가 확인이 필요한 것으로 보고됐다. 디지털뉴스부기자 dtnews@dt.co.kr &amp;lt;연합뉴스&amp;gt; /</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>